<commit_message>
(v1.3.0.9022) mo_matching_score(), poorman update, as.rsi() fix
</commit_message>
<xml_diff>
--- a/data-raw/antibiotics.xlsx
+++ b/data-raw/antibiotics.xlsx
@@ -4053,7 +4053,7 @@
     <t xml:space="preserve">Piperacillin/tazobactam</t>
   </si>
   <si>
-    <t xml:space="preserve">c("p/t", "piptaz", "pita", "pt", "ptc", "ptz", "tzp")</t>
+    <t xml:space="preserve">c("p/t", "piptaz", "piptazo", "pita", "pt", "ptc", "ptz", "tzp")</t>
   </si>
   <si>
     <t xml:space="preserve">c("", "tazocel", "tazocillin", "tazocin", "zosyn")</t>
@@ -6458,7 +6458,7 @@
         <v>63</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K9" t="s">
         <v>22</v>
@@ -6502,7 +6502,7 @@
         <v>70</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K10" t="s">
         <v>22</v>
@@ -7637,7 +7637,9 @@
       <c r="I43" t="s">
         <v>20</v>
       </c>
-      <c r="J43"/>
+      <c r="J43" t="n">
+        <v>15</v>
+      </c>
       <c r="K43"/>
       <c r="L43"/>
       <c r="M43"/>
@@ -9665,7 +9667,9 @@
       <c r="I100" t="s">
         <v>443</v>
       </c>
-      <c r="J100"/>
+      <c r="J100" t="n">
+        <v>2.1</v>
+      </c>
       <c r="K100"/>
       <c r="L100"/>
       <c r="M100"/>
@@ -11575,7 +11579,9 @@
       <c r="I153" t="s">
         <v>685</v>
       </c>
-      <c r="J153"/>
+      <c r="J153" t="n">
+        <v>0.2</v>
+      </c>
       <c r="K153"/>
       <c r="L153"/>
       <c r="M153"/>
@@ -12385,7 +12391,9 @@
       <c r="I175" t="s">
         <v>784</v>
       </c>
-      <c r="J175"/>
+      <c r="J175" t="n">
+        <v>0.75</v>
+      </c>
       <c r="K175"/>
       <c r="L175"/>
       <c r="M175"/>
@@ -13095,7 +13103,9 @@
       <c r="I195" t="s">
         <v>864</v>
       </c>
-      <c r="J195"/>
+      <c r="J195" t="n">
+        <v>0.32</v>
+      </c>
       <c r="K195"/>
       <c r="L195"/>
       <c r="M195"/>
@@ -14307,7 +14317,9 @@
       <c r="I230" t="s">
         <v>1007</v>
       </c>
-      <c r="J230"/>
+      <c r="J230" t="n">
+        <v>0.4</v>
+      </c>
       <c r="K230"/>
       <c r="L230"/>
       <c r="M230"/>
@@ -15141,7 +15153,9 @@
       <c r="I253" t="s">
         <v>1100</v>
       </c>
-      <c r="J253"/>
+      <c r="J253" t="n">
+        <v>1.2</v>
+      </c>
       <c r="K253"/>
       <c r="L253" t="n">
         <v>1</v>
@@ -18077,7 +18091,9 @@
       <c r="I336" t="s">
         <v>1435</v>
       </c>
-      <c r="J336"/>
+      <c r="J336" t="n">
+        <v>0.2</v>
+      </c>
       <c r="K336"/>
       <c r="L336"/>
       <c r="M336"/>
@@ -18865,7 +18881,9 @@
       <c r="I358" t="s">
         <v>20</v>
       </c>
-      <c r="J358"/>
+      <c r="J358" t="n">
+        <v>86</v>
+      </c>
       <c r="K358"/>
       <c r="L358"/>
       <c r="M358"/>
@@ -20843,7 +20861,9 @@
       <c r="I412" t="s">
         <v>1734</v>
       </c>
-      <c r="J412"/>
+      <c r="J412" t="n">
+        <v>0.2</v>
+      </c>
       <c r="K412"/>
       <c r="L412"/>
       <c r="M412"/>

</xml_diff>

<commit_message>
(v1.6.0.9017) extra system codes
</commit_message>
<xml_diff>
--- a/data-raw/antibiotics.xlsx
+++ b/data-raw/antibiotics.xlsx
@@ -104,7 +104,7 @@
     <t xml:space="preserve">Other antifungals for topical use</t>
   </si>
   <si>
-    <t xml:space="preserve">c("5flc", "fluo")</t>
+    <t xml:space="preserve">c("5flc", "fcu", "fluo", "fluy")</t>
   </si>
   <si>
     <t xml:space="preserve">c("alcobon", "ancobon", "ancotil", "ancotyl", "flucitosina", "flucystine", "flucytosin", "flucytosine", "flucytosinum", "flucytosone", "fluocytosine", "fluorcytosine")</t>
@@ -249,7 +249,7 @@
     <t xml:space="preserve">Antibiotics</t>
   </si>
   <si>
-    <t xml:space="preserve">c("amfb", "amph")</t>
+    <t xml:space="preserve">c("amf", "amfb", "amph")</t>
   </si>
   <si>
     <t xml:space="preserve">c("abelcet", "abelecet", "ambisome", "amfotericina b", "amphocin", "amphomoronal", "amphortericin b", "amphotec", "amphotericin", "amphotericin b", "amphotericine b", "amphotericinum b", "amphozone", "anfotericine b", "fungilin", "fungisome", "fungisone", "fungizone", "halizon")</t>
@@ -1986,7 +1986,7 @@
     <t xml:space="preserve">Polymyxins</t>
   </si>
   <si>
-    <t xml:space="preserve">c("cl", "coli", "cs", "ct")</t>
+    <t xml:space="preserve">c("cl", "coli", "cs", "cst", "ct")</t>
   </si>
   <si>
     <t xml:space="preserve">c("belcomycine", "colimycin", "colimycin sulphate", "colisticin", "colistimethate", "colistimethate sodium", "colistin sulfate", "colistin sulphate", "colomycin", "coly-mycin", "polymyxin e", "polymyxin e. sulfate", "promixin", "totazina")</t>
@@ -2500,7 +2500,7 @@
     <t xml:space="preserve">Triazole derivatives</t>
   </si>
   <si>
-    <t xml:space="preserve">c("fluc", "fluz")</t>
+    <t xml:space="preserve">c("fluc", "fluz", "flz")</t>
   </si>
   <si>
     <t xml:space="preserve">c("alflucoz", "alfumet", "biocanol", "biozole", "biozolene", "canzol", "cryptal", "diflazon", "diflucan", "dimycon", "elazor", "flucazol", "fluconazol", "fluconazole", "fluconazole capsules", "fluconazolum", "flucostat", "flukezol", "flunazol", "flunizol", "flusol", "fluzon", "fluzone", "forcan", "fuconal", "fungata", "loitin", "oxifugol", "pritenzol", "syscan", "trican", "triconal", "triflucan", "zoltec")</t>
@@ -2551,7 +2551,7 @@
     <t xml:space="preserve">Fosfomycin</t>
   </si>
   <si>
-    <t xml:space="preserve">c("ff", "fm", "fo", "fos", "fosf")</t>
+    <t xml:space="preserve">c("ff", "fm", "fo", "fof", "fos", "fosf")</t>
   </si>
   <si>
     <t xml:space="preserve">c("fosfocina", "fosfomicina", "fosfomycin", "fosfomycin sodium", "fosfomycine", "fosfomycinum", "fosfonomycin", "monuril", "monurol", "phosphonemycin", "phosphonomycin", "veramina")</t>
@@ -2601,7 +2601,7 @@
     <t xml:space="preserve">Steroid antibacterials</t>
   </si>
   <si>
-    <t xml:space="preserve">fusi</t>
+    <t xml:space="preserve">c("fa", "fusi")</t>
   </si>
   <si>
     <t xml:space="preserve">c("acide fusidique", "acido fusidico", "acidum fusidicum", "flucidin", "fucidate", "fucidate sodium", "fucidic acid", "fucidin", "fucidin acid", "fucithalmic", "fusidate", "fusidate acid", "fusidic acid", "fusidine", "fusidinic acid", "ramycin")</t>
@@ -2676,7 +2676,7 @@
     <t xml:space="preserve">Gentamicin-high</t>
   </si>
   <si>
-    <t xml:space="preserve">c("gehl", "genta high", "gentamicin high")</t>
+    <t xml:space="preserve">c("g_h", "gehl", "genta high", "gentamicin high")</t>
   </si>
   <si>
     <t xml:space="preserve">GEP</t>
@@ -2915,7 +2915,7 @@
     <t xml:space="preserve">Kanamycin-high</t>
   </si>
   <si>
-    <t xml:space="preserve">c("", "kahl")</t>
+    <t xml:space="preserve">c("", "k_h", "kahl")</t>
   </si>
   <si>
     <t xml:space="preserve">KAC</t>
@@ -2936,7 +2936,7 @@
     <t xml:space="preserve">Imidazole derivatives</t>
   </si>
   <si>
-    <t xml:space="preserve">keto</t>
+    <t xml:space="preserve">c("keto", "ktc")</t>
   </si>
   <si>
     <t xml:space="preserve">c("extina", "fungarest", "fungoral", "ketocanazole", "ketoconazol", "ketoconazole", "ketoconazolum", "ketoderm", "nizoral", "xolegel")</t>
@@ -4047,7 +4047,7 @@
     <t xml:space="preserve">Piperacillin/tazobactam</t>
   </si>
   <si>
-    <t xml:space="preserve">c("p/t", "piptaz", "piptazo", "pita", "pt", "ptc", "ptz", "tzp")</t>
+    <t xml:space="preserve">c("p/t", "piptaz", "piptazo", "pit", "pita", "pt", "ptc", "ptz", "tzp")</t>
   </si>
   <si>
     <t xml:space="preserve">c("", "tazocel", "tazocillin", "tazocin", "zosyn")</t>
@@ -4661,7 +4661,7 @@
     <t xml:space="preserve">Sparfloxacin</t>
   </si>
   <si>
-    <t xml:space="preserve">c("", "spar")</t>
+    <t xml:space="preserve">c("", "spa", "spar")</t>
   </si>
   <si>
     <t xml:space="preserve">c("esparfloxacino", "sparfloxacin", "sparfloxacine", "sparfloxacinum")</t>
@@ -4727,7 +4727,7 @@
     <t xml:space="preserve">Streptomycin</t>
   </si>
   <si>
-    <t xml:space="preserve">c("s", "str", "stre")</t>
+    <t xml:space="preserve">c("s", "stm", "str", "stre")</t>
   </si>
   <si>
     <t xml:space="preserve">c("agrept", "agrimycin", "chemform", "estreptomicina", "neodiestreptopab", "strepcen", "streptomicina", "streptomycin", "streptomycin a", "streptomycin spx", "streptomycin sulfate", "streptomycine", "streptomyzin", "vetstrep")</t>
@@ -4742,7 +4742,7 @@
     <t xml:space="preserve">Streptomycin-high</t>
   </si>
   <si>
-    <t xml:space="preserve">c("sthl", "strepto high", "streptomycin high")</t>
+    <t xml:space="preserve">c("s_h", "sthl", "strepto high", "streptomycin high")</t>
   </si>
   <si>
     <t xml:space="preserve">STI</t>
@@ -5504,7 +5504,7 @@
     <t xml:space="preserve">Tigecycline</t>
   </si>
   <si>
-    <t xml:space="preserve">c("tgc", "tige")</t>
+    <t xml:space="preserve">c("tgc", "tig", "tige")</t>
   </si>
   <si>
     <t xml:space="preserve">c("haizheng li xing", "tigeciclina", "tigecyclin", "tigecycline", "tigecycline hydrate", "tigecyclinum", "tigilcycline", "tygacil")</t>
@@ -5639,7 +5639,7 @@
     <t xml:space="preserve">Trimethoprim</t>
   </si>
   <si>
-    <t xml:space="preserve">c("t", "tmp", "tr", "trim", "w")</t>
+    <t xml:space="preserve">c("t", "tmp", "tr", "tri", "trim", "w")</t>
   </si>
   <si>
     <t xml:space="preserve">c("abaprim", "alprim", "anitrim", "antrima", "antrimox", "bacdan", "bacidal", "bacide", "bacterial", "bacticel", "bactifor", "bactin", "bactoprim", "bactramin", "bactrim", "bencole", "bethaprim", "biosulten", "briscotrim", "chemotrin", "colizole", "colizole ds", "conprim", "cotrimel", "cotrimoxizole", "deprim", "dosulfin", "duocide", "esbesul", "espectrin", "euctrim", "exbesul", "fermagex", "fortrim", "idotrim", "ikaprim", "instalac", "kombinax", "lagatrim", "lagatrim forte", "lastrim", "lescot", 
@@ -5785,7 +5785,7 @@
     <t xml:space="preserve">Voriconazole</t>
   </si>
   <si>
-    <t xml:space="preserve">vori</t>
+    <t xml:space="preserve">c("vori", "vrc")</t>
   </si>
   <si>
     <t xml:space="preserve">c("pfizer", "vfend i.v.", "voriconazol", "voriconazole", "voriconazolum", "vorikonazole")</t>

</xml_diff>

<commit_message>
(v2.1.1.9093) New brand names
</commit_message>
<xml_diff>
--- a/data-raw/antibiotics.xlsx
+++ b/data-raw/antibiotics.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>aminopar,aminosalicylic,aminosalicylic acid,aminosalyl,aminox,apacil,deapasil,entepas,ferrosan,gabbropas,granupas,helipidyl,hellipidyl,neopasalate,osacyl,pamacyl,pamisyl,paramycin,parasal,parasalicil,parasalindon,pasalon,pasara,pascorbic,pasdium,paser granules,paskalium,pasmed,pasnodia,pasolac,propasa,rezipas,teebacin</t>
+          <t>aminacyl,aminopar,aminosalicylate,aminosalicylic,aminosalicylic acid,aminosalyl,aminosalyle,aminox,apacil,deapasil,entepas,ferrosan,gabbropas,granupas,helipidyl,hellipidyl,nemasol,neopasalate,nippas,osacyl,p.a.s.,pamacyl,pamisyl,paramisan,paramycin,parasal,parasalicil,parasalindon,pasade,pasalon,pasara,pascorbic,pasdium,paser granules,paskalium,pasmed,pasnal,pasnodia,pasolac,passodico,propasa,rezipas,salvis,sodiopas,teebacin</t>
         </is>
       </c>
       <c r="J2">
@@ -548,7 +548,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t/>
+          <t>medemycin,mydecamycin</t>
         </is>
       </c>
       <c r="J3" t="e">
@@ -606,7 +606,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>acetylspiramycin,foromacidin b,spiramycin ii</t>
+          <t>formacidine,foromacidin,foromacidin a,foromacidin b,rovamicina,rovamycin,rovamycine,spiramycin i</t>
         </is>
       </c>
       <c r="J4" t="e">
@@ -668,7 +668,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>adesulfone sodium,aldapsone,aldesulfona sodica,aldesulfone,aldesulfone sodique,aldesulfone sodium,aldesulphone sodium,diamidin,diasone,diasone sodium,diazon,novotrone,sodium aldesulphone,sodium sulfoxone,sulfoxone sodium</t>
+          <t>adesulfone,aldapsone,aldesulfona sodica,aldesulfone,aldesulfone sodique,aldesulphone,diamidin,diason,diasone,diasoneenterab,diazon,novotrone,sulfoxone</t>
         </is>
       </c>
       <c r="J5">
@@ -732,7 +732,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>amicacin,amikacillin,amikacin,amikacin base,amikacin dihydrate,amikacin free base,amikacin sulfate,amikacina,amikacine,amikacinum,amikavet,amikin,amiklin,amikozit,amukin,arikace,arikayce liposomal,briclin,kaminax,lukadin,mikavir,pierami,potentox</t>
+          <t>ambutyrosin a,ambutyrosin b,ambuyrosin a,amicacin,amikacillin,amikacin dihydrate,amikacin free,amikacina,amikacine,amikacinum,amikavet,amikin,amiklin,amikozit,amukin,arikace,arikayce liposomal,briclin,butirosin a,butirosin b,butyrosin a,butyrosin b,kaminax,lukadin,mikavir,pierami,potentox</t>
         </is>
       </c>
       <c r="J6" t="e">
@@ -854,7 +854,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>amorolfina,amorolfine,amorolfinum,loceryl</t>
+          <t>amorolfina,amorolfine hcl?,amorolfinum,bekiron,corbel,curanail,fenpropemorph,fenpropimorph,fenpropimorphe,funbas,loceryl,locetar,mildofix,mistral,mistral t,odenil,pekiron</t>
         </is>
       </c>
       <c r="J8" t="e">
@@ -916,7 +916,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>actimoxi,amoclen,amolin,amopen,amopenixin,amoxibiotic,amoxicaps,amoxicilina,amoxicillin,amoxicillin hydrate,amoxicilline,amoxicillinum,amoxiden,amoxil,amoxivet,amoxy,amoxycillin,amoxyke,anemolin,aspenil,atoksilin,biomox,bristamox,cemoxin,clamoxyl,damoxy,delacillin,demoksil,dispermox,efpenix,flemoxin,hiconcil,histocillin,hydroxyampicillin,ibiamox,imacillin,lamoxy,largopen,metafarma capsules,metifarma capsules,moksilin,moxacin,moxatag,ospamox,pamoxicillin,piramox,promoxil,remoxil,robamox,sawamox pm,tolodina,topramoxin,unicillin,utimox,vetramox</t>
+          <t>actimoxi,acuotricina,agram,alfamox,alfida,alfoxil enjektabl,amitron,amoclen,amodex,amoksicillin,amoksicillin forte,amolin,amopen,amopenixin,amophar,amoran,amoxibiotic,amoxicaps,amoxicilina,amoxicillin pulsys,amoxicilline,amoxicillinsalt,amoxicillinum,amoxidal,amoxiden,amoxil,amoxil trihydrate,amoxillat,amoxina,amoxine,amoxipen,amoxivet,amoxy,amoxycillin,amoxyke,anemolin,aspenil,atoksilin,biomox,bristamox,cemoxin,ciblor,clamoxyl,damoxy,danoxillin,delacillin,demoksil,dispermox,dura,efpenix,eupen,flemoxin,flemoxine,galenamox,gramidil,hiconcil,himinomax,histocillin,hydroxyampicillin,ibiamox,imacillin,izoltil,kentrocyllin,lamoxy,largopen,larotid,matasedrin,metafarma capsules,metifarma,metifarma capsules,moksilin,moxacin,moxaline,moxatag,neotetranase,novabritine,ospamox,pacetocin,pamocil,pamoxicillin,paradroxil,pasetocin,penamox,piramox,promoxil,quimiopen,remoxil,riotapen,robamox,sawacillin,sawamox,siganopen,simplamox,sintopen,tolodina,topramoxin,trifamox,trimox,unicillin,utimox,velamox,vetramox,wymox,zamocillin,zamocilline,zimox</t>
         </is>
       </c>
       <c r="J9">
@@ -982,7 +982,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>amocla,amoclan,amoclav,amoksiclav,amoxsiklav,amoxyclav,augmentan,augmentin,augmentin xr,augmentine,auspilic,clamentin,clamobit,clavamox,clavinex,clavoxilin plus,clavulin,clavumox,coamoxiclav,eumetinex,kmoxilin,spectramox,spektramox,synulox,viaclav,xiclav</t>
+          <t>amocla,amoclan,amoclav,amoksiclav,amox clav,amoxsiklav,amoxyclav,augmentan,augmentin,augmentine,auspilic,clamentin,clamobit,clavamox,clavinex,clavoxilin plus,clavulin,clavumox,coamoxiclav,eumetinex,kmoxilin,spectramox,spektramox,synulox,viaclav,xiclav</t>
         </is>
       </c>
       <c r="J10">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>abelcet,abelecet,ambisome,amfotericina b,amphocin,amphomoronal,amphortericin b,amphotec,amphotericin,amphotericin b,amphotericine b,amphotericinum b,amphozone,anfotericine b,fungilin,fungisome,fungisone,fungizone,halizon</t>
+          <t>abelcet,abelecet,ambisome,amfotericina b,amphocin,amphomoronal,amphortericin b,amphotec,amphotericin,amphotericine b,amphotericinum b,amphozone,anfotericine b,fungilin,fungisome,fungisone,fungizone,halizon,nyotran,nystatinum,terrastatin</t>
         </is>
       </c>
       <c r="J12">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>acillin,adobacillin,amblosin,amcill,amfipen,amfipen v,amipenix s,ampichel,ampicil,ampicilina,ampicillin,ampicillin a,ampicillin acid,ampicillin anhydrate,ampicillin anhydrous,ampicillin base,ampicillin hydrate,ampicillin sodium,ampicillina,ampicilline,ampicillinum,ampicin,ampifarm,ampikel,ampimed,ampipenin,ampiscel,ampisyn,ampivax,ampivet,amplacilina,amplin,amplipenyl,amplisom,amplital,anhydrous ampicillin,austrapen,binotal,bonapicillin,britacil,campicillin,copharcilin,delcillin,deripen,divercillin,doktacillin,duphacillin,grampenil,guicitrina,guicitrine,lifeampil,marcillin,morepen,norobrittin,nuvapen,olin kid,omnipen,orbicilina,pen a oral,pen ampil,penbristol,penbritin,penbritin paediatric,penbritin syrup,penbrock,penicline,penimic,pensyn,pentrex,pentrexl,pentrexyl,pentritin,pfizerpen a,polycillin,polyflex,ponecil,princillin,principen,qidamp,racenacillin,redicilin,rosampline,roscillin,semicillin,semicillin r,servicillin,sumipanto,synpenin,texcillin,tokiocillin,tolomol,totacillin,totalciclina,totapen,trifacilina,ukapen,ultrabion,ultrabron,vampen,viccillin,viccillin s,vidocillin,wypicil</t>
+          <t>acillin,adobacillin,amblosin,amcap,amcill,amfipen,amfipen v,amipenix s,amperil,ampichel,ampicil,ampicilina,ampicillin a,ampicillin acid,ampicillina,ampicilline,ampicillinesalt,ampicillinsalt,ampicillinum,ampicin,ampifarm,ampikel,ampimed,ampinova,ampipenin,ampiplus simplex,ampiscel,ampisyn,ampivax,ampivet,amplacilina,amplin,amplipenyl,amplisom,amplital,austrapen,benzopenicillin,binotal,bonapicillin,britacil,campicillin,citteral,compocillin g,copharcilin,cymbi,delcillin,deripen,divercillin,doktacillin,domicillin,duphacillin,galofak,grampenil,guicitrina,guicitrine,lifeampil,marcillin,morepen,norobrittin,nuvapen,olin kid,omnipen,orbicilina,pen a,pen ampil,penbristol,penbritin,penbrock,penialmen,penicline,penimic,pensyn,pentrex,pentrexl,pentrexyl,pentritin,pfizerpen a,polycillin,polyflex,ponecil,princillin,principen,qidamp,racenacillin,redicilin,rosampline,roscillin,semicillin,semicillin r,servicillin,sumipanto,synpenin,texcillin,tokiocillin,tolomol,totacillin,totalciclina,totapen,trafarbiot,trifacilina,ukapen,ultrabion,ultrabron,vampen,viccillin,viccillin s,vidocillin,wypicil</t>
         </is>
       </c>
       <c r="J14">
@@ -1356,7 +1356,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>amprocidum,amprol,amprolio,amprolium,amprolium chloride,amprovine,thiacoccid</t>
+          <t>amprid for calves,amprocidum,amprol,amprolio,amprolium chloride,amprolium ion,amprolsol,ampromed for calves,ampromed for cattle,amprovine,cocciaid,cocciprol,corid,mepyrium,thiacoccid</t>
         </is>
       </c>
       <c r="J16" t="e">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>anidulafungin,anidulafungina,anidulafungine,anidulafunginum,ecalta,eraxis</t>
+          <t>anidulafungina,anidulafungine,anidulafunginum,biafungin,ecalta,eraxis,rezafungin acetate,rezafungin cation,rezafungin ion,rezafungin?,rezzayo</t>
         </is>
       </c>
       <c r="J17" t="e">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>apalcilina,apalcillin,apalcilline,apalcillinum</t>
+          <t>apalcilina,apalcilline,apalcillinsalt,apalcillinum,lumota</t>
         </is>
       </c>
       <c r="J18" t="e">
@@ -1536,7 +1536,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>ambylan,apralan,apramicina,apramycin,apramycine,apramycinum,nebramycin ii</t>
+          <t>ambylan,apralan,apramicina,apramycine,apramycinum,casein hydrolysate,nebramycin,nebramycin vii</t>
         </is>
       </c>
       <c r="J19" t="e">
@@ -1594,7 +1594,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>arbekacin,arbekacina,arbekacine,arbekacini sulfas,arbekacinum,habekacin,haberacin</t>
+          <t>ambutyrosin a,ambutyrosin b,ambuyrosin a,arbekacina,arbekacine,arbekacini sulfas,arbekacinum,butirosin a,butirosin b,butyrosin a,butyrosin b,haberacin</t>
         </is>
       </c>
       <c r="J20" t="e">
@@ -1654,7 +1654,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>aspoxicilina,aspoxicillan,aspoxicillin,aspoxicilline,aspoxicillinum</t>
+          <t>amoxycillin,aspoxicilina,aspoxicillan,aspoxicilline,aspoxicillinum</t>
         </is>
       </c>
       <c r="J21" t="e">
@@ -1714,7 +1714,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>astromicin,astromicin a,astromicina,astromicine,astromicinum,fortimicin,fortimicin a</t>
+          <t>astromicin a,astromicina,astromicine,astromicinum,fortimicin,fortimicin a,istamycin a</t>
         </is>
       </c>
       <c r="J22" t="e">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>avibactam,avibactam free acid,avibactamfreeacid</t>
+          <t>avibactam free acid,avibactamfreeacid</t>
         </is>
       </c>
       <c r="J23" t="e">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>avilamycin,avilamycina,avilamycine,avilamycinum,surmax</t>
+          <t>avilamycin a,avilamycina,avilamycine,avilamycinum,surmax</t>
         </is>
       </c>
       <c r="J24" t="e">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>avoparcin,avoparcina,avoparcine,avoparcinum,avotan</t>
+          <t>aerovanc,avoparcina,avoparcine,avoparcinum,avotan,firvanq,firvanq kit,targocid,tecoplanina,tecoplanine,tecoplaninum,teichomycin,teicoplanina,teicoplanine,teicoplaninum</t>
         </is>
       </c>
       <c r="J25" t="e">
@@ -1950,7 +1950,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>azidocilina,azidocillin,azidocillina,azidocilline,azidocillinum</t>
+          <t>amcap,amcill,ampen,amperil,ampinova,azidocilina,azidocillina,azidocilline,azidocillinum,cymbi,deripen,guicitrine,pen a,penbritin,principen,trafarbiot,wypicil</t>
         </is>
       </c>
       <c r="J26">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>aritromicina,aruzilina,azasite,azenil,azifast,azigram,azimakrol,azithramycine,azithrocin,azithromycin,azithromycine,azithromycinum,azitrocin,azitromax,azitromicina,azitromicine,azitromin,aziwin,aziwok,aztrin,azyter,azythromycin,durasite,hemomycin,macrozit,misultina,mixoterin,setron,sumamed,toraseptol,tromix,trozocina,trulimax,xithrone,zentavion,zithrax,zithromac,zithromax,zithromax iv,zithromycin,zitrim,zitromax,zitrotek,zmax sr,zythromax</t>
+          <t>aritromicina,aruzilina,azasite,azenil,azifast,azigram,azimakrol,azithramycine,azithrocin,azithromycine,azithromycinum,azitrocin,azitromax,azitromicina,azitromicine,azitromin,aziwin,aziwok,aztrin,azyter,azythromycin,durasite,hemomycin,macrozit,misultina,mixoterin,setron,sumamed,toraseptol,tromix,trozocina,trulimax,xithrone,zentavion,zithrax,zithromac,zithromax,zithromycin,zitrim,zitromax,zitrotek,zmax,zythromax</t>
         </is>
       </c>
       <c r="J27">
@@ -2142,7 +2142,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>azlocilina,azlocillin,azlocilline,azlocillinum</t>
+          <t>azlin,azlocilina,azlocilline,azlocillinsalt,azlocillinum,securopen</t>
         </is>
       </c>
       <c r="J29" t="e">
@@ -2206,7 +2206,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>azactam,azetreonam,azonam,azthreonam,aztreon,aztreonam,nebactam,primbactam</t>
+          <t>azactam,azetreonam,azonam,azthreonam,aztreon,nebactam,primbactam</t>
         </is>
       </c>
       <c r="J30" t="e">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>bacampicilina,bacampicillin,bacampicilline,bacampicillinum,penglobe</t>
+          <t>alphacilina,alphacillin,ambacamp,ambaxin,bacacil,bacampicilina,bacampicilline,bacampicillinum,berocillin,centurina,devonium,diancina,inacilin,maxifen,penglobe,pivatil,pondocil,pondocillin,pondocillina,sanguicillin,spectrobid,velbacil</t>
         </is>
       </c>
       <c r="J33">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>fortracin,md bacitracin</t>
+          <t>altracin,ayfivin,baciguent,baciim,baciliquin,bacilliquin,bacitek ointment,bacitracin a,bacitracin powder,bacitracina,bacitracine,bacitracinum,fortracin,md bacitracin,mycitracin,parentracin,penitracin,septa,spectrocin plus,topitracin,topitrasin,tropitracin,zutracin</t>
         </is>
       </c>
       <c r="J34" t="e">
@@ -2504,7 +2504,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>bedaquiline,sirturo</t>
+          <t>bedaquiline ?,sirturo</t>
         </is>
       </c>
       <c r="J35">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>aminodeoxykanamycin,becanamicina,bekanamycin,bekanamycine,bekanamycinum,kanamycin b,klebcil,nebramycin v</t>
+          <t>aminodeoxykanamycin,becanamicina,bekanamycine,bekanamycinum,kanamycin b,klebcil,nebramycin v</t>
         </is>
       </c>
       <c r="J36" t="e">
@@ -2756,7 +2756,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>abbocillin,ayercillin,bencilpenicilina,benzopenicillin,benzyl penicillin,benzylpenicillin,benzylpenicillin g,benzylpenicilline,benzylpenicillinum,bicillin,cillora,cilloral,cilopen,compocillin g,cosmopen,dropcillin,free penicillin g,free penicillin ii,galofak,gelacillin,liquacillin,megacillin,pencillin g,penicillin,penicilling,pentids,permapen,pfizerpen,pfizerpen g,pharmacillin,pradupen,specilline g,ursopen</t>
+          <t>abbocillin,amcap,amcill,american penicillin,amperil,ampinova,ayercillin,bencilpenicilina,benzopenicillin,benzyl penicillin,benzylpenicillin g,benzylpenicilline,benzylpenicillinsalt,benzylpenicillinum,bicillin,capicillin,cillora,cilloral,cilopen,cintrisul,compocillin g,cosmopen,cristapen,crystapen,cymbi,dropcillin,eskacillin,ethacillin,falapen,forpen,free penicillin g,free penicillin,galofak,gelacillin,hipercilina,hyasorb,hylenta,lemopen,liquacillin,liquapen,megacillin,megacillin tablets,monocillin,monopen,mycofarm,nalpen g,novocillin,paclin g,penalev,penbritin,pencillin g,penicillin,penicillin g,penicillin g k,penicilling,penicillinum,penilaryn,penisem,pentid,pentids,permapen,pfizerpen,pfizerpen g,pharmacillin,pradupen,principen,qidpen g,scotcil,specilline g,sugracillin,sugracillinsalt,tabilin,trafarbiot,tu cillin,ursopen,veticillin</t>
         </is>
       </c>
       <c r="J39" t="e">
@@ -2816,7 +2816,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>besifloxacin,besivance</t>
+          <t>besifloxacin hcl?,besivance</t>
         </is>
       </c>
       <c r="J40" t="e">
@@ -2874,7 +2874,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>biapenem,biapenern,bipenem,omegacin</t>
+          <t>biapenern,bipenem,omegacin</t>
         </is>
       </c>
       <c r="J41" t="e">
@@ -2934,7 +2934,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>aizumycin,bacfeed,bacteron,bicozamicina,bicozamycin,bicozamycine,bicozamycinum,bicyclomycin</t>
+          <t>aizumycin,bacfeed,bacteron,bicozamicina,bicozamycin,bicozamycine,bicozamycinum</t>
         </is>
       </c>
       <c r="J42" t="e">
@@ -2996,7 +2996,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>brodimoprim,brodimoprima,brodimoprime,brodimoprimum,bromdimoprim,hyprim,unitrim</t>
+          <t>brodimoprima,brodimoprime,brodimoprimum,bromdimoprim,hyprim,unitrim</t>
         </is>
       </c>
       <c r="J43">
@@ -3056,7 +3056,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>butaconazole,butoconazol,butoconazole,butoconazolum,compositenstarke,dahlin,femstat,gynofort,polyfructosanum</t>
+          <t>butaconazole,butoconazol,butoconazolum,compositenstarke,dahlin,femstat,gynofort,polyfructosanum</t>
         </is>
       </c>
       <c r="J44" t="e">
@@ -3114,7 +3114,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>cadazolid</t>
+          <t/>
         </is>
       </c>
       <c r="J45" t="e">
@@ -3240,7 +3240,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t/>
+          <t>capstat,cyclo,hexanamide,tuberactinomycin o</t>
         </is>
       </c>
       <c r="J47" t="e">
@@ -3304,7 +3304,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>anabactyl,carbenicilina,carbenicillin,carbenicillina,carbenicilline,carbenicillinum,geopen,pyopen</t>
+          <t>anabactyl,carbecin,carbenicilina,carbenicillin disalt,carbenicillina,carbenicilline,carbenicillinum,dicarbenicillin,dipenicillin,fugacillin,geopen,gripenin,hyoper,microcillin,piopen,pyocianil,pyoclox,pyopan,pyopen,pyopene</t>
         </is>
       </c>
       <c r="J48" t="e">
@@ -3368,7 +3368,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>carindacilina,carindacillin,carindacilline,carindacillinum</t>
+          <t>carindacilina,carindacilline,carindacillinsalt,carindacillinum,geocillin,indanylcarbinicillin,urobac</t>
         </is>
       </c>
       <c r="J49">
@@ -3428,7 +3428,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>carumonam,carumonamum</t>
+          <t>carumonamum</t>
         </is>
       </c>
       <c r="J50" t="e">
@@ -3492,7 +3492,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>cancidas,capsofungin,caspofungin</t>
+          <t>cancidas,capsofungin,caspo,caspofungin acetate,caspofungina</t>
         </is>
       </c>
       <c r="J51" t="e">
@@ -3556,7 +3556,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>cefacetril,cefacetrile,cefacetrilo,cefacetrilum,celospor,celtol,cephacetrile,cristacef,vetrimast</t>
+          <t>cefacetril,cefacetrilo,cefacetrilum,celospor,celtol,cephacetrile,cristacef,vetrimast</t>
         </is>
       </c>
       <c r="J52" t="e">
@@ -3618,7 +3618,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>alenfral,alfacet,ceclor,ceclor cd,cefaclor,cefaclor anhydrous,cefaclor impurity c,cefaclor monohydrate,cefaclorimpurityc,cefacloro,cefaclorum,cefeaclor,cephaclor,dystaclor mr,keflor,kefral,panoral,raniclor</t>
+          <t>alenfral,alfacet,alfatil,alfatil kapseln,ceclor,cefachlor,cefaclor impurity c,cefaclor monohydrate,cefaclorimpurityc,cefacloro,cefaclorum,cefeaclor,cephaclor,cephalexin,distaclor,dystaclor,keflor,kefolor,kefolor suspension,kefral,keftab,muco panoral,panacef,panoral,raniclor</t>
         </is>
       </c>
       <c r="J53">
@@ -3682,7 +3682,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>anhydrous cefadroxil,cefadrops,cefadroxil,cefadroxil anhydrous,cefadroxilo,cefadroxilum,cefradroxil,cephadroxil,duracef,duricef,sumacef,ultracef</t>
+          <t>brisoral,cefadrops,cefadroxilo,cefadroxilum,cefradroxil,cefzil,cephadroxil,duracef,duricef,procef,sumacef,ultracef</t>
         </is>
       </c>
       <c r="J54">
@@ -3746,7 +3746,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>alcephin,alexin,alsporin,amplex,anhydrous cefalexin,anhydrous cephalexin,biocef,carnosporin,cefablan,cefadal,cefadin,cefadina,cefaleksin,cefalessina,cefalexin,cefalexin anhydrous,cefalexina,cefalexine,cefalexinum,cefalin,cefaloto,cefaseptin,ceffanex,ceflax,ceforal,cefovit,celexin,cepastar,cepexin,cephacillin,cephalexin,cephalexin anhydrous,cephalexine,cephalexinum,cephanasten,cephaxin,cephin,ceporex,ceporex forte,ceporexin,ceporexine,cerexin,cerexins,cophalexin,durantel,durantel ds,erocetin,factagard,felexin,ibilex,ibrexin,inphalex,kefalospes,keflet,keflex,kefolan,keforal,keftab,kekrinal,kidolex,lafarine,larixin,lenocef,lexibiotico,lonflex,lopilexin,madlexin,mamalexin,mamlexin,medoxine,neokef,neolexina,novolexin,optocef,oracef,oriphex,oroxin,ortisporina,ospexin,palitrex,panixine disperdose,pectril,pyassan,roceph,roceph distab,sanaxin,sartosona,sencephalin,sepexin,servispor,sialexin,sinthecillin,sporicef,sporidex,syncle,synecl,tepaxin,tokiolexin,uphalexin,voxxim,winlex,zozarine</t>
+          <t>adcadina,alcephin,alexin,alfatil,alfatil kapseln,alsporin,ambal,amplex,cephalexin,aristosporin,azabort,bactopenor,beliam,biocef,carnosporin,ceclor,cefablan,cefacet,cefachlor,cefaclor monohydrate,cefadal,cefadin,cefadina,cefalekey,cefaleksin,cefalessina,cefalexgobens,cefalexin generics,cefalexina,cefalexina northia,cefalexina richet,cefalexine,cefalexinum,cefalin,cefalival,cefaloto,cefanex,cefaseptin,ceffanex,cefibacter,ceflax,ceforal,cefovit,celexin,cepastar,cepexin,cephacillin,cephalex von,cephalexine,cephalexinum,cephalobene,cephanasten,cephaxin,cephin,ceporex,ceporex forte,ceporexin,ceporexine,cerexin,cerexins,cophalexin,distaclor,domucef,doriman,durantel,efemida,erocetin,factagard,felexin,henina,ibilex,ibrexin,inphalex,karilexina,kefalospes,keflet,keflex,keflor,kefolan,kefolor,kefolor suspension,keforal,keftab,kekrinal,kidolex,lafarine,larixin,lenocef,lexibiotico,loisine,lonflex,lopilexin,losporal,madlexin,maksipor,mamalexin,mamlexin,medolexin,medoxine,muco panoral,neokef,neolexina,noveol,novolexin,optocef,oracef,oriphex,oroxin,ortisporina,ospexin,palitrex,panacef,panixine,panixine disperdose,panoral,pectril,prindex,pyassan,raniclor,rilexine,roceph,roceph distab,rogevil,sanaxin,sartosona,sencephalin,sepexin,servicef,servispor,sialexin,sinthecillin,sintolexyn,sporicef,sporidex,syncle,synecl,tepaxin,theratrex,tokiolexin,uphalexin,viosporine,voxxim,winlex,zabytrex,zozarine</t>
         </is>
       </c>
       <c r="J55">
@@ -3810,7 +3810,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>aliporina,ampligram,cefaloridin,cefaloridina,cefaloridine,cefaloridinum,cefalorizin,ceflorin,cepaloridin,cepalorin,cephalomycine,cephaloridin,cephaloridine,cephaloridinum,ceporan,ceporin,ceporine,cilifor,deflorin,faredina,floridin,glaxoridin,intrasporin,keflodin,keflordin,kefloridin,kefspor,lloncefal,loridine,sasperin,sefacin,verolgin,vioviantine</t>
+          <t>aliporina,ampligram,cefaloridin,cefaloridina,cefaloridinum,cefalorizin,ceflorin,cepaloridin,cepalorin,cephalomycine,cephaloridin,cephaloridine,cephaloridinum,ceporan,ceporin,ceporine,cilifor,deflorin,faredina,floridin,glaxoridin,intrasporin,keflodin,keflordin,kefloridin,kefspor,lloncefal,loridine,sasperin,sefacin,verolgin,vioviantine</t>
         </is>
       </c>
       <c r="J56" t="e">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>cefalothin,cefalotin,cefalotina,cefalotina fabra,cefalotine,cefalotinum,cemastin,cephalothinum,cephalotin,cephalotin acid,coaxin,keflin,seffin</t>
+          <t>cefalothin,cefalothine,cefalotina,cefalotina fabra,cefalotina sodica,cefalotine,cefalotinsalt,cefalotinum,cemastin,cephalothin,cephalothinsalt,cephalothinum,cephalotin,cephalotin acid,cephalotinsalt,ceporacin,cepovenin,cet injektionsfl,coaxin,keflin,lospoven,microtin,seffin,synclotin,tokiosarl ampullen,toricelocin</t>
         </is>
       </c>
       <c r="J57" t="e">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>cefadole,cefamandol,cefamandole,cefamandolum,cephadole,cephamandole,kefamandol,kefdole,mancef</t>
+          <t>cefadole,cefamandol,cefamandolesalt,cefamandolum,cephadole,cephamandole,kefamandol,kefdole,mancef</t>
         </is>
       </c>
       <c r="J58" t="e">
@@ -4002,7 +4002,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>ambrocef,cefadyl,cefapilin,cefapirin,cefapirina,cefapirine,cefapirinum,cefaprin,cefaprin sodium,cefatrex,cefatrexyl,cephapirine,metricure</t>
+          <t>ambrocef,brisfirina,brisporin,bristocef,cefa lak,cefadyl,cefalak,cefaloject,cefapilin,cefapirina,cefapirina sodica,cefapirine,cefapirinsalt,cefapirinum,cefaprin,cefatrex,cefatrexyl,cephapirin,cephapirine,cephapirinsalt,cephatrexil,cephatrexyl,metricure</t>
         </is>
       </c>
       <c r="J59" t="e">
@@ -4066,7 +4066,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>bricef,cefatrix,cefatrizine,cefatrizino,cefatrizinum,cephatriazine,cepticol,cetrazil,latocef,orosporina,trizina</t>
+          <t>bricef,cefatrix,cefatrizino,cefatrizinum,cephatriazine,cepticol,cetrazil,latocef,orosporina,orotric,seapuro,seapuron,trizina</t>
         </is>
       </c>
       <c r="J60">
@@ -4130,7 +4130,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>cefazedon,cefazedona,cefazedone,cefazedone acid,cefazedonum,refosporen,refosporene,refosporin</t>
+          <t>cefazedon,cefazedona,cefazedone acid,cefazedonesalt,cefazedonum,refosporen,refosporene,refosporin</t>
         </is>
       </c>
       <c r="J61" t="e">
@@ -4194,7 +4194,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>atirin,cefamezin,cefamezine,cefazina,cefazolin,cefazolin acid,cefazolina,cefazoline,cefazolinum,cephamezine,cephazolidin,cephazolin,cephazoline,elzogram,firmacef,kefzol,liviclina,totacef</t>
+          <t>ancef,atirin,biazolina,cefabiozim,cefacidal,cefalomicina,cefamedin,cefamezin,cefamezine,cefazil,cefazina,cefazolin acid,cefazolina,cefazoline,cefazolinsalt,cefazolinum,cephamezine,cephazolidin,cephazolin,cephazoline,elzogram,firmacef,gramaxin,kefzol,lampocef,liviclina,neofazol,recef,totacef,zolicef,zolin,zolisint</t>
         </is>
       </c>
       <c r="J62" t="e">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>cefbuperazona,cefbuperazone,cefbuperazonum,cefbuperzaone,cerbuperazone,tomiporan</t>
+          <t>cefbuperazona,cefbuperazonesalt,cefbuperazonum,cefbuperzaone,cerbuperazone,keiperazon,tomiporan</t>
         </is>
       </c>
       <c r="J63" t="e">
@@ -4314,7 +4314,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>cefcamate,cefcapene</t>
+          <t>cefcamate</t>
         </is>
       </c>
       <c r="J64">
@@ -4374,7 +4374,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>cefcamate pivoxil,cefcapene piroxil</t>
+          <t>cefcamate,cefcamate pivoxil,cefcapene piroxil,flomox,flumax</t>
         </is>
       </c>
       <c r="J65" t="e">
@@ -4436,7 +4436,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>cefdinir,cefdinir anhydrous,cefdinirum,cefdinyl,cefdirnir,ceftinex,cefzon,omnicef</t>
+          <t>cefdinir impurity g,cefdinirum,cefdinyl,cefdirnir,ceftinex,cefzon,omnicef</t>
         </is>
       </c>
       <c r="J66">
@@ -4500,7 +4500,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>cefditoren</t>
+          <t>spectracef</t>
         </is>
       </c>
       <c r="J67">
@@ -4560,7 +4560,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>cefditoren,cefditoren pi voxil,cefditoren pivoxil,cefditorin,cefditorin pivoxil,meiact,spectracef</t>
+          <t>cefditoren pi voxil,cefditorin,cefditorin pivoxil,meiact,spectracef</t>
         </is>
       </c>
       <c r="J68" t="e">
@@ -4622,7 +4622,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>axepim,cefepima,cefepime,cefepimum,cepimax,cepimex,maxcef,maxipime</t>
+          <t>axepim,cefepima,cefepimum,cepimax,cepimex,maxcef,maxipime</t>
         </is>
       </c>
       <c r="J69" t="e">
@@ -4980,7 +4980,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>cefetamet,cefetametum,cepime o,deacetoxycefotaxime</t>
+          <t>cefetametum,cepime o,deacetoxycefotaxime,epocelin</t>
         </is>
       </c>
       <c r="J75">
@@ -5040,7 +5040,7 @@
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>cefetamet pivoxyl,globocef</t>
+          <t>cefetamet pivoxyl,cefetametpivoxil,ceftamet pivoxil,cefyl,globocef</t>
         </is>
       </c>
       <c r="J76" t="e">
@@ -5098,7 +5098,7 @@
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>cefetecol,cefetecol anhydrous</t>
+          <t/>
         </is>
       </c>
       <c r="J77" t="e">
@@ -5156,7 +5156,7 @@
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>cefetrizole,cefetrizolum</t>
+          <t>cefetrizolum</t>
         </is>
       </c>
       <c r="J78" t="e">
@@ -5214,7 +5214,7 @@
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>cefiderocol</t>
+          <t>fetcroja</t>
         </is>
       </c>
       <c r="J79" t="e">
@@ -5278,7 +5278,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>anhydrous cefixime,cefixim,cefixima,cefixime,cefixime anhydrous,cefixime hydrate,cefiximum,cefixoral,cefspan,cephoral,citropen,denvar,necopen,oroken,suprax,tricef,unixime</t>
+          <t>cefixim,cefixima,cefixime impurity d,cefiximum,cefixoral,cefspan,cephoral,citropen,denvar,necopen,oroken,suprax,tricef,unixime</t>
         </is>
       </c>
       <c r="J80">
@@ -5404,7 +5404,7 @@
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>bestron,cefmax,cefmenoxima,cefmenoxime,cefmenoximum</t>
+          <t>bestron,cefmax,cefmenoxima,cefmenoximum,cemix,tacef</t>
         </is>
       </c>
       <c r="J82" t="e">
@@ -5468,7 +5468,7 @@
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>cefmetazole,cefmetazolesodium,cefmetazolo,cefmetazolum</t>
+          <t>cefmetazolesalt,cefmetazolesodium,cefmetazolo,cefmetazolum,cefmetazon,metafar,zefazone</t>
         </is>
       </c>
       <c r="J83" t="e">
@@ -5528,7 +5528,7 @@
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>cefminox,cefminoxum</t>
+          <t>alteporina,cefminoxum,meicelin,tencef</t>
         </is>
       </c>
       <c r="J84" t="e">
@@ -5592,7 +5592,7 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>cefodizima,cefodizime,cefodizime acid,cefodizime disodium,cefodizimum,cefodizme,diezime,modivid,neucef,timecef</t>
+          <t>cefodizima,cefodizime acid,cefodizime disalt,cefodizime disodium,cefodizimum,cefodizme,diezime,kenicef,modivid,neucef,timecef</t>
         </is>
       </c>
       <c r="J85" t="e">
@@ -5656,7 +5656,7 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>cefonicid,cefonicido,cefonicidum,monocef</t>
+          <t>cefonicid disalt,cefonicide,cefonicido,cefonicidsalt,cefonicidum,monocef,monocid</t>
         </is>
       </c>
       <c r="J86" t="e">
@@ -5720,7 +5720,7 @@
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>bioperazone,cefobid,cefoperazine,cefoperazon,cefoperazone,cefoperazone acid,cefoperazono,cefoperazonum,cefozon,medocef,myticef,pathozone,peracef</t>
+          <t>bioperazone,cefobid,cefobis,cefoneg,cefoper,cefoperazin,cefoperazine,cefoperazon,cefoperazone acid,cefoperazonesalt,cefoperazono,cefoperazonum,cefozon,medocef,myticef,pathozone,peracef,tomabef</t>
         </is>
       </c>
       <c r="J87" t="e">
@@ -5848,7 +5848,7 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>ceforanide,ceforanido,ceforanidum,precef,radacef</t>
+          <t>ceforanido,ceforanidum,precef,radacef</t>
         </is>
       </c>
       <c r="J89" t="e">
@@ -5908,7 +5908,7 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>cefoselis,cefoselis sulfate,wincef,winsef</t>
+          <t>wincef,winsef</t>
         </is>
       </c>
       <c r="J90" t="e">
@@ -5970,7 +5970,7 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>cefotaxim,cefotaxim hikma,cefotaxima,cefotaxima acid,cefotaxime,cefotaxime acid,cefotaximum,cephotaxime,claforan,omnatax</t>
+          <t>anticefotaxime,cefotax,cefotaxim,cefotaxim hikma,cefotaxima,cefotaxima acid,cefotaxime acid,cefotaximeimpurity d,cefotaximesalt,cefotaximsalt,cefotaximum,cephotaxime,claforan,kefotex,omnatax,pretor,ralopar,tolycar,tolycor,zariviz</t>
         </is>
       </c>
       <c r="J91" t="e">
@@ -6150,7 +6150,7 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>apacef,cefotan,cefotetan,cefotetan acid,cefotetan free acid,cefotetanum</t>
+          <t>apacef,cefotan,cefotetan acid,cefotetan free acid,cefotetanum</t>
         </is>
       </c>
       <c r="J94" t="e">
@@ -6214,7 +6214,7 @@
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>cefotiam,cefotiam?,cefotiamum,ceradolan,ceradon,haloapor</t>
+          <t>cefotiam?,cefotiamum,ceradolan,ceradon,haloapor,halospor,pansporin,pansporin ampullen,pansporine,spizef</t>
         </is>
       </c>
       <c r="J95">
@@ -6276,7 +6276,7 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>cefotiam cilexetil,pansporin t</t>
+          <t>cefotiam cilexetil,pansporin t,taketiam,texodil</t>
         </is>
       </c>
       <c r="J96" t="e">
@@ -6334,7 +6334,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>cefovecin</t>
+          <t>cefovecinsalt,convenia</t>
         </is>
       </c>
       <c r="J97" t="e">
@@ -6396,7 +6396,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>cefoxitin,cefoxitina,cefoxitine,cefoxitinum,cefoxotin,cenomycin,cephoxitin,mefoxin,mefoxitin,rephoxitin</t>
+          <t>betacef,cefoxil,cefoxitina,cefoxitine,cefoxitinsalt,cefoxitinum,cefoxotin,cenomycin,cephoxitin,farmoxin,mefoxin,mefoxithin,mefoxitin,merxin,rephoxitin</t>
         </is>
       </c>
       <c r="J98" t="e">
@@ -6514,7 +6514,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>cefozopran</t>
+          <t>cefozopran?,firstcin</t>
         </is>
       </c>
       <c r="J100" t="e">
@@ -6574,7 +6574,7 @@
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>cefpimizol,cefpimizole,cefpimizole sodium,cefpimizolum</t>
+          <t>cefpimizol,cefpimizolesalt,cefpimizolum,renilan</t>
         </is>
       </c>
       <c r="J101" t="e">
@@ -6636,7 +6636,7 @@
       </c>
       <c r="I102" t="inlineStr">
         <is>
-          <t>cefpiramide,cefpiramide acid,cefpiramido,cefpiramidum</t>
+          <t>cefpiramide acid,cefpiramidesalt,cefpiramido,cefpiramidum,sepatren,suncefal,tamicin</t>
         </is>
       </c>
       <c r="J102" t="e">
@@ -6700,7 +6700,7 @@
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>broact,cefpiroma,cefpirome,cefpiromum,cefrom,cerfpirome,keiten</t>
+          <t>broact,cefpiroma,cefpiromum,cefrom,cerfpirome,keiten,romecef</t>
         </is>
       </c>
       <c r="J103" t="e">
@@ -6764,7 +6764,7 @@
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>cefpodoxim acid,cefpodoxima,cefpodoxime,cefpodoxime acid,cefpodoximum,epoxim</t>
+          <t>anticefotaxime,cefotax,cefotaxim,cefotaxime acid,cefotaximeimpurity d,cefpodoxim acid,cefpodoxima,cefpodoxime acid,cefpodoximum,claforan,epoxim,kefotex</t>
         </is>
       </c>
       <c r="J104">
@@ -6824,7 +6824,7 @@
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>cefodox,cefoprox,cefpodoxime proxetil,cepodem,orelox,orelox paed,otreon,podomexef,simplicef,vantin</t>
+          <t>cefodox,cefodoxime proxetil,cefoprox,cefpodoximproxetil,cepodem,orelox,orelox paed,otreon,podomexef,simplicef,vantin</t>
         </is>
       </c>
       <c r="J105" t="e">
@@ -6944,7 +6944,7 @@
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>arzimol,brisoral,cefprozil,cefprozil anhydrous,cefprozil hydrate,cefprozilo,cefprozilum,cefzil,cronocef,procef,serozil</t>
+          <t>arzimol,brisoral,cefprozilo,cefprozilum,cefzil,cronocef,procef,serozil</t>
         </is>
       </c>
       <c r="J107">
@@ -7004,7 +7004,7 @@
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>cefquinoma,cefquinome,cefquinomum,cobactan</t>
+          <t>cefquinoma,cefquinomum,cobactan</t>
         </is>
       </c>
       <c r="J108" t="e">
@@ -7066,7 +7066,7 @@
       </c>
       <c r="I109" t="inlineStr">
         <is>
-          <t>cefroxadin,cefroxadine,cefroxadino,cefroxadinum,oraspor</t>
+          <t>cefroxadin,cefroxadin dihydrate,cefroxadino,cefroxadinum,oraspor</t>
         </is>
       </c>
       <c r="J109">
@@ -7130,7 +7130,7 @@
       </c>
       <c r="I110" t="inlineStr">
         <is>
-          <t>cefonomil,cefsulodin,cefsulodine,cefsulodino,cefsulodinum</t>
+          <t>cefomonil,cefonomil,cefsulodine,cefsulodino,cefsulodinsalt,cefsulodinum,pseudocef,pseudomonil,pyocefal,sulcephalosporin,takesulin,tilmapor,ulfaret</t>
         </is>
       </c>
       <c r="J110" t="e">
@@ -7190,7 +7190,7 @@
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>cefsulmid,cefsumide,cefsumido,cefsumidum</t>
+          <t>cefsulmid,cefsumido,cefsumidum</t>
         </is>
       </c>
       <c r="J111" t="e">
@@ -7248,7 +7248,7 @@
       </c>
       <c r="I112" t="inlineStr">
         <is>
-          <t>ceftaroline fosamil,teflaro,zinforo</t>
+          <t>ceftaroine,ceftaroline fosamil,teflaro,zinforo</t>
         </is>
       </c>
       <c r="J112" t="e">
@@ -7370,7 +7370,7 @@
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>ceftazidim,ceftazidima,ceftazidime,ceftazidimum,ceptaz,fortaz,fortum,pentacef,tazicef,tazidime</t>
+          <t>ceftazidim,ceftazidima,ceftazidimum,ceftazimide,ceptaz,fortam,fortaz,fortum,glazidim,modacin,pentacef,tazicef,tazidime</t>
         </is>
       </c>
       <c r="J114" t="e">
@@ -7552,7 +7552,7 @@
       </c>
       <c r="I117" t="inlineStr">
         <is>
-          <t>cefteram,cefterame,cefteramum,ceftetrame</t>
+          <t>cefterame,cefteramum,ceftetrame</t>
         </is>
       </c>
       <c r="J117">
@@ -7612,7 +7612,7 @@
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>cefteram pivoxil,cefterampivoxil,tomiron</t>
+          <t>cefterampivoxil,tomiron</t>
         </is>
       </c>
       <c r="J118" t="e">
@@ -7674,7 +7674,7 @@
       </c>
       <c r="I119" t="inlineStr">
         <is>
-          <t>ceftezol,ceftezole,ceftezolo,ceftezolum,demethylcefazolin</t>
+          <t>alomen,ceftezol,ceftezolesalt,ceftezolo,ceftezolum,celoslin,demethylcefazolin,falomesin</t>
         </is>
       </c>
       <c r="J119" t="e">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="I120" t="inlineStr">
         <is>
-          <t>ceftem,ceftibuten,ceftibuten dihydrate,ceftibuten hydrate,ceftibutene,ceftibuteno,ceftibutenum,ceftibutin,cephem,ceprifran,isocef,keimax</t>
+          <t>cedax,ceftem,ceftibuten dihydrate,ceftibutene,ceftibuteno,ceftibutenum,ceftibutin,cephem,ceprifran,isocef,keimax,seftem</t>
         </is>
       </c>
       <c r="J120">
@@ -7798,7 +7798,7 @@
       </c>
       <c r="I121" t="inlineStr">
         <is>
-          <t>ceftiofur,ceftiofurum,excede,excenel,naxcel</t>
+          <t>ceftiofurum,excede,excenel,naxcel</t>
         </is>
       </c>
       <c r="J121" t="e">
@@ -7860,7 +7860,7 @@
       </c>
       <c r="I122" t="inlineStr">
         <is>
-          <t>cefizox,ceftisomin,ceftix,ceftizoxima,ceftizoxime,ceftizoximum,epocelin,eposerin</t>
+          <t>cefizox,ceftisomin,ceftix,ceftizoxima,ceftizoximesalt,ceftizoximum,epocelin,eposerin</t>
         </is>
       </c>
       <c r="J122" t="e">
@@ -7978,7 +7978,7 @@
       </c>
       <c r="I124" t="inlineStr">
         <is>
-          <t>ceftobiprole</t>
+          <t/>
         </is>
       </c>
       <c r="J124" t="e">
@@ -8040,7 +8040,7 @@
       </c>
       <c r="I125" t="inlineStr">
         <is>
-          <t/>
+          <t>zevtera</t>
         </is>
       </c>
       <c r="J125" t="e">
@@ -8168,7 +8168,7 @@
       </c>
       <c r="I127" t="inlineStr">
         <is>
-          <t>biotrakson,cefatriaxone,cefatriaxone hydrate,ceftriaxon,ceftriaxona,ceftriaxone,ceftriaxone sodium,ceftriaxonum,ceftriazone,cephtriaxone,longacef,rocefin,rocephalin,rocephin,rocephine,rophex</t>
+          <t>biotrakson,cefatriaxone,ceftriaxon,ceftriaxona,ceftriaxonum,ceftriazone,cephtriaxone,longacef,rocefin,rocephalin,rocephin,rocephine,rophex</t>
         </is>
       </c>
       <c r="J127" t="e">
@@ -8296,7 +8296,7 @@
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>biofuroksym,cefuril,cefuroxim,cefuroxima,cefuroxime,cefuroxime acid,cefuroximine,cefuroximo,cefuroximum,cephuroxime,kefurox,sharox,zinacef,zinacef danmark</t>
+          <t>anaptivan,biociclin,biofuroksym,bioxima,cefofix,cefumax,cefurex,cefuril,cefurox,cefuroxim,cefuroxim curasan,cefuroxim fresenius,cefuroxim genericsn,cefuroxim hexal,cefuroxim lilly,cefuroxim norcox,cefuroxima,cefuroxima fabra,cefuroxima richet,cefuroxime acid,cefuroxime free acid,cefuroximeimpurity e,cefuroximesalt,cefuroximine,cefuroximo,cefuroximum,cephuroxime,cetroxil,colifossim,curoxim,curoxima,curoxime,froxal,furoxil,kefurox,kesint,ketocef,lifurox,medoxim,sharox,spectrazolr,ultroxim,zinacef,zinacef danmark,zinnat</t>
         </is>
       </c>
       <c r="J129">
@@ -8358,7 +8358,7 @@
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>altacef,bioracef,cefaks,cefazine,ceftin,cefurax,cefuroximaxetil,cefuroxime,cefuroxime axetil,celocid,cepazine,cethixim,cetoxil,coliofossim,elobact,forcef,furoxime,kalcef,maxitil,medoxm,nivador,novador,novocef,oraxim,zinnat</t>
+          <t>altacef,bioracef,cefaks,cefazine,ceftin,cefurax,cefuroximaxetil,celocid,cepazine,cethixim,cetoxil,coliofossim,elobact,forcef,furoxime,kalcef,maxitil,medoxm,nivador,novador,novocef,oraxim,zinnat</t>
         </is>
       </c>
       <c r="J130" t="e">
@@ -8478,7 +8478,7 @@
       </c>
       <c r="I132" t="inlineStr">
         <is>
-          <t>cefuzonam,cefuzonam sodium,cefuzoname,cefuzonamum</t>
+          <t>cefuzoname,cefuzonamum,cefzoname,cosmosin,mtc.na</t>
         </is>
       </c>
       <c r="J132" t="e">
@@ -8540,7 +8540,7 @@
       </c>
       <c r="I133" t="inlineStr">
         <is>
-          <t>anspor,cefradin,cefradina,cefradine,cefradine hydrate,cefradinum,cekodin,cephradin,cephradine,cephradine anhydrous,cephradine hydrate,eskacef,infexin,megace f,megacef,sefril,velocef,velosef</t>
+          <t>anspor,cefradin,cefradina,cefradine,cefradine dihydrate,cefradinum,cekodin,cephradin,cephradine dihydrate,eskacef,infexin,megace f,megacef,sefril,velocef,velosef</t>
         </is>
       </c>
       <c r="J133">
@@ -8602,7 +8602,7 @@
       </c>
       <c r="I134" t="inlineStr">
         <is>
-          <t>cetocycline,cetocyline,cetotetrine,chelocardin</t>
+          <t>cetocyline,cetotetrine,chelocardin</t>
         </is>
       </c>
       <c r="J134" t="e">
@@ -8664,7 +8664,7 @@
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>alficetyn,ambofen,amphenicol,amphicol,amseclor,anacetin,aquamycetin,austracil,austracol,biocetin,biophenicol,catilan,ch loramex,chemiceticol,chemicetin,chemicetina,chlomin,chlomycol,chloramex,chloramfenikol,chloramficin,chloramfilin,chloramphenicol,chloramphenicole,chloramphenicolum,chloramsaar,chlorasol,chlorbiotic,chloricol,chlormycetin r,chlornitromycin,chloroamphenicol,chlorocaps,chlorocid,chlorocid s,chlorocide,chlorocidin c,chlorocidin c tetran,chlorocin,chlorocol,chlorofair,chloroject l,chloromax,chloromycetin,chloromycetny,chloromyxin,chloronitrin,chloroptic,chloroptic s.o.p,chloroptic s.o.p.,chlorovules,chlorsig,cidocetine,ciplamycetin,cloramfen,cloramfenicol,cloramfenicolo,cloramficin,cloramical,cloramicol,cloramidina,cloranfenicol,cloroamfenicolo,clorocyn,cloromisan,cloromissan,clorosintex,comycetin,cylphenicol,desphen,detreomycin,detreomycine,dextromycetin,doctamicina,duphenicol,econochlor,embacetin,emetren,enicol,enteromycetin,erbaplast,ertilen,f armicetina,farmicetina,fenicol,globenicol,glorous,gloveticol,halcetin,halomycetin,hortfenicol,interomycetine,intramycetin,intramyctin,isicetin,ismicetina,isophenicol,isopto fenicol,juvamycetin,kamaver,kemicetina,kemicetine,kloramfenikol,klorita,klorocid s,laevomycetinum,leukamycin,leukomyan,leukomycin,levocin,levomicetina,levomitsetin,levomycetin,levoplast,levosin,levovetin,loromicetina,loromisan,loromisin,mastiphen,mediamycetine,medichol,micloretin,micochlorine,micoclorina,microcetina,mychel,mycinol,myclocin,mycochlorin,myscel,normimycin v,novochlorocap,novomycetin,novophenicol,ocuphenicol,oftalent,oleomycetin,opclor,opelor,ophthochlor,ophthocort,ophtochlor,optomycin,otachron,otophen,pantovernil,paraxin,pentamycetin,quemicetina,rivomycin,romphenil,ronfenil,ronphenil,septicol,sificetina,sintomicetin,sintomicetina,sintomicetine r,sno phenicol,soluthor,stanomycetin,synthomycetin,synthomycetine,synthomycine,syntomycin,tevcocin,tevcosin,tifomycin,tifomycine,tiromycetin,treomicetina,tyfomycine,unimycetin,veticol,vice ton,viceton</t>
+          <t>alficetyn,ambofen,amphenicol,amphicol,amseclor,anacetin,aquamycetin,austracil,austracol,biocetin,biophenicol,catilan,ch loramex,chemiceticol,chemicetin,chemicetina,chlomin,chlomycol,chloramex,chloramfenikol,chloramficin,chloramfilin,chloramphenicol levo,chloramphenicole,chloramphenicolum,chloramsaar,chlorasol,chlorbiotic,chloricol,chlormycetin r,chlornitromycin,chloroamphenicol,chlorocaps,chlorocid,chlorocid s,chlorocide,chlorocidin c,chlorocidin c tetran,chlorocin,chlorocol,chlorofair,chloroject l,chloromax,chloromycetin,chloromycetny,chloromyxin,chloronitrin,chloroptic,chloroptic s.o.p,chloroptic s.o.p.,chlorovules,chlorsig,cidocetine,ciplamycetin,cloramfen,cloramfenicol,cloramfenicolo,cloramficin,cloramical,cloramicol,cloramidina,cloranfenicol,cloroamfenicolo,clorocyn,cloromisan,cloromissan,clorosintex,comycetin,cylphenicol,desphen,detreomycin,detreomycine,dextramycin,dextromycetin,doctamicina,duphenicol,econochlor,embacetin,emetren,enicol,enteromycetin,erbaplast,ertilen,f armicetina,farmicetina,fenicol,globenicol,glorous,gloveticol,halcetin,halomycetin,hortfenicol,interomycetine,intramycetin,intramyctin,isicetin,ismicetina,isophenicol,isopto fenicol,juvamycetin,kamaver,kemicetina,kemicetine,kloramfenikol,klorita,klorocid s,laevomycetinum,leukamycin,leukomyan,leukomycin,levocin,levomicetina,levomitsetin,levomycetin,levoplast,levosin,levovetin,loromicetina,loromisan,loromisin,mastiphen,mediamycetine,medichol,micloretin,micochlorine,micoclorina,microcetina,mychel,mycinol,myclocin,mycochlorin,myscel,normimycin v,novochlorocap,novomycetin,novophenicol,ocuphenicol,oftalent,oleomycetin,opclor,opelor,ophthochlor,ophthocort,ophtochlor,optomycin,otachron,otophen,pantovernil,paraxin,pentamycetin,quemicetina,rivomycin,romphenil,ronfenil,ronphenil,septicol,sificetina,sintomicetin,sintomicetina,sintomicetine r,sno phenicol,soluthor,stanomycetin,synthomycetin,synthomycetine,synthomycine,syntomycin,tevcocin,tevcosin,tifomycin,tifomycine,tiromycetin,treomicetina,tyfomycine,unimycetin,veticol,vice ton,viceton</t>
         </is>
       </c>
       <c r="J135">
@@ -8730,7 +8730,7 @@
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>acronize,aueromycin,aureocina,aureomycin,aureomykoin,biomitsin,biomycin,biomycin a,chlormax,chlorotetracycline,chlortetracycline,chlortetracyclinum,chrysomykine,clortetraciclina,duomycin,flamycin,uromycin</t>
+          <t>acronize,alexomycin,aueromycin,aureocarmyl,aureociclina,aureocina,aureocycline,aureomycin,aureomykoin,auxeomycin,biomitsin,biomycin,biomycin a,chlormax,chlorotetracycline,chlortetracyclinum,chrysomykine,clorocipan,clortetraciclina,clortetrin,declomycin,declostatin,deganol,demeclor,demeplus,demetraciclina,demetraclin,detracin,detravis,diuciclin,duomycin,elkamicina,fermycin soluble,flamycin,isphamycin,ledermicina,ledermycin,ledermycine,mexocine,novotriclina,perciclina,periciclina,sumaclina,uromycin,veraciclina</t>
         </is>
       </c>
       <c r="J136">
@@ -8790,7 +8790,7 @@
       </c>
       <c r="I137" t="inlineStr">
         <is>
-          <t>bastcillin,calthor,ciclacilina,ciclacillin,ciclacilline,ciclacillinum,ciclacillum,citosarin,cyclacillin,cyclapen,noblicil,orfilina,peamezin,syngacillin,ultracillin,vastcillin,vipicil,wyvital</t>
+          <t>bastcillin,calthor,ciclacilina,ciclacilline,ciclacillinum,ciclacillum,citosarin,cyclacillin,cyclapen,noblicil,orfilina,peamezin,syngacillin,ultracillin,vastcillin,vipicil,wyvital</t>
         </is>
       </c>
       <c r="J137" t="e">
@@ -8852,7 +8852,7 @@
       </c>
       <c r="I138" t="inlineStr">
         <is>
-          <t>butaconazole,butoconazol,butoconazole,butoconazolum,ciclodan,ciclopirox,ciclopirox gel,ciclopirox olamin,ciclopiroxum,compositenstarke,dahlin,femstat,gynofort,loprox,loprox cream,loprox gel,penlac,polyfructosanum,stieprox</t>
+          <t>butaconazole,butoconazol,butoconazolum,ciclodan,ciclopirox gel,ciclopirox olamin,ciclopiroxum,compositenstarke,dahlin,femstat,gynofort,loprox,loprox cream,loprox gel,penlac,polyfructosanum,stieprox</t>
         </is>
       </c>
       <c r="J138" t="e">
@@ -8914,7 +8914,7 @@
       </c>
       <c r="I139" t="inlineStr">
         <is>
-          <t>azolinic acid,cinobac,cinobactin,cinoxacin,cinoxacine,cinoxacino,cinoxacinum,clinoxacin,noxigram,uronorm</t>
+          <t>azolinic acid,cinobac,cinobactin,cinoxacine,cinoxacino,cinoxacinum,clinoxacin,noxigram,uronorm</t>
         </is>
       </c>
       <c r="J139">
@@ -8978,7 +8978,7 @@
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>alcon cilox,auripro,bacquinor,baflox,baycip,bernoflox,cetraxal,ciflox,cifloxin,ciloxan,ciplus,ciprecu,ciprine,ciprinol,cipro i.v.,cipro iv,cipro xl,cipro xr,ciprobay,ciprobay uro,ciprocinol,ciprodar,ciproflox,ciprofloxacin,ciprofloxacina,ciprofloxacine,ciprofloxacino,ciprofloxacinum,ciprogis,ciprolin,ciprolon,cipromycin,ciproquinol,ciprowin,ciproxan,ciproxin,ciproxina,ciproxine,ciriax,citopcin,corsacin,cyprobay,fimoflox,flociprin,ipiflox,italnik,linhaliq,otiprio,probiox,proflaxin,quinolid,quintor,rancif,roxytal,septicide,sophixin ofteno,spitacin,superocin,velmonit,velomonit,zumaflox</t>
+          <t>alcipro,alcon cilox,auripro,bacquinor,baflox,baycip,belmacina,bernoflox,catex,cenin,ceprimax,cetraxal,ciflan,ciflosin,ciflox,cifloxin,cilox,ciloxan,cipad,ciplus,ciprecu,ciprenit,ciprine,ciprinol,cipro,ciprobay,ciprobay uro,ciprocinal,ciprocinol,ciprodar,ciproflox,ciprofloxacina,ciprofloxacine,ciprofloxacino,ciprofloxacinum,ciprofur,ciprogis,ciproktan,ciprolin,ciprolon,cipromycin,cipronex,cipropol,ciproquinol,ciprowin,ciproxan,ciproxin,ciproxina,ciproxine,ciriax,citeral,citopcin,corsacin,cunesin,cyprobay,cyproxan,disfabac,felixene,fimoflox,flociprin,floxacipron,flunas,globuce,inkamil,ipiflox,italnik,keefloxin,linhaliq,loxacid,lypro,megaflox,microgan,nixin,novidat,novoquin,ofitin,oftacilox,ophaflox,otiprio,phaproxin,piprol,plenolyt,probiox,proflaxin,proquin,proquinxr,proxacin,quinoflox,quinolid,quintor,quipro,rancif,renator,roflazin,roxytal,sepcen,septicide,septocipro,siprogut,sophixin,sophixin ofteno,spitacin,strox,suiflox,superocin,supraflox,uritent,utiminx,velmonit,velomonit,zumaflox</t>
         </is>
       </c>
       <c r="J140">
@@ -9230,7 +9230,7 @@
       </c>
       <c r="I144" t="inlineStr">
         <is>
-          <t>abbotic,astromen,biaxin,biaxin filmtab,biaxin hp,biaxin xl,biaxin xl filmtab,bicrolid,clacee,clacid,clacine,clambiotic,clarem,claribid,claricide,claridar,claripen,clarith,clarithromycin,clarithromycine,clarithromycinum,claritromicina,clathromycin,crixan,cyllid,cyllind,fromilid,heliclar,klabax,klacid,klaciped,klaricid,klaricid h.p,klaricid h.p.,klaricid pediatric,klaricid xl,klarid,klarin,kofron,mabicrol,macladin,maclar,prevpac,veclam,vikrol,zeclar</t>
+          <t>abbotic,abboticine,astromen,biaxin,biaxin filmtab,biaxin xl filmtab,bicrolid,bristamycin,clacee,clacid,clacine,clambiotic,clarem,claribid,claricide,claridar,claripen,clarith,clarithromycine,clarithromycinum,claritromicina,clathromycin,crixan,cyllid,cyllind,dowmycin e,durapaediat,e.e.s,e.e.s.,ees granules,eratrex,eryliquid,erypar,eryped,erythrocin,erythrocin stearate,erythrocin w,erythroped,esinol,ethril,fromilid,gallimycin,heliclar,klabax,klacid,klaciped,klaricid,klarid,klarin,kofron,mabicrol,macladin,maclar,meberyt,pediamycin,prevpac,qidmycin,refkas,veclam,vikrol,wyamycin,wyamycin e,wyamycin s,zeclar</t>
         </is>
       </c>
       <c r="J144">
@@ -9292,7 +9292,7 @@
       </c>
       <c r="I145" t="inlineStr">
         <is>
-          <t>acide clavulanique,acido clavulanico,acidum clavulanicum,clavulanate,clavulanate acid,clavulanate lithium,clavulanateacid,clavulanic acid,clavulansaeure,clavulansaure,clavulinic acid,clavulox,serdaxin,sodium clavulanate</t>
+          <t>acide clavulanique,acido clavulanico,acidum clavulanicum,amonate,clavulanate,clavulanate acid,clavulanate lithium,clavulanateacid,clavulansaeure,clavulansaure,clavulinic acid,clavulox,lithium clavulanate,serdaxin</t>
         </is>
       </c>
       <c r="J145" t="e">
@@ -9350,7 +9350,7 @@
       </c>
       <c r="I146" t="inlineStr">
         <is>
-          <t>clinafloxacin</t>
+          <t>spifloxacin</t>
         </is>
       </c>
       <c r="J146" t="e">
@@ -9412,7 +9412,7 @@
       </c>
       <c r="I147" t="inlineStr">
         <is>
-          <t>antirobe,chlolincocin,clindaderm,clindamicina,clindamycin,clindamycine,clindamycinum,clinimycin,dalacin c,dalacine,klimicin,sobelin</t>
+          <t>antirobe,antirobe aquadrops,antirobe capsules,benzaclin,chlolincocin,cleocin,clindacure,clindaderm,clindamed,clindamicina,clindamycine,clindamycinum,clinimycin,clinsol,clintabs,dalacin c,dalacine,klimicin,sobelin,zydaclin</t>
         </is>
       </c>
       <c r="J147">
@@ -9536,7 +9536,7 @@
       </c>
       <c r="I149" t="inlineStr">
         <is>
-          <t>chlofazimine,clofazimin,clofazimina,clofazimine,clofaziminum,colfazimine,lampren,lamprene,riminophenazine</t>
+          <t>chlofazimine,clofazimin,clofazimina,clofaziminum,colfazimine,lampren,lamprene,riminophenazine</t>
         </is>
       </c>
       <c r="J149">
@@ -9600,7 +9600,7 @@
       </c>
       <c r="I150" t="inlineStr">
         <is>
-          <t>clofoctol,clofoctolo,clofoctolum,gramplus,octofene</t>
+          <t>clofoctolo,clofoctolum,gramplus,octofene</t>
         </is>
       </c>
       <c r="J150" t="e">
@@ -9662,7 +9662,7 @@
       </c>
       <c r="I151" t="inlineStr">
         <is>
-          <t>chlomethocillin,clometacillin,clometocilina,clometocillin,clometocilline,clometocillinum,rixapen</t>
+          <t>chlomethocillin,clometacillin,clomethacillin,clomethocillin,clometocilina,clometocilline,clometocillinsalt,clometocillinum,rixapen</t>
         </is>
       </c>
       <c r="J151">
@@ -9726,7 +9726,7 @@
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>chlormethylencycline,clomociclina,clomocyclin,clomocycline,clomocyclinum,megaclor</t>
+          <t>alexomycin,aureocarmyl,aureociclina,aureocycline,aureomycin,auxeomycin,chlormethylencycline,clomociclina,clomocyclin,clomocyclinum,clorocipan,clortetrin,declomycin,declostatin,deganol,demeclor,demeplus,demetraciclina,demetraclin,detracin,detravis,diuciclin,elkamicina,fermycin soluble,isphamycin,ledermicina,ledermycin,ledermycine,megaclor,mexocine,novotriclina,perciclina,periciclina,sumaclina,veraciclina</t>
         </is>
       </c>
       <c r="J152">
@@ -9786,7 +9786,7 @@
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>canesten,canesten cream,canesten solution,canestene,canestine,canifug,chlotrimazole,cimitidine,clomatin,clotrimaderm,clotrimaderm cream,clotrimazol,clotrimazole,clotrimazolum,cutistad,desamix f,diphenylmethane,empecid,esparol,fem care,femcare,gyne lotrimin,jidesheng,kanesten,klotrimazole,lotrimax,lotrimin,lotrimin af,lotrimin af cream,lotrimin af lotion,lotrimin af solution,lotrimin cream,lotrimin lotion,lotrimin solution,monobaycuten,mycelax,mycelex,mycelex cream,mycelex g,mycelex otc,mycelex solution,mycelex troches,mycelex twin pack,myclo cream,myclo solution,myclo spray solution,mycofug,mycosporin,mykosporin,nalbix,otomax,pedisafe,rimazole,stiemazol,tibatin,trimysten,trivagizole,veltrim</t>
+          <t>canesten,canesten cream,canesten solution,canestene,canestine,canifug,chlotrimazole,cimitidine,clomatin,clotrimaderm,clotrimaderm cream,clotrimazol,clotrimazolum,cutistad,desamix f,diphenylmethane,empecid,esparol,fem care,femcare,gyne lotrimin,imidazole,jidesheng,kanesten,klotrimazole,lombazol,lombazole,lombazolum,lotrimax,lotrimin,lotrimin af cream,lotrimin af lotion,lotrimin af solution,lotrimin cream,lotrimin lotion,lotrimin solution,monobaycuten,mycelax,mycelex,mycelex cream,mycelex g,mycelex otc,mycelex solution,mycelex troches,mycelex twin pack,myclo cream,myclo solution,myclo spray solution,mycofug,mycosporin,mykosporin,nalbix,otomax,pedisafe,rimazole,stiemazol,tibatin,trimysten,trivagizole,veltrim</t>
         </is>
       </c>
       <c r="J153" t="e">
@@ -9848,7 +9848,7 @@
       </c>
       <c r="I154" t="inlineStr">
         <is>
-          <t>chloroxacillin,clossacillina,cloxacilina,cloxacillin,cloxacillin sodium,cloxacilline,cloxacillinna,cloxacillinum,cloxapen,methocillin s,orbenin,syntarpen,tegopen</t>
+          <t>ankerbin,austrastaph,biocloxin,brispen,chloroxacillin,ciclex,clocil,clossacillina,cloxacilina,cloxacillinanhydrous,cloxacilline,cloxacillinna,cloxacillinsalt,cloxacillinum,cloxapen,constaphyl,dariclox,dichlorstapenor,diclocil,dicloxacillinhydrate,diflor,digloxilline,dycill,dynapen,ekvacillin,gelstaph,methocillin s,novapen,noxaben,orbenin,pathocil,prevencilina p,prostaphilin a,prostaphlin a,stampen,staphcillin a banyu,staphybiotic,syntarpen,syntarpensalt,tegopen</t>
         </is>
       </c>
       <c r="J154">
@@ -9914,7 +9914,7 @@
       </c>
       <c r="I155" t="inlineStr">
         <is>
-          <t>belcomycine,colimycin,colimycin sulphate,colisticin,colistimethate,colistimethate sodium,colistin sulfate,colistin sulphate,colobreathe,colomycin,coly-mycin,polymyxin e,polymyxin e. sulfate,promixin,totazina</t>
+          <t>belcomycine,colimycin,colisticin,colisticina,colistimethate,colistina,colistine,colistinum,colobreathe,colomycin,coly-mycin,colymysin s,kangdisu,kolimitsin,polymyxin e,polymyxin e.,promixin,totazina</t>
         </is>
       </c>
       <c r="J155">
@@ -10038,7 +10038,7 @@
       </c>
       <c r="I157" t="inlineStr">
         <is>
-          <t>cicloserina,closerin,closina,cyclorin,cycloserin,cycloserine,cycloserinum,farmiserina,micoserina,miroserina,miroseryn,novoserin,oxamicina,oxamycin,seromycin,tebemicina,tisomycin,wasserina</t>
+          <t>cicloserina,closerin,closina,cyclorin,cycloserin,cycloserinum,farmiserina,levcicloserina,levcycloserine,levcycloserinum,micoserina,miroserina,miroseryn,novoserin,oxamicina,oxamycin,seromycin,tebemicina,tisomycin,wasserina</t>
         </is>
       </c>
       <c r="J157">
@@ -10102,7 +10102,7 @@
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>dalbavancin,dalvance</t>
+          <t>dalbavancin?,dalbavancina,dalvance,zeven</t>
         </is>
       </c>
       <c r="J158" t="e">
@@ -10162,7 +10162,7 @@
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>advocin,danofloxacin,danofloxacine,danofloxacino,danofloxacinum</t>
+          <t>advocin,danofloxacine,danofloxacino,danofloxacinum</t>
         </is>
       </c>
       <c r="J159" t="e">
@@ -10224,7 +10224,7 @@
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>aczone,araldite ht,atrisone,avlosulfon,avlosulfone,avlosulphone,avsulfor,bis sulfone,bissulfone,bissulphone,croysulfone,croysulphone,dapson,dapsona,dapsone,dapsonum,di sulfone,diaphenyl sulfone,diaphenylsulfon,diaphenylsulfone,diaphenylsulphon,diaphenylsulphone,dimitone,diphenasone,diphone,disulfone,disulone,disulphone,dubronax,dubronaz,dumitone,eporal,metabolite c,novophone,protogen,servidapson,slphadione,sulfadione,sulfona,sulfone ucb,sulfonyldianiline,sulphadione,sulphonyldianiline,sumicure s,tarimyl,udolac</t>
+          <t>aczone,araldite,atrisone,avlosulfon,avlosulfone,avlosulphone,avsulfor,bis sulfone,bis sulfoxide,bissulfone,bissulphone,croysulfone,croysulphone,dapson,dapsona,dapsonum,di sulfone,di sulfoxide,diaphenyl sulfone,diaphenylsulfon,diaphenylsulfone,diaphenylsulphon,diaphenylsulphone,dimitone,diphenasone,diphone,disulfone,disulone,disulphone,dubronax,dubronaz,dumitone,eporal,medapsol,metabolite c,novophone,protogen,servidapson,slphadione,sulfadione,sulfona,sulfone ucb,sulfonyldianiline,sulphadione,sulphonyldianiline,sumicure s,tarimyl,udolac</t>
         </is>
       </c>
       <c r="J160">
@@ -10288,7 +10288,7 @@
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>cidecin,cubicin,dapcin,daptomicina,daptomycine,daptomycinum</t>
+          <t>cidecin,cubicin,dapcin,daptomicina,daptomycin for,daptomycine,daptomycinum,dapzura,deptomycin</t>
         </is>
       </c>
       <c r="J161" t="e">
@@ -10348,7 +10348,7 @@
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>baxdela,delafloxacin,delafloxacinum,quofenix</t>
+          <t>baxdela,delafloxacinum,quofenix</t>
         </is>
       </c>
       <c r="J162">
@@ -10414,7 +10414,7 @@
       </c>
       <c r="I163" t="inlineStr">
         <is>
-          <t>delamanid,deltyba</t>
+          <t>deltyba</t>
         </is>
       </c>
       <c r="J163">
@@ -10478,7 +10478,7 @@
       </c>
       <c r="I164" t="inlineStr">
         <is>
-          <t>bioterciclin,clortetrin,declomycin,deganol,demeclociclina,demeclocycline,demeclocyclinum,demeclor,demetraclin,diuciclin,elkamicina,ledermycin,mexocine,novotriclina,perciclina,sumaclina</t>
+          <t>alexomycin,aureocarmyl,aureociclina,aureocycline,aureomycin,auxeomycin,bioterciclin,clorocipan,clortetrin,declomycin,declostatin,deganol,demeclociclina,demeclocyclinum,demeclor,demeplus,demetraciclina,demetraclin,detracin,detravis,diuciclin,elkamicina,fermycin soluble,isphamycin,ledermicina,ledermycin,ledermycine,mexocine,novotriclina,perciclina,periciclina,sumaclina,veraciclina</t>
         </is>
       </c>
       <c r="J164">
@@ -10542,7 +10542,7 @@
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>debecacin,dibekacin,dibekacin sulfate,dibekacina,dibekacine,dibekacinum,dideoxykanamycin b,kappati,orbicin,panamicin</t>
+          <t>debecacin,dibekacina,dibekacine,dibekacinum,dideoxykanamycin b,kappati,orbicin,panamicin</t>
         </is>
       </c>
       <c r="J165" t="e">
@@ -10606,7 +10606,7 @@
       </c>
       <c r="I166" t="inlineStr">
         <is>
-          <t>dichloroxacillin,diclossacillina,dicloxaciclin,dicloxacilin,dicloxacilina,dicloxacillin,dicloxacillin sodium,dicloxacillina,dicloxacilline,dicloxacillinum,dicloxacycline,dycill,dynapen,maclicine,nm|| dicloxacillin,pathocil</t>
+          <t>ankerbin,austrastaph,biocloxin,brispen,ciclex,clocil,cloxacillinanhydrous,cloxacillinsalt,constaphyl,dariclox,dichloroxacillin,dichlorstapenor,diclocil,diclossacillina,dicloxaciclin,dicloxacilin,dicloxacilina,dicloxacillina,dicloxacilline,dicloxacillinhydrate,dicloxacillinum,dicloxacycline,diflor,digloxilline,dycill,dynapen,ekvacillin,gelstaph,maclicine,nm|| dicloxacillin,novapen,noxaben,orbenin,pathocil,prevencilina p,prostaphilin a,prostaphlin a,stampen,staphcillin a banyu,staphybiotic,syntarpensalt,tegopen</t>
         </is>
       </c>
       <c r="J166">
@@ -10668,7 +10668,7 @@
       </c>
       <c r="I167" t="inlineStr">
         <is>
-          <t>dicural,difloxacin,pulsaflox</t>
+          <t>dicural,dicural tablets,pulsaflox</t>
         </is>
       </c>
       <c r="J167" t="e">
@@ -10730,7 +10730,7 @@
       </c>
       <c r="I168" t="inlineStr">
         <is>
-          <t>dirithromycin,dirithromycine,dirithromycinum,diritromicina,divitross,dynabac,noriclan,valodin</t>
+          <t>dirithromycine,dirithromycinum,diritromicina,divitross,dynabac,noriclan,valodin</t>
         </is>
       </c>
       <c r="J168">
@@ -10794,7 +10794,7 @@
       </c>
       <c r="I169" t="inlineStr">
         <is>
-          <t>doribax,doripenem,doripenem hydrate,finibax</t>
+          <t>doribax,dripenem,finibax</t>
         </is>
       </c>
       <c r="J169" t="e">
@@ -10858,7 +10858,7 @@
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>atridox,azudoxat,deoxymykoin,dossiciclina,doxcycline anhydrous,doxiciclina,doxirobe,doxitard,doxivetin,doxycen,doxychel,doxycin,doxycyclin,doxycycline,doxycycline calcium,doxycycline hyclate,doxycyclinum,doxylin,doxysol,doxytec,doxytetracycline,hydramycin,investin,jenacyclin,liviatin,monodox,oracea,periostat,ronaxan,spanor,supracyclin,vibramycin,vibramycin novum,vibramycine,vibravenos,zenavod</t>
+          <t>abbocin,alamycin,aquacycline,atridox,azudoxat,bi steclin,biosolvomycin,biotet,bisolvomycin,chrysocin,dalimycin,dalinmycin,deoxymykoin,dossiciclina,doxcycline,doxiciclina,doxirobe,doxitard,doxivetin,doxycen,doxychel,doxycin,doxycyclin,doxycycline calcium,doxycycline hyclate,doxycyclinum,doxylin,doxysol,doxytec,doxytetracycline,elinton,engemycin,hydramycin,hydrocyclin,imperacin,intaloxin,investin,jenacyclin,liquachel,liviatin,macodyn,mepatar,monodox,oracea,otetryn,oxacycline,oxamycen,oxatet,oxlopar,oxy,oxybiocycline,oxycycline,oxydon,oxyject,oxymykoin,oxysteclin,oxytet,oxytetracycline.hcl,oxytetral,oxytetrin,oxytracyl,oxyvet,periostat,ronaxan,spanor,stecsolin,supracyclin,terraject,terramycin,tetran hydrochloride,toxinal,unimycin,vendarcin,vibramycin,vibramycin novum,vibramycine,vibravenos,zenavod</t>
         </is>
       </c>
       <c r="J170">
@@ -10924,7 +10924,7 @@
       </c>
       <c r="I171" t="inlineStr">
         <is>
-          <t>econazol,econazole,econazolum,ecostatin,ecostatin cream,palavale,pevaryl,spectazole,spectazole cream</t>
+          <t>bromazil,chloramizol,clinafarm,deccosil,deccozil,econazol,econazolum,ecostatin,ecostatin cream,enilconazol,enilconazole,eniloconazol,fecundal,flo pro imz,flopro imz,florasan,freshgard,freshguard,fungaflor,fungazil,imaverol,imaversol,imazalil,imidazole,magnate,nuzone,palavale,pevaryl,rappor plus,spectazole,spectazole cream</t>
         </is>
       </c>
       <c r="J171" t="e">
@@ -10986,7 +10986,7 @@
       </c>
       <c r="I172" t="inlineStr">
         <is>
-          <t>almitil,bactidan,bactidron,comprecin,enofloxacine,enoksetin,enoram,enoxacin,enoxacina,enoxacine,enoxacino,enoxacinum,enoxen,enoxin,enoxor,flumark,penetrex</t>
+          <t>almitil,bactidan,bactidron,comprecin,enofloxacine,enoksetin,enoram,enoxacina,enoxacine,enoxacino,enoxacinum,enoxen,enoxin,enoxor,flumark,penetrex</t>
         </is>
       </c>
       <c r="J172">
@@ -11046,7 +11046,7 @@
       </c>
       <c r="I173" t="inlineStr">
         <is>
-          <t>baytril,enrofloxacin,enrofloxacine,enrofloxacino,enrofloxacinum,enroxil</t>
+          <t>baytril,enrofloxacine,enrofloxacino,enrofloxacinum,enroxil</t>
         </is>
       </c>
       <c r="J173" t="e">
@@ -11104,7 +11104,7 @@
       </c>
       <c r="I174" t="inlineStr">
         <is>
-          <t>enviomicina,enviomycin,enviomycina,enviomycinum,tuberactin</t>
+          <t>enviomicina,enviomycina,enviomycinum,tuberactin</t>
         </is>
       </c>
       <c r="J174" t="e">
@@ -11226,7 +11226,7 @@
       </c>
       <c r="I176" t="inlineStr">
         <is>
-          <t>dexacillin,dihydroampicillin,epicilina,epicillin,epicilline,epicillinum</t>
+          <t>dexacillin,dihydroampicillin,epicilina,epicilline,epicillinum</t>
         </is>
       </c>
       <c r="J176">
@@ -11288,7 +11288,7 @@
       </c>
       <c r="I177" t="inlineStr">
         <is>
-          <t>epiroprim,epiroprima,epiroprime,epiroprimum</t>
+          <t>epiroprima,epiroprime,epiroprimum</t>
         </is>
       </c>
       <c r="J177" t="e">
@@ -11350,7 +11350,7 @@
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>eravacycline,xerava</t>
+          <t>xerava</t>
         </is>
       </c>
       <c r="J178" t="e">
@@ -11414,7 +11414,7 @@
       </c>
       <c r="I179" t="inlineStr">
         <is>
-          <t>ertapenem,invanz</t>
+          <t>ertapenem?,ertapenemhydrate,ertapenemsalt,invanz</t>
         </is>
       </c>
       <c r="J179" t="e">
@@ -11478,7 +11478,7 @@
       </c>
       <c r="I180" t="inlineStr">
         <is>
-          <t>abboticin,abomacetin,acneryne,acnesol,akne cordes losung,aknederm ery gel,aknemycin,austrias,benzamycin,bristamycin,derimer,deripil,dotycin,dumotrycin,emuvin,emycin,endoeritrin,erecin,erisone,eritomicina,eritrocina,eritromicina,ermycin,eryacne,eryacnen,eryc sprinkles,erycen,erycette,erycin,erycinum,eryderm,erydermer,erygel,eryhexal,erymax,erymed,erypar,erysafe,erytab,erythrocin,erythrocin stearate,erythroderm,erythrogran,erythroguent,erythromid,erythromycin,erythromycin a,erythromycin base,erythromycin lactate,erythromycine,erythromycines,erythromycinum,erytop,erytrociclin,ilocaps,ilosone,iloticina,ilotycin,ilotycin gluceptate,ilotycin t.s.,inderm,inderm gel,indermretcin,latotryd,lederpax,mephamycin,mercina,oftamolets,paediathrocin,pantoderm,pantodrin,pantomicina,pce dispertab,pharyngocin,primacine,propiocine,proterytrin,retcin,robimycin,romycin,sansac,skid gel e,staticin,stiemicyn,stiemycin,theramycin z,tiloryth,tiprocin,torlamicina,udima ery gel,wyamycin s</t>
+          <t>abboticin,abboticine,abomacetin,acneryne,acnesol,akne cordes losung,aknederm ery gel,aknemycin,austrias,benzamycin,bristamycin,derimer,deripil,dotycin,dowmycin e,dumotrycin,durapaediat,e.e.s,e.e.s.,ees granules,emuvin,emycin,endoeritrin,eratrex,erecin,erisone,eritomicina,eritrocina,eritromicina,ermycin,eryacne,eryacnen,eryc sprinkles,erycen,erycette,erycin,erycinum,eryderm,erydermer,erygel,eryhexal,eryliquid,erymax,erymed,erypar,eryped,erysafe,erytab,erythrocin,erythrocin stearate,erythrocin w,erythroderm,erythrogran,erythroguent,erythromid,erythromycin a,erythromycin lactate,erythromycine,erythromycines,erythromycinum,erythroped,erytop,erytrociclin,esinol,ethril,gallimycin,ilocaps,ilosone,iloticina,ilotycin,ilotycin gluceptate,inderm,inderm gel,indermretcin,latotryd,lederpax,meberyt,mephamycin,mercina,oftamolets,paediathrocin,pantoderm,pantodrin,pantomicina,pce dispertab,pediamycin,pharyngocin,primacine,propiocine,proterytrin,qidmycin,refkas,retcin,robimycin,romycin,sansac,skid gel e,staticin,stiemicyn,stiemycin,theramycin z,tiloryth,tiprocin,torlamicina,udima ery gel,wyamycin,wyamycin e,wyamycin s</t>
         </is>
       </c>
       <c r="J180">
@@ -11544,7 +11544,7 @@
       </c>
       <c r="I181" t="inlineStr">
         <is>
-          <t>aethambutolum,diambutol,ebutol,etambutol,etambutolo,etapiam,ethambutol,ethambutolum,myambutol,mycobutol,purderal,servambutol,tibutol</t>
+          <t>aethambutolum,dadibutol,diambutol,ebutol,etambutol,etambutolo,etapiam,ethambutolum,myambutol,mycobutol,purderal,servambutol,tibutol</t>
         </is>
       </c>
       <c r="J181">
@@ -11672,7 +11672,7 @@
       </c>
       <c r="I183" t="inlineStr">
         <is>
-          <t>aethionamidum,aetina,aetiva,amidazin,amidazine,ethatyl,ethimide,ethina,ethinamide,ethionamide,ethionamidum,ethioniamide,ethylisothiamide,ethyonomide,etimid,etiocidan,etionamid,etionamida,etionamide,etioniamid,etionid,etionizin,etionizina,etionizine,fatoliamid,iridocin,iridocin bayer,iridozin,isothin,isotiamida,itiocide,nicotion,nisotin,nizotin,rigenicid,sertinon,teberus,thianid,thianide,thioamide,thiodine,thiomid,thioniden,tianid,tiomid,trecator,trecator sc,trekator,trescatyl,trescazide,tubenamide,tubermin,tuberoid,tuberoson</t>
+          <t>aethionamidum,aetina,aetiva,amidazin,amidazine,ethatyl,ethimide,ethina,ethinamide,ethionamidum,ethioniamide,ethylisothiamide,ethyonomide,etimid,etiocidan,etionamid,etionamida,etionamide,etioniamid,etionid,etionizin,etionizina,etionizine,fatoliamid,iridocin,iridocin bayer,iridozin,isothin,isotiamida,itiocide,nicotion,nisotin,nizotin,rigenicid,sertinon,teberus,thianid,thianide,thioamide,thiodine,thiomid,thioniden,tianid,tiomid,trecator,trekator,trescatyl,trescazide,tubenamide,tubermin,tuberoid,tuberoson</t>
         </is>
       </c>
       <c r="J183">
@@ -11732,7 +11732,7 @@
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>amprol plus,ethopabat,ethopabate,ethyl pabate</t>
+          <t>amprol plus,ethopabat,ethyl pabate</t>
         </is>
       </c>
       <c r="J184" t="e">
@@ -11850,7 +11850,7 @@
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>faropenem,faropenem sodium,fropenem,fropenum sodium</t>
+          <t>farom,faropenemhydrate,faropenemsalt,fropenem,fropenum,furopenem</t>
         </is>
       </c>
       <c r="J186">
@@ -11910,7 +11910,7 @@
       </c>
       <c r="I187" t="inlineStr">
         <is>
-          <t>dificid,dificlir,difimicin,fidaxomicin,lipiarmicin,lipiarmycin,lipiarrmycin,tiacumicin b</t>
+          <t>dificid,dificlir,difimicin,lipiarmicin,lipiarmycin,lipiarrmycin,tiacumicin b</t>
         </is>
       </c>
       <c r="J187">
@@ -11970,7 +11970,7 @@
       </c>
       <c r="I188" t="inlineStr">
         <is>
-          <t>finafloxacin</t>
+          <t/>
         </is>
       </c>
       <c r="J188" t="e">
@@ -12028,7 +12028,7 @@
       </c>
       <c r="I189" t="inlineStr">
         <is>
-          <t>flavophospholipol,moenomycin complex</t>
+          <t>bambermicina,bambermycin,bambermycine,bambermycinum,flavofosfolipol,flavophospholipol,gainpro,menomycin,moenomycin complex</t>
         </is>
       </c>
       <c r="J189" t="e">
@@ -12090,7 +12090,7 @@
       </c>
       <c r="I190" t="inlineStr">
         <is>
-          <t>fleroxacin,fleroxacine,fleroxacino,fleroxacinum,fleroxicin,megalocin,megalone,megalosin,quinodis</t>
+          <t>fleroxacine,fleroxacino,fleroxacinum,fleroxicin,megalocin,megalone,megalosin,quinodis</t>
         </is>
       </c>
       <c r="J190">
@@ -12152,7 +12152,7 @@
       </c>
       <c r="I191" t="inlineStr">
         <is>
-          <t>flomoxef,flomoxefo,flomoxefum</t>
+          <t>flomoxefo,flomoxefsalt,flomoxefum,flumarin</t>
         </is>
       </c>
       <c r="J191" t="e">
@@ -12212,7 +12212,7 @@
       </c>
       <c r="I192" t="inlineStr">
         <is>
-          <t>aquafen,florfenicol,nuflor,nuflor gold</t>
+          <t>aquafen,descocin,dexawin,dextrosulphenidol,efnicol,fricol,hyrazin,igralin,macphenicol,masatirin,neomyson,nuflor,nuflor gold,racephenicol,rincrol,thiamcol,thiamphenicol epimer,thiocymetin,urfamicina,urfamycine,urophenyl</t>
         </is>
       </c>
       <c r="J192" t="e">
@@ -12274,7 +12274,7 @@
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t>culpen,floxacillin,floxacillin sodium,floxapen,floxapen sodium salt,fluclox,flucloxacilina,flucloxacillin,flucloxacilline,flucloxacillinum,fluorochloroxacillin,staphylex</t>
+          <t>ankerbin,austrastaph,bactopen,cloxacap,cloxacillinanhydrous,cloxacillinhydrate,cloxacillinsalt,cloxapen,cloxypen,culpen,dariclox,ekvacillin,floxacillin,floxapen,floxapen sodium salt,fluclox,flucloxacilina,flucloxacilline,flucloxacillinum,fluorochloroxacillin,gelstaph,latocillin,orbenin,orbeninhydrate,prevencilina p,prostaphilin a,prostaphlin a,staphybiotic,staphylex,syntarpensalt,tegopen</t>
         </is>
       </c>
       <c r="J193">
@@ -12340,7 +12340,7 @@
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>alflucoz,alfumet,alkanazole,biocanol,biozole,biozolene,canzol,cryptal,diflazon,diflucan,dimycon,elazor,flucazol,fluconazol,fluconazole,fluconazole capsules,fluconazoli,fluconazolum,flucoral,flucostat,flukezol,flunazol,flunizol,flusol,fluzon,fluzone,forcan,fuconal,fungata,loitin,oxifugol,pritenzol,syscan,trican,triconal,triflucan,zoltec</t>
+          <t>alflucoz,alfumet,alkanazole,biocanol,biozole,biozolene,canzol,cryptal,diflazon,diflucan,dimycon,elazor,flucazol,fluconazol,fluconazole capsules,fluconazoli,fluconazolum,flucoral,flucostat,flukezol,flunazol,flunizol,flusol,fluzon,fluzone,forcan,fuconal,fungata,loitin,oxifugol,pritenzol,syscan,trican,triconal,triflucan,zoltec</t>
         </is>
       </c>
       <c r="J194">
@@ -12406,7 +12406,7 @@
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>alcobon,ancoban,ancobon,ancotil,ancotyl,flourocytosine,flucitosina,flucystine,flucytosin,flucytosine,flucytosinum,flucytosone,fluocytosine,fluorcytosine,fluorocytosine</t>
+          <t>alcobon,ancoban,ancobon,ancotil,ancotyl,flourocytosine,flucitosina,flucystine,flucytosin,flucytosinum,flucytosone,fluocytosine,fluorcytosine,fluorocytosine</t>
         </is>
       </c>
       <c r="J195">
@@ -12472,7 +12472,7 @@
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>apurone,fantacin,flumequine,flumequino,flumequinum,flumigal,flumiquil,flumisol,flumix,imequyl</t>
+          <t>apurone,fantacin,flumequino,flumequinum,flumigal,flumiquil,flumisol,flumix,imequyl</t>
         </is>
       </c>
       <c r="J196">
@@ -12536,7 +12536,7 @@
       </c>
       <c r="I197" t="inlineStr">
         <is>
-          <t>flurithromicina,flurithromycime,flurithromycin,flurithromycine,flurithromycinum,fluritromicina,fluritromycinum,flurizic</t>
+          <t>abboticine,beritromicina,berythromycin,berythromycine,berythromycinum,bristamycin,dowmycin e,eratrex,erypar,erythrocin,erythrocin stearate,erythromycin b,ethril,flurithromicina,flurithromycime,flurithromycine,flurithromycinum,fluritromicina,fluritromycinum,flurizic,gallimycin,meberyt,qidmycin,wyamycin s</t>
         </is>
       </c>
       <c r="J197">
@@ -12596,7 +12596,7 @@
       </c>
       <c r="I198" t="inlineStr">
         <is>
-          <t>fosfluconazole,phosfluconazole,procif,prodif</t>
+          <t>phosfluconazole,procif,prodif</t>
         </is>
       </c>
       <c r="J198" t="e">
@@ -12658,7 +12658,7 @@
       </c>
       <c r="I199" t="inlineStr">
         <is>
-          <t>calcium fosfomycin,fosfocina,fosfomicin,fosfomicina,fosfomycin,fosfomycin sodium,fosfomycine,fosfomycinum,fosfonomycin,infectophos,monuril,monurol,phosphonemycin,phosphonomycin,veramina</t>
+          <t>calcium fosfomycin,fosfocina,fosfomicin,fosfomicina,fosfomycine,fosfomycinum,fosfonomycin,infectophos,monuril,monurol,phosphonemycin,phosphonomycin,veramina</t>
         </is>
       </c>
       <c r="J199">
@@ -12720,7 +12720,7 @@
       </c>
       <c r="I200" t="inlineStr">
         <is>
-          <t>fosmidomycin,fosmidomycina,fosmidomycine,fosmidomycinum</t>
+          <t>fosmidomycina,fosmidomycine,fosmidomycinsalt,fosmidomycinsalt?,fosmidomycinum</t>
         </is>
       </c>
       <c r="J200" t="e">
@@ -12778,7 +12778,7 @@
       </c>
       <c r="I201" t="inlineStr">
         <is>
-          <t>actilin,actiline,antibiotique,bycomycin,dekamycin iii,endomixin,enterfram,fradiomycin,fradiomycin b,fradiomycinum,framicetina,framidal,framycetin,framycetin sulfate,framycetine,framycetinum,framycin,framygen,francetin,fraquinol,jernadex,myacine,myacyne,mycerin,mycifradin,neobrettin,neolate,neomas,neomcin,neomicina,neomin,neomycin,neomycin b,neomycin b sulfate,neomycin solution,neomycin sulfate,neomycin sulphate,neomycinb,neomycine,neomycinum,nivemycin,pimavecort,soframycin,soframycine,tuttomycin,vonamycin,vonamycin powder v</t>
+          <t>actilin,actiline,antibiotique,bycomycin,dekamycin iii,endomixin,enterfram,fradiomycin,fradiomycin b,fradiomycinum,framicetina,framidal,framycetine,framycetinum,framycin,framygen,francetin,fraquinol,jernadex,myacine,myacyne,mycerin,mycifradin,neobrettin,neolate,neomas,neomcin,neomicina,neomin,neomycin b,neomycin solution,neomycinb,neomycine,neomycinum,nivemycin,pimavecort,soframycin,soframycine,tuttomycin,vonamycin,vonamycin powder v</t>
         </is>
       </c>
       <c r="J201" t="e">
@@ -12840,7 +12840,7 @@
       </c>
       <c r="I202" t="inlineStr">
         <is>
-          <t>akritoin,furagin,furaginum,furamag,furazidin,furazidine</t>
+          <t>akritoin,furagin,furaginum,furamag,furazidine,nitro macro</t>
         </is>
       </c>
       <c r="J202">
@@ -12900,7 +12900,7 @@
       </c>
       <c r="I203" t="inlineStr">
         <is>
-          <t>bifuron,corizium,coryzium,diafuron,enterotoxon,furall,furaxon,furaxone,furazol,furazolidine,furazolidon,furazolidona,furazolidone,furazolidonum,furazolum,furazon,furidon,furovag,furox aerosol powder,furoxal,furoxane,furoxon,furoxone,furoxone liquid,furoxone swine mix,furozolidine,giardil,giarlam,medaron,neftin,nicolen,nifulidone,nifuran,nifurazolidone,nifurazolidonum,nitrofurazolidone,nitrofurazolidonum,nitrofuroxon,optazol,ortazol,puradin,roptazol,sclaventerol,tikofuran,topazone,trichofuron,tricofuron,tricoron,trifurox,viofuragyn</t>
+          <t>bifuron,corizium,coryzium,diafuron,enterotoxon,furall,furaxon,furaxone,furazol,furazolidine,furazolidon,furazolidona,furazolidonum,furazolum,furazon,furidon,furmethoxadone,furovag,furox aerosol powder,furoxal,furoxane,furoxon,furoxone,furoxone liquid,furoxone swine mix,furozolidine,giardil,giarlam,medaron,neftin,nicolen,nifulidone,nifuran,nifurazolidone,nifurazolidonum,nitrofuradoxadone,nitrofuradoxon,nitrofurazolidone,nitrofurazolidonum,nitrofuroxon,optazol,ortazol,puradin,roptazol,sclaventerol,tikofuran,topazone,trichofuron,tricofuron,tricoron,trifurox,viofuragyn</t>
         </is>
       </c>
       <c r="J203" t="e">
@@ -12962,7 +12962,7 @@
       </c>
       <c r="I204" t="inlineStr">
         <is>
-          <t>acide fusidique,acido fusidico,acidum fusidicum,flucidin,fucidate,fucidate sodium,fucidic acid,fucidin,fucidin acid,fucithalmic,fusidate,fusidate acid,fusidic acid,fusidicacid,fusidine,fusidinic acid,ramycin,taksta</t>
+          <t>acide fusidique,acido fusidico,acidum fusidicum,flucidin,fucidate,fucidic acid,fucidin,fucidin acid,fucidin leo,fucidina,fucidine,fucithalmic,fusidate,fusidate acid,fusidic acidsalt,fusidicacid,fusidin,fusidine,fusidinic acid,intertulle fucidin,ramycin,taksta</t>
         </is>
       </c>
       <c r="J204">
@@ -13024,7 +13024,7 @@
       </c>
       <c r="I205" t="inlineStr">
         <is>
-          <t>gamithromycin</t>
+          <t>azasite</t>
         </is>
       </c>
       <c r="J205" t="e">
@@ -13082,7 +13082,7 @@
       </c>
       <c r="I206" t="inlineStr">
         <is>
-          <t>ganefloxacin,garenfloxacin,garenoxacin</t>
+          <t>ganefloxacin,garenfloxacin,garenoxacin mesilate</t>
         </is>
       </c>
       <c r="J206">
@@ -13146,7 +13146,7 @@
       </c>
       <c r="I207" t="inlineStr">
         <is>
-          <t>gatiflo,gatifloxacin,gatifloxacin hydrate,gatifloxacine,gatifloxcin,gatilox,gatiquin,gatispan,tequin,tequin and zymar,zymaxid</t>
+          <t>acorafloxacin,avarofloxacin,balofloxacin,bilimin,gatiflo,gatifloxacine,gatifloxcin,gatilox,gatiquin,gatispan,tequin,tequin and zymar,zymaxid</t>
         </is>
       </c>
       <c r="J207">
@@ -13212,7 +13212,7 @@
       </c>
       <c r="I208" t="inlineStr">
         <is>
-          <t>factiv,factive,gemifioxacin,gemifloxacin,gemifloxacine,gemifloxacino,gemifloxacinum</t>
+          <t>factiv,factive,gemifioxacin,gemifloxacine,gemifloxacino,gemifloxacinum</t>
         </is>
       </c>
       <c r="J208">
@@ -13278,7 +13278,7 @@
       </c>
       <c r="I209" t="inlineStr">
         <is>
-          <t>apogen,centicin,cidomycin,garamycin,garasol,genoptic liquifilm,genoptic s.o.p.,gentacycol,gentafair,gentak,gentamar,gentamcin sulfate,gentamicin,gentamicina,gentamicine,gentamicins,gentamicinum,gentamycin,gentamycins,gentamycinum,gentavet,gentocin,jenamicin,lyramycin,oksitselanim,refobacin,refobacin tm,septigen,uromycine</t>
+          <t>apogen,centicin,cidomycin,garamycin,garasol,genoptic liquifilm,genoptic s.o.p.,gentacycol,gentafair,gentak,gentamar,gentamcin,gentamicin c,gentamicin cla,gentamicina,gentamicine,gentamicins,gentamicinum,gentamycin,gentamycins,gentamycinum,gentavet,gentocin,jenamicin,liposomal gentamicin,lyramycin,oksitselanim,refobacin,septigen,septocin,uromycine</t>
         </is>
       </c>
       <c r="J209" t="e">
@@ -13396,7 +13396,7 @@
       </c>
       <c r="I211" t="inlineStr">
         <is>
-          <t>gepotidacin</t>
+          <t/>
         </is>
       </c>
       <c r="J211" t="e">
@@ -13458,7 +13458,7 @@
       </c>
       <c r="I212" t="inlineStr">
         <is>
-          <t>grepafloxacin</t>
+          <t>lungaskin,raxar,vaxar</t>
         </is>
       </c>
       <c r="J212">
@@ -13518,7 +13518,7 @@
       </c>
       <c r="I213" t="inlineStr">
         <is>
-          <t>amudane,curling factor,delmofulvina,fulcin,fulcine,fulvican grisactin,fulvicin,fulvicin bolus,fulvidex,fulvina,fulvinil,fulvistatin,fungivin,greosin,gresfeed,gricin,grifulin,grifulvin,grifulvin v,grisactin,grisactin ultra,grisactin v,griscofulvin,grise ostatin,grisefuline,griseo,griseoflulvin,griseofulvin,griseofulvin forte,griseofulvina,griseofulvine,griseofulvinum,griseomix,griseostatin,grisetin,grisofulvin,grisovin,grisovin fp,grizeofulvin,grysio,guservin,lamoryl,likuden,likunden,murfulvin,poncyl,spirofulvin,sporostatin xan,xuanjing</t>
+          <t>amudane,curling factor,delmofulvina,fulcin,fulcine,fulvican grisactin,fulvicin,fulvicin bolus,fulvidex,fulvina,fulvinil,fulvistatin,fungivin,greosin,gresfeed,gricin,grifulin,grifulvin,grifulvin v,grisactin,grisactin ultra,grisactin v,griscofulvin,grise ostatin,grisefuline,griseo,griseoflulvin,griseofulvicacid,griseofulvin forte,griseofulvina,griseofulvine,griseofulvinum,griseomix,griseostatin,grisetin,grisofulvin,grisovin,grisowen,grizeofulvin,grysio,guservin,lamoryl,likuden,likunden,murfulvin,poncyl,spirofulvin,sporostatin xan,xuanjing</t>
         </is>
       </c>
       <c r="J213">
@@ -13578,7 +13578,7 @@
       </c>
       <c r="I214" t="inlineStr">
         <is>
-          <t>arbekacin sulfate,arbekacin sulphate,habekacin,habekacin sulfate,habekacin xsulfate,habekacinxsulfate</t>
+          <t>amikacin bis,amikacin disulfate,amikacini sulfas,amikafur,amikan,amikin,amitrex,arikayce,biklin,biodacyn,chemacin,fabianol,habekacin xsulfate,habekacinxsulfate,kaminax,likacin,pierami</t>
         </is>
       </c>
       <c r="J214" t="e">
@@ -13640,7 +13640,7 @@
       </c>
       <c r="I215" t="inlineStr">
         <is>
-          <t>cabimicina,hachimicina,hachimycin,hachimycine,hachimycinum,trichomycinum,trichonat</t>
+          <t>cabimicina,hachimicina,hachimycine,hachimycinum,trichomycinum,trichonat</t>
         </is>
       </c>
       <c r="J215" t="e">
@@ -13702,7 +13702,7 @@
       </c>
       <c r="I216" t="inlineStr">
         <is>
-          <t>etacillina,hetacilina,hetacillin,hetacillin acid,hetacilline,hetacillinum,phenazacillin,versapen</t>
+          <t>etacillina,hetacilina,hetacillin acid,hetacillin potassium,hetacilline,hetacillinum,natacillin,phenazacillin,polymast,potassium hetacillin,versapen,versatrex</t>
         </is>
       </c>
       <c r="J216">
@@ -13762,7 +13762,7 @@
       </c>
       <c r="I217" t="inlineStr">
         <is>
-          <t>antihelmycin,hydromycin b,hygrovetine</t>
+          <t>antihelmycin,destomycin a,destomysin,hyanthelmix,hydromycin b,hygrovectine,hygrovetine</t>
         </is>
       </c>
       <c r="J217" t="e">
@@ -13820,7 +13820,7 @@
       </c>
       <c r="I218" t="inlineStr">
         <is>
-          <t>ibrexafungerp</t>
+          <t/>
         </is>
       </c>
       <c r="J218" t="e">
@@ -13878,7 +13878,7 @@
       </c>
       <c r="I219" t="inlineStr">
         <is>
-          <t>iclaprim,mersarex</t>
+          <t>mersarex</t>
         </is>
       </c>
       <c r="J219" t="e">
@@ -13940,7 +13940,7 @@
       </c>
       <c r="I220" t="inlineStr">
         <is>
-          <t>imipemide,imipenem,imipenem anhydrous,imipenem hydrate,imipenem/cilastatin,imipenemum,imipenen,primaxin,recarbrio .,tienamycin</t>
+          <t>imipemide,imipenem monohydrate,imipenem/cilastatin,imipenemum,imipenen,primaxin,recarbrio .,tienam,tienamycin</t>
         </is>
       </c>
       <c r="J220" t="e">
@@ -14118,7 +14118,7 @@
       </c>
       <c r="I223" t="inlineStr">
         <is>
-          <t>isavuconazole</t>
+          <t>ravuconazole</t>
         </is>
       </c>
       <c r="J223">
@@ -14184,7 +14184,7 @@
       </c>
       <c r="I224" t="inlineStr">
         <is>
-          <t>isepacin,isepalline,isepamicin,isepamicina,isepamicine,isepamicinsulphate,isepamicinum</t>
+          <t>isepacin,isepalline,isepamicina,isepamicine,isepamicinsulphate,isepamicinum</t>
         </is>
       </c>
       <c r="J224" t="e">
@@ -14248,7 +14248,7 @@
       </c>
       <c r="I225" t="inlineStr">
         <is>
-          <t>isoconazol,isoconazole,isoconazolum,travogen</t>
+          <t>bromazil,chloramizol,clinafarm,deccosil,deccozil,enilconazol,enilconazole,eniloconazol,fecundal,flo pro imz,flopro imz,florasan,freshgard,freshguard,fungaflor,fungazil,imaverol,imaversol,imazalil,imidazole,isoconazol,isoconazolum,magnate,nuzone,rappor plus,travogen</t>
         </is>
       </c>
       <c r="J225" t="e">
@@ -14310,7 +14310,7 @@
       </c>
       <c r="I226" t="inlineStr">
         <is>
-          <t>abdizide,andrazide,anidrasona,antimicina,antituberkulosum,armacide,armazid,armazide,atcotibine,azt + isoniazid,azuren,bacillin,cemidon,chemiazid,chemidon,continazine,cortinazine,cotinazin,cotinizin,defonin,dianicotyl,dibutin,diforin,dinacrin,ditubin,ebidene,eralon,ertuban,eutizon,evalon,fetefu,fimalene,hid rasonil,hidranizil,hidrasonil,hidrulta,hidrun,hycozid,hydrazid,hydrazide,hyozid,i.a.i.,idrazil,inizid,ipcazide,iscotin,isidrina,ismazide,isobicina,isocid,isocidene,isocotin,isohydrazide,isokin,isolyn,isonerit,isonex,isoniacid,isoniazid,isoniazid sa,isoniazida,isoniazide,isoniazidum,isonicazide,isonicid,isonico,isonicotan,isonicotil,isonicotinhydrazid,isonicotinohydrazide,isonide,isonidrin,isonikazid,isonilex,isonin,isonindon,isonirit,isoniton,isonizida,isonizide,isotamine,isotebe,isotebezid,isotinyl,isozid,isozide,isozyd,laniazid,laniozid,lanizid,mayambutol,mybasan,neoteben,neoxin,neumandin,niadrin,nicazide,nicetal,nicizina,niconyl,nicotibina,nicotibine,nicotisan,nicozide,nidaton,nidrazid,nikozid,niplen,nitadon,niteban,nydrazid,nyscozid,pelazid,percin,phthisen,pycazide,pyreazid,pyricidin,pyridicin,pyrizidin,raumanon,razide,retozide,rifater,rimicid,rimifon,rimiphone,rimitsid,robiselin,robisellin,roxifen,sanohidrazina,sauterazid,sauterzid,stanozide,tebecid,tebenic,tebexin,tebilon,teebaconin,tekazin,tibazide,tibemid,tibiazide,tibinide,tibison,tibivis,tibizide,tibusan,tisiodrazida,tizide,tubazid,tubazide,tubeco,tubecotubercid,tuberian,tubicon,tubilysin,tubizid,tubomel,unicocyde,unicozyde,vazadrine,vederon,zidafimia,zinadon,zonazide</t>
+          <t>abdizide,acetyl isoniazid,acetylisoniazide,andrazide,anidrasona,antimicina,antituberkulosum,armacide,armazid,armazide,atcotibine,azt + isoniazid,azuren,bacillin,cemidon,chemiazid,chemidon,continazine,cortinazine,cotinazin,cotinizin,defonin,dianicotyl,dibutin,diforin,dinacrin,ditubin,ebidene,eralon,ertuban,eutizon,evalon,fetefu,fimalene,hid rasonil,hidranizil,hidrasonil,hidrulta,hidrun,hycozid,hydrazid,hydrazide,hyozid,i.a.i.,idrazil,inizid,ipcazide,iscotin,isidrina,ismazide,isobicina,isocid,isocidene,isocotin,isohydrazide,isokin,isolyn,isonerit,isonex,isoniacid,isoniazida,isoniazide,isoniazidum,isonicazide,isonicid,isonico,isonicotan,isonicotil,isonicotinhydrazid,isonicotinohydrazide,isonide,isonidrin,isonikazid,isonilex,isonin,isonindon,isonirit,isoniton,isonizida,isonizide,isotamine,isotebe,isotebezid,isotinyl,isozid,isozide,isozyd,laniazid,laniozid,lanizid,mayambutol,mybasan,neoteben,neoxin,neumandin,niadrin,nicazide,nicetal,nicizina,niconyl,nicotibina,nicotibine,nicotisan,nicozide,nidaton,nidrazid,nikozid,niplen,nitadon,niteban,nydrazid,nyscozid,pelazid,percin,phthisen,pycazide,pyreazid,pyricidin,pyridicin,pyrizidin,raumanon,razide,retozide,rifater,rimicid,rimifon,rimiphone,rimitsid,robiselin,robisellin,roxifen,sanohidrazina,sauterazid,sauterzid,stanozide,tebecid,tebenic,tebexin,tebilon,teebaconin,tekazin,tibazide,tibemid,tibiazide,tibinide,tibison,tibivis,tibizide,tibusan,tisiodrazida,tizide,tubazid,tubazide,tubeco,tubecotubercid,tuberian,tubicon,tubilysin,tubizid,tubomel,unicocyde,unicozyde,vazadrine,vederon,zidafimia,zinadon,zonazide</t>
         </is>
       </c>
       <c r="J226">
@@ -14438,7 +14438,7 @@
       </c>
       <c r="I228" t="inlineStr">
         <is>
-          <t>intraconazole,itraconazol,itraconazole,itraconazolo,itraconazolum,itraconzaole,itrazole,itrizole,oriconazole,sporanox</t>
+          <t>candistat,canditral,fungitraxx,intraconazole,itrac,itraconazol,itraconazolo,itraconazolum,itraconzaole,itrafungol,itralek,itrazole,itrizole,lozanoc,onmel,oriconazole,orungal,sempera,spherazole,sporamelt,sporanox,sporonox,tolsura,traconal,triasporin</t>
         </is>
       </c>
       <c r="J228">
@@ -14504,7 +14504,7 @@
       </c>
       <c r="I229" t="inlineStr">
         <is>
-          <t>jomybel,josacine,josamicina,josamycin,josamycine,josamycinum</t>
+          <t>jomybel,josacine,josamicina,josamycine,josamycinum,medemycin,mydecamycin</t>
         </is>
       </c>
       <c r="J229">
@@ -14568,7 +14568,7 @@
       </c>
       <c r="I230" t="inlineStr">
         <is>
-          <t>kanamicina,kanamycin,kanamycin a,kanamycin base,kanamycin sulfate,kanamycina,kanamycine,kanamycins,kanamycinum,kantrex,kenamycin a,klebcil,liposomal kanamycin</t>
+          <t>kanamicina,kanamycin a,kanamycina,kanamycine,kanamycins,kanamycinum,kantrex,kenamycin a,klebcil,liposomal kanamycin</t>
         </is>
       </c>
       <c r="J230">
@@ -14750,7 +14750,7 @@
       </c>
       <c r="I233" t="inlineStr">
         <is>
-          <t>extina,fungarest,fungoral,ketocanazole,ketoconazol,ketoconazole,ketoconazolum,ketoderm,nizoral,xolegel</t>
+          <t>brizoral,cerasootheket,extina,fungarest,fungoral,ketaconazole,ketocanazole,ketoconazol,ketoconazole foam,ketoconazolum,ketodan,ketoderm,ketoisdin,ketomax tris flush,ketozole,kuric,levoketoconazole,nizoral,normocort,onofin k,orifungal m,panfungol,piperazine,recorlev,sebazole,suffusiontris,teryzolin,terzolin,xolegel</t>
         </is>
       </c>
       <c r="J233">
@@ -14810,7 +14810,7 @@
       </c>
       <c r="I234" t="inlineStr">
         <is>
-          <t>jomybel,josacine,josamicina,josamycin,josamycine,josamycinum</t>
+          <t>jomybel,josacine,josamicina,josamycine,josamycinum</t>
         </is>
       </c>
       <c r="J234" t="e">
@@ -14868,7 +14868,7 @@
       </c>
       <c r="I235" t="inlineStr">
         <is>
-          <t>avatec,lasalocid,lasalocid a,lasalocide,lasalocide a,lasalocido,lasalocidum</t>
+          <t>avatec,bovatec,bovatec r,lasalocid a,lasalocid a na salt,lasalocid asalt,lasalocide,lasalocide a,lasalocido,lasalocidsalt,lasalocidum</t>
         </is>
       </c>
       <c r="J235" t="e">
@@ -14930,7 +14930,7 @@
       </c>
       <c r="I236" t="inlineStr">
         <is>
-          <t>lascufloxacin</t>
+          <t>lasvic</t>
         </is>
       </c>
       <c r="J236">
@@ -14994,7 +14994,7 @@
       </c>
       <c r="I237" t="inlineStr">
         <is>
-          <t>disodium moxalactam,festamoxin,lamoxactam,latamoxef,latamoxefum,moxalactamsupplement,shiomarin</t>
+          <t>dilatamoxef,dimoxalactam,disodium moxalactam,festamoxin,lamoxactam,latamoxefum,moxalactam,moxalactam disalt,moxalactamsalt,moxalactamsupplement,moxam,shiomarin</t>
         </is>
       </c>
       <c r="J237" t="e">
@@ -15054,7 +15054,7 @@
       </c>
       <c r="I238" t="inlineStr">
         <is>
-          <t>lefamulin,xenleta</t>
+          <t>lefamulin acetate,lefamulin acetate?,lefamulinacetate,xenleta</t>
         </is>
       </c>
       <c r="J238" t="e">
@@ -15112,7 +15112,7 @@
       </c>
       <c r="I239" t="inlineStr">
         <is>
-          <t>lenampicilina,lenampicillin,lenampicillin hcl,lenampicilline,lenampicillinum</t>
+          <t>lenampicilina,lenampicilline,lenampicillinum,takacillin,valacillin,varacillin</t>
         </is>
       </c>
       <c r="J239" t="e">
@@ -15174,7 +15174,7 @@
       </c>
       <c r="I240" t="inlineStr">
         <is>
-          <t>aeroquin,anhydrous ofloxacin,cravit,cravit hydrate,cravit iv,cravit ophthalmic,elequine,floxacin,floxel,fluoroquinolone,iquix hydrate,leroxacin,lesacin,levaquin,levaquin hydrate,levo floxacin,levofiexacin,levofloxacin,levofloxacin hydrate,levofloxacine,levofloxacino,levofloxacinum,levokacin,levoxacin,mosardal,nofaxin,ofloxcacin,oftaquix,quinsair,quixin,reskuin,tavanic,unibiotic,venaxan,volequin</t>
+          <t>aeroquin,cravit,cravit ophthalmic,dextrofloxacin,dextrofloxacine,elequine,floxacin,floxel,fluoroquinolone,iquix,leroxacin,lesacin,levaquin,levo floxacin,levofiexacin,levofloxacine,levofloxacino,levofloxacinum,levokacin,levoxacin,mosardal,nofaxin,ofloxacin impurity e,ofloxcacin,oftaquix,quinsair,quixin,reskuin,tavanic,unibiotic,venaxan,volequin</t>
         </is>
       </c>
       <c r="J240">
@@ -15298,7 +15298,7 @@
       </c>
       <c r="I242" t="inlineStr">
         <is>
-          <t>levonadifloxacin</t>
+          <t/>
         </is>
       </c>
       <c r="J242" t="e">
@@ -15418,7 +15418,7 @@
       </c>
       <c r="I244" t="inlineStr">
         <is>
-          <t>bactramycin,cillimycin,frademicina,jiemycin,lincocin,lincolcina,lincolnensin,lincomicina,lincomycin,lincomycin a,lincomycine,lincomycinum,lincorex</t>
+          <t>albiotic,bactramycin,cillimycin,frademicina,jiemycin,lincocin,lincogap,lincolcina,lincolnensin,lincomicina,lincomix,lincomycin a,lincomycin soluble,lincomycine,lincomycinum,lincorex,mycivin</t>
         </is>
       </c>
       <c r="J244">
@@ -15484,7 +15484,7 @@
       </c>
       <c r="I245" t="inlineStr">
         <is>
-          <t>linezlid,linezoid,linezolid,linezolide,linezolidum,zivoxid,zyvoxa,zyvoxam,zyvoxid</t>
+          <t>linezlid,linezoid,linezolide,linezolidum,zivoxid,zyvoxa,zyvoxam,zyvoxid</t>
         </is>
       </c>
       <c r="J245">
@@ -15608,7 +15608,7 @@
       </c>
       <c r="I247" t="inlineStr">
         <is>
-          <t>lomefloxacin,lomefloxacine,lomefloxacino,lomefloxacinum,maxaquin</t>
+          <t>bareon,logiflox,lomebact,lomefloxacine,lomefloxacino,lomefloxacinum,maxaquin,maxaquine,mazaquin,okacin,okacyn,uniquin</t>
         </is>
       </c>
       <c r="J247">
@@ -15672,7 +15672,7 @@
       </c>
       <c r="I248" t="inlineStr">
         <is>
-          <t>anhydrous loracarbef,lorabid,loracabef,loracarbef,loracarbefum,lorbef,loribid</t>
+          <t>carbac,lorabid,loracabef,loracarbefum,lorafem,lorbef,loribid</t>
         </is>
       </c>
       <c r="J248">
@@ -15736,7 +15736,7 @@
       </c>
       <c r="I249" t="inlineStr">
         <is>
-          <t>biovetin,chlortetracyclin,ciclisin,ciclolysal,ciclolysine,infaciclina,limeciclina,lisinbiotic,lymecyclin,lymecycline,lymecyclinum,mucomycin,ntetracycline,tetralisal,tetralysal,vebicyclysal</t>
+          <t>biovetin,chlortetracyclin,ciclisin,ciclolysal,ciclolysine,infaciclina,limeciclina,lisinbiotic,lymecyclin,lymecyclinum,mucomycin,ntetracycline,tetralisal,tetralysal,vebicyclysal</t>
         </is>
       </c>
       <c r="J249">
@@ -15802,7 +15802,7 @@
       </c>
       <c r="I250" t="inlineStr">
         <is>
-          <t>acido mandelico,almond acid,ammonium mandelate,amygdalic acid,benzoglycolic acid,hydroxyacetic acid,kyselina mandlova,mandelic acid,paramandelic acid,phenylglycolic acid,uromaline</t>
+          <t>acido mandelico,almond acid,ammonium mandelate,amygdalate,amygdalic acid,benzoglycolic acid,hydroxyacetic acid,kyselina mandlova,methyl,methyl mandelic acid,paramandelate,paramandelic acid,phenylglycolate,phenylglycolic acid,phenylhydroxyacetate,uromaline</t>
         </is>
       </c>
       <c r="J250">
@@ -15862,7 +15862,7 @@
       </c>
       <c r="I251" t="inlineStr">
         <is>
-          <t>manogepix</t>
+          <t/>
         </is>
       </c>
       <c r="J251" t="e">
@@ -15920,7 +15920,7 @@
       </c>
       <c r="I252" t="inlineStr">
         <is>
-          <t>marbocyl,marbofloxacin,marbofloxacine,marbofloxacino,marbofloxacinum,zeniquin</t>
+          <t>marbocyl,marbofloxacine,marbofloxacino,marbofloxacinum,zeniquin</t>
         </is>
       </c>
       <c r="J252" t="e">
@@ -15982,7 +15982,7 @@
       </c>
       <c r="I253" t="inlineStr">
         <is>
-          <t>amdinocillin,coactin,hexacillin,mecilinamo,mecillinam,mecillinamum,micillinam,penicillin hx,selexidin</t>
+          <t>amdinocillin,coactin,hexacillin,mecilinamo,mecillinamum,micillinam,penicillin,selexidin</t>
         </is>
       </c>
       <c r="J253" t="e">
@@ -16104,7 +16104,7 @@
       </c>
       <c r="I255" t="inlineStr">
         <is>
-          <t>meronem,meropen,meropenem,meropenem anhydrous,meropenem hydrate,meropenem trihydrate,meropenemum,merrem,merrem i.v.,merrem iv</t>
+          <t>meronem,meropen,meropenem trihydrate,meropenemum,merrem</t>
         </is>
       </c>
       <c r="J255" t="e">
@@ -16286,7 +16286,7 @@
       </c>
       <c r="I258" t="inlineStr">
         <is>
-          <t>mesulfamide,mesulfamido,mesulfamidum</t>
+          <t>mesulfamido,mesulfamidum</t>
         </is>
       </c>
       <c r="J258" t="e">
@@ -16348,7 +16348,7 @@
       </c>
       <c r="I259" t="inlineStr">
         <is>
-          <t>bialatan,metaciclina,metacycline,metacyclinum,methacycline,methacycline base,methacyclinum,methylenecycline,physiomycine,rondomycin</t>
+          <t>abbocin,alamycin,aquacycline,bi steclin,bialatan,biosolvomycin,biotet,bisolvomycin,chrysocin,dalimycin,dalinmycin,elinton,engemycin,hydrocyclin,imperacin,intaloxin,liquachel,macodyn,mepatar,metaciclina,metacyclinum,methacycline,methacyclinum,methylenecycline,otetryn,oxacycline,oxamycen,oxatet,oxlopar,oxy,oxybiocycline,oxycycline,oxydon,oxyject,oxymykoin,oxysteclin,oxytet,oxytetracycline.hcl,oxytetral,oxytetrin,oxytracyl,oxyvet,physiomycine,rondomycin,stecsolin,terraject,terramycin,tetran hydrochloride,toxinal,unimycin,vendarcin,vibramycin</t>
         </is>
       </c>
       <c r="J259">
@@ -16412,7 +16412,7 @@
       </c>
       <c r="I260" t="inlineStr">
         <is>
-          <t>blomopen,bonopen,celinmicina,elatocilline,fedacilina kapseln,filorex,italcina kapseln,magnipen,metabacter ampullen,metambac,metampicilina,metampicillin,metampicillin sodium,metampicillina,metampicilline,metampicillinum,methampicillin,metiskia ampullen,micinovo,micinovo ampullen,pangocilin,probiotic,rastomycin k,relyothenate,ruticina,rutizina,rutizina ampullen,sedomycin,suvipen,suvipen ampullen,tampilen ampullen,teonicon trofen,viderpen,viderpin,vioplex</t>
+          <t>amcap,amcill,ampen,amperil,ampinova,blomopen,bonopen,celinmicina,cymbi,deripen,elatocilline,fedacilina kapseln,filorex,guicitrine,italcina kapseln,magnipen,metabacter ampullen,metambac,metampen,metampicilina,metampicillina,metampicilline,metampicillinsalt,metampicillinum,methampicillin,metiskia ampullen,micinovo,micinovo ampullen,ocelina,pangocilin,pen a,penbritin,principen,probiotic,rastomycin k,relyothenate,ruticina,rutizina,rutizina ampullen,sedomycin,serfabiotic,suvipen,suvipen ampullen,tampilen ampullen,teonicon trofen,trafarbiot,viderpen,viderpin,vioplex,wypicil</t>
         </is>
       </c>
       <c r="J260">
@@ -16478,7 +16478,7 @@
       </c>
       <c r="I261" t="inlineStr">
         <is>
-          <t>aceto hmt,aminoform,aminoformaldehyde,ammoform,ammonioformaldehyde,antihydral,cystamin,cystex,cystogen,duirexol,ekagom h,esametilentetramina,formamine,formin,h.m.t.,heksa k,herax uts,heterin,hexa b,hexaform,hexaloids,hexamethylamine,hexamethylenamine,hexamethyleneamine,hexamethylentetramin,hexamine,hexamine silver,hexamine superfine,hexaminum,hexasan,hexilmethylenamine,mandelamine,metenamina,metenamine,methamin,methenamin,methenamine,methenamine silver,methenaminum,metramine,naphthamine,nocceler h,preparation af,resotropin,sanceler h,sanceler ht,silver methenamine,uramin,uratrine,urisol,uritone,urodeine,urotropin,urotropine,vesaloin,vesalvine,xametrin</t>
+          <t>aceto hmt,aminoform,aminoformaldehyde,ammoform,ammonioformaldehyde,antihydral,cystamin,cystex,cystogen,duirexol,ekagom h,esametilentetramina,formamine,formin,h.m.t.,heksa k,herax uts,heterin,hexa b,hexaform,hexaloids,hexamethylamine,hexamethylenamine,hexamethyleneamine,hexamethylentetramin,hexamine,hexamine silver,hexamine superfine,hexaminum,hexasan,hexilmethylenamine,mandelamine,metenamina,metenamine,methamin,methenamin,methenamine silver,methenaminum,metramine,naphthamine,nocceler h,pellurin,preparation,resotropin,sanceler h,sanceler,silver methenamine,uramin,uratrine,urisol,uritone,urodeine,urotropin,urotropine,vesaloin,vesalvine,xametrin</t>
         </is>
       </c>
       <c r="J261">
@@ -16542,7 +16542,7 @@
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>dimocillin,metacillin,methcilline,methicillin,methicillinum,methycillin,meticilina,meticillin,meticillina,meticilline,meticillinum,staphcillin</t>
+          <t>belfacillin,celbenin,celpilline,cinopenil,dimocillin,estafcilina,flabelline,lucopenin,metacillin,methcilline,methicillin,methicillinanhydrous,methicillinhydrate,methicillinsalt,methicillinum,methycillin,meticilina,meticillina,meticilline,meticillinsalt,meticillinum,penaureus,penysol,staficyn,staphcillin,synticillin</t>
         </is>
       </c>
       <c r="J262" t="e">
@@ -16602,7 +16602,7 @@
       </c>
       <c r="I263" t="inlineStr">
         <is>
-          <t>methioprim,metioprim,metioprima,metioprime,metioprimum</t>
+          <t>methioprim,metioprima,metioprime,metioprimum</t>
         </is>
       </c>
       <c r="J263" t="e">
@@ -16660,7 +16660,7 @@
       </c>
       <c r="I264" t="inlineStr">
         <is>
-          <t>metioxate,metioxato,metioxatum</t>
+          <t>metioxato,metioxatum</t>
         </is>
       </c>
       <c r="J264" t="e">
@@ -16722,7 +16722,7 @@
       </c>
       <c r="I265" t="inlineStr">
         <is>
-          <t>acromona,anagiardil,arilin,atrivyl,danizol,deflamon,donnan,efloran,elyzol,entizol,flagemona,flagesol,flagil,flagyl,flagyl er,flagyl i.v.,flagyl i.v. rtu,flazol,flegyl,florazole,fossyol,giatricol,ginefla vir,gineflavir,helidac,mepagyl,meronidal,methronidazole,metric,metro cream,metro gel,metro i.v,metro i.v.,metro iv,metrocream,metrodzhil,metrogel,metrogyl,metrolag,metrolotion,metrolyl,metromidol,metronidaz,metronidazol,metronidazole,metronidazole usp,metronidazolo,metronidazolum,metrotop,metrozine,metryl,mexibol,mexibol 'silanes',monagyl,monasin,nidagel,nidagyl,noritate,novonidazol,nuvessa,orvagil,polibiotic,protostat,rathimed,rosased,sanatrichom,satric,takimetol,trichazol,trichex,tricho cordes,trichobrol,trichocide,trichomol,trichopal,trichopol,tricocet,tricom,tricowas b,trikacide,trikamon,trikhopol,trikojol,trikozol,trimeks,trivazol,vagilen,vagimid,vandazole,vertisal,wagitran,zadstat,zidoval</t>
+          <t>acromona,anagiardil,arilin,atrivyl,danizol,deflamon,donnan,efloran,elyzol,entizol,flagemona,flagesol,flagil,flagyl,flagyl i.v. rtu,flazol,flegyl,florazole,fossyol,giatricol,ginefla vir,gineflavir,helidac,hmmni,hydroxydimetridazole,hydroxymetronidazole,isometronidazole,izoklion,mepagyl,meronidal,methronidazole,metric,metro cream,metro gel,metro,metrocream,metrodzhil,metrogel,metrogyl,metrolag,metrolotion,metrolyl,metromidol,metronidaz,metronidazol,metronidazole usp,metronidazolo,metronidazolum,metrotop,metrozine,metryl,mexibol,mexibol 'silanes',mizonidazole,mnzoh,monagyl,monasin,nidagel,nidagyl,noritate,novonidazol,nuvessa,orvagil,polibiotic,protostat,rathimed,rosased,sanatrichom,satric,takimetol,trichazol,trichex,tricho cordes,trichobrol,trichocide,trichomol,trichopal,trichopol,tricocet,tricom,tricowas b,trikacide,trikamon,trikhopol,trikojol,trikozol,trimeks,trivazol,vagilen,vagimid,vandazole,vertisal,wagitran,zadstat,zidoval</t>
         </is>
       </c>
       <c r="J265">
@@ -16788,7 +16788,7 @@
       </c>
       <c r="I266" t="inlineStr">
         <is>
-          <t>mezlin,mezlocilina,mezlocillin,mezlocillin acid,mezlocillin sodium,mezlocilline,mezlocillinum,multocillin</t>
+          <t>baycipen,baypen,mezlin,mezlocilina,mezlocillin acid,mezlocilline,mezlocillinsalt,mezlocillinum,multocillin</t>
         </is>
       </c>
       <c r="J266" t="e">
@@ -16910,7 +16910,7 @@
       </c>
       <c r="I268" t="inlineStr">
         <is>
-          <t>micafungin,mycamine</t>
+          <t>fungard,funguard,micafungin?,micafunginsalt,mycamine</t>
         </is>
       </c>
       <c r="J268" t="e">
@@ -16974,7 +16974,7 @@
       </c>
       <c r="I269" t="inlineStr">
         <is>
-          <t>aflorix,albistat,andergin,brentan,conofite,dactarin,daktarin,daktarin iv,florid,lotrimin af,micantin,miconasil nitrate,miconazol,miconazole,miconazole base,miconazolo,miconazolum,micozole,minostate,monista,monistat,monistat iv,oravig,vusion,zimybase,zimycan</t>
+          <t>aflorix,albistat,andergin,brentan,bromazil,chloramizol,clinafarm,conofite,dactarin,daktarin,deccosil,deccozil,enilconazol,enilconazole,eniloconazol,fecundal,flo pro imz,flopro imz,florasan,florid,freshgard,freshguard,fungaflor,fungazil,imaverol,imaversol,imazalil,imidazole,lotrimin,magnate,micantin,miconasil nitrate,miconazol,miconazolo,miconazolum,micozole,minostate,monista,monistat,nuzone,oravig,rappor plus,vusion,zimybase,zimycan</t>
         </is>
       </c>
       <c r="J269">
@@ -17036,7 +17036,7 @@
       </c>
       <c r="I270" t="inlineStr">
         <is>
-          <t>gentamicin c,micromicin,micromycin,micronomicin,micronomicina,micronomicine,micronomicinum,sagamicin,santemycin</t>
+          <t>garamycin,gentamicin c,gentamicin cla,gentamycin,gentocin,liposomal gentamicin,micromicin,micromycin,micronomicina,micronomicine,micronomicinum,sagamicin,santemycin,septocin</t>
         </is>
       </c>
       <c r="J270" t="e">
@@ -17098,7 +17098,7 @@
       </c>
       <c r="I271" t="inlineStr">
         <is>
-          <t>aboren,espinomycin a,macropen,madecacine,medemycin,midecamicina,midecamycin,midecamycin a,midecamycine,midecamycinum,midecin,momicine,mydecamycin,myoxam,normicina,rubimycin,turimycin p</t>
+          <t>aboren,espinomycin a,macropen,madecacine,medemycin,midecamicina,midecamycin a,midecamycine,midecamycinum,midecin,momicine,mydecamycin,myoxam,normicina,rubimycin,turimycin p</t>
         </is>
       </c>
       <c r="J271">
@@ -17160,7 +17160,7 @@
       </c>
       <c r="I272" t="inlineStr">
         <is>
-          <t>miloxacin,miloxacine,miloxacino,miloxacinum</t>
+          <t>miloxacine,miloxacino,miloxacinum</t>
         </is>
       </c>
       <c r="J272" t="e">
@@ -17222,7 +17222,7 @@
       </c>
       <c r="I273" t="inlineStr">
         <is>
-          <t>akamin,aknemin,borymycin,dynacin,klinomycin,minociclina,minocin,minocline,minocyclin,minocycline,minocyclinum,minocyn,minoderm,minomycin,sebomin,solodyn,vectrin</t>
+          <t>acnez,akamin,aknemin,amzeeq,arestin,borymycin,dynacin,klinomycin,lederderm,minociclina,minocin,minocline,minocyclin,minocyclinum,minocyn,minoderm,minolira,minomax,minomycin,minomycin chloride,mynocine,periocline,sebomin,solodyn,vectrin,ximino,zilxi</t>
         </is>
       </c>
       <c r="J273">
@@ -17288,7 +17288,7 @@
       </c>
       <c r="I274" t="inlineStr">
         <is>
-          <t>acecamycin,macroral,midecamycin acetate,miocamen,miocamycin,miocamycine,miokamycin,myocamicin,ponsinomycin</t>
+          <t>acecamycin,macroral,medemycin,midecamycin acetate,miocamen,miocamycine,miokamycin,mydecamycin,myocamicin,ponsinomycin</t>
         </is>
       </c>
       <c r="J274">
@@ -17348,7 +17348,7 @@
       </c>
       <c r="I275" t="inlineStr">
         <is>
-          <t>monensin sodium,sodium monensin</t>
+          <t>coban,elancoban,monelan,monensic acid,monensin,monensin granulated,monensina,monensine,monensinum,romensin,rumensin</t>
         </is>
       </c>
       <c r="J275" t="e">
@@ -17410,7 +17410,7 @@
       </c>
       <c r="I276" t="inlineStr">
         <is>
-          <t>morfazinamide,morfazinammide,morfgazinamide,morinamida,morinamide,morinamide hcl,morinamidum,morphazinamid,morphazinamide,piazofolina,piazolin,piazolina</t>
+          <t>morfazinamide,morfazinammide,morfgazinamide,morinamida,morinamidum,morphazinamid,morphazinamide,piazofolina,piazolin,piazolina</t>
         </is>
       </c>
       <c r="J276" t="e">
@@ -17472,7 +17472,7 @@
       </c>
       <c r="I277" t="inlineStr">
         <is>
-          <t>actira,avelox,avelox i.v.,avelox iv,avolex,izilox,moxeza,moxifloxacin,moxifloxacine,moxivig,vigamox,zimoxin</t>
+          <t>actira,actura,avalox,avelox,avelox abc pack,avolex,balofloxacin,bilimin,izilox,moxeza,moxifloxacine,moxivig,octegra,vegamox,vigamox,zimoxin</t>
         </is>
       </c>
       <c r="J277">
@@ -17534,7 +17534,7 @@
       </c>
       <c r="I278" t="inlineStr">
         <is>
-          <t>bactoderm,bactroban,bactroban nasal,bactroban ointment,centany,mupirocin,mupirocina,mupirocine,mupirocinum,plasimine,pseudomonic acid,pseudomonic acid a,turixin</t>
+          <t>bactoderm,bactroban,bactroban nasal,bactroban ointment,centany,lithium mupirocin,mupirocin impurity a,mupirocina,mupirocine,mupirocinum,plasimine,pseudomonic acid,pseudomonic acid a,pseudomonic acid i,turixin</t>
         </is>
       </c>
       <c r="J278" t="e">
@@ -17592,7 +17592,7 @@
       </c>
       <c r="I279" t="inlineStr">
         <is>
-          <t>nacubactam</t>
+          <t>nacubactam?</t>
         </is>
       </c>
       <c r="J279" t="e">
@@ -17650,7 +17650,7 @@
       </c>
       <c r="I280" t="inlineStr">
         <is>
-          <t>acuatim,nadifloxacin,nadifloxacine,nadifloxacino,nadifloxacinum,nadixa,nadoxin</t>
+          <t>acuatim,nadifloxacine,nadifloxacino,nadifloxacinum,nadixa,nadoxin</t>
         </is>
       </c>
       <c r="J280" t="e">
@@ -17708,7 +17708,7 @@
       </c>
       <c r="I281" t="inlineStr">
         <is>
-          <t>nafcilina,nafcillin,nafcillin sodium,nafcilline,nafcillinum,nallpen,naphcillin,unipen</t>
+          <t>nafcil,nafcilina,nafcillinanhydrous,nafcilline,nafcillinhydrate,nafcillinmonohydrate,nafcillinsalt,nafcillinum,naftopen,nallpen,naphcillin,naphthicillin,unipen</t>
         </is>
       </c>
       <c r="J281" t="e">
@@ -17768,7 +17768,7 @@
       </c>
       <c r="I282" t="inlineStr">
         <is>
-          <t>nafithromycin</t>
+          <t/>
         </is>
       </c>
       <c r="J282" t="e">
@@ -17830,7 +17830,7 @@
       </c>
       <c r="I283" t="inlineStr">
         <is>
-          <t>acide nalidixico,acide nalidixique,acido nalidissico,acido nalidixico,acidum nalidixicum,betaxina,dixiben,dixinal,eucisten,eucistin,innoxalomn,innoxalon,jicsron,kusnarin,naldixic acid,nalidic acid,nalidicron,nalidixan,nalidixane,nalidixate,nalidixate sodium,nalidixic,nalidixic acid,nalidixicacid,nalidixin,nalidixinic acid,nalidixinsaure,nalitucsan,nalurin,narigix,naxuril,neggram,negram,nevigramon,nicelate,nogram,poleon,sicmylon,specifen,specifin,unaserus,uralgin,uriben,uriclar,urisal,urodixin,uroman,uroneg,uronidix,uropan,wintomylon,wintron</t>
+          <t>acide amfonelique,acide nalidixico,acide nalidixique,acido anfonelico,acido nalidissico,acido nalidixico,acidum amfonelicum,acidum nalidixicum,amfonelic acid,amfonelinsaeure,baktogram,betaxina,chemiurin,dixiben,dixilina,dixinal,eucisten,eucistin,innoxalomn,innoxalon,jicsron,kusnarin,naldixic acid,nalidic acid,nalidicron,nalidixan,nalidixane,nalidixate,nalidixateanhydrous,nalidixic,nalidixicacid,nalidixin,nalidixinic acid,nalidixinsaure,nalitucsan,nalurin,narigix,naxuril,neggram,negram,nevigramon,nicelate,nogram,poleon,sicmylon,specifen,specifin,unaserus,uralgin,uriben,uriclar,urisal,urodixin,uroman,uroneg,uronidix,uropan,wintomylon,wintron</t>
         </is>
       </c>
       <c r="J283">
@@ -17890,7 +17890,7 @@
       </c>
       <c r="I284" t="inlineStr">
         <is>
-          <t>monteban,narasin,narasin a,narasine,narasino,narasinum,narasul</t>
+          <t>monteban,narasin a,narasine,narasino,narasinum,narasul</t>
         </is>
       </c>
       <c r="J284" t="e">
@@ -17952,7 +17952,7 @@
       </c>
       <c r="I285" t="inlineStr">
         <is>
-          <t>nemonoxacin</t>
+          <t/>
         </is>
       </c>
       <c r="J285" t="e">
@@ -18014,7 +18014,7 @@
       </c>
       <c r="I286" t="inlineStr">
         <is>
-          <t>actilin,actiline,antibiotique,bycomycin,dekamycin iii,endomixin,enterfram,fradiomycin,fradiomycin b,fradiomycinum,framicetina,framidal,framycetin,framycetin sulfate,framycetine,framycetinum,framycin,framygen,francetin,fraquinol,jernadex,myacine,myacyne,mycerin,mycifradin,neobrettin,neolate,neomas,neomcin,neomicina,neomin,neomycin,neomycin b,neomycin b sulfate,neomycin solution,neomycin sulfate,neomycin sulphate,neomycinb,neomycine,neomycinum,nivemycin,pimavecort,soframycin,soframycine,tuttomycin,vonamycin,vonamycin powder v</t>
+          <t>actilin,actiline,antibiotique,bycomycin,dekamycin iii,endomixin,enterfram,fradiomycin,fradiomycin b,fradiomycinum,framicetina,framidal,framycetine,framycetinum,framycin,framygen,francetin,fraquinol,jernadex,myacine,myacyne,mycerin,mycifradin,neobrettin,neolate,neomas,neomcin,neomicina,neomin,neomycin b,neomycin solution,neomycinb,neomycine,neomycinum,nivemycin,pimavecort,soframycin,soframycine,tuttomycin,vonamycin,vonamycin powder v</t>
         </is>
       </c>
       <c r="J286">
@@ -18080,7 +18080,7 @@
       </c>
       <c r="I287" t="inlineStr">
         <is>
-          <t>netillin,netilmicin,netilmicin sulfate,netilmicina,netilmicine,netilmicinum,netilyn,netira,nettacin,vectacin</t>
+          <t>netillin,netilmicina,netilmicine,netilmicinum,netilyn,netira,nettacin,vectacin</t>
         </is>
       </c>
       <c r="J287">
@@ -18142,7 +18142,7 @@
       </c>
       <c r="I288" t="inlineStr">
         <is>
-          <t>nicarb,nicarbasin,nicarbazin,nicarbazine,nicoxin,nicrazin,nicrazine,nirazin</t>
+          <t>nicarb,nicarbasin,nicarbazine,nicoxin,nicrazin,nicrazine,nirazin</t>
         </is>
       </c>
       <c r="J288" t="e">
@@ -18200,7 +18200,7 @@
       </c>
       <c r="I289" t="inlineStr">
         <is>
-          <t>abimasten,nifuroquina,nifuroquine,nifuroquinum,quinaldofur</t>
+          <t>abimasten,nifuroquina,nifuroquinum,quinaldofur</t>
         </is>
       </c>
       <c r="J289" t="e">
@@ -18262,7 +18262,7 @@
       </c>
       <c r="I290" t="inlineStr">
         <is>
-          <t>levantin,nifurtoinol,nifurtoinolo,nifurtoinolum,urfadin,urfadine,urfadyn</t>
+          <t>levantin,nifurmazol,nifurmazole,nifurmazolo,nifurmazolum,nifurtoinolo,nifurtoinolum,urfadin,urfadine,urfadyn</t>
         </is>
       </c>
       <c r="J290">
@@ -18322,7 +18322,7 @@
       </c>
       <c r="I291" t="inlineStr">
         <is>
-          <t>adrovet,alinia,azt + nitazoxanide,colufase,cryptaz,dexidex,heliton,kidonax,nitaxozanid,nitaxozanide,nitazox,nitazoxamide,nitazoxanid,nitazoxanida,nitazoxanide,nitazoxanidum,nitrazoxanide,omniparax,pacovanton,paramix,taenitaz</t>
+          <t>adrovet,alinia,azt + nitazoxanide,colufase,cryptaz,dexidex,heliton,kidonax,nitaxozanid,nitaxozanide,nitazox,nitazoxamide,nitazoxanid,nitazoxanida,nitazoxanidum,nitrazoxanide,omniparax,pacovanton,paramix,taenitaz</t>
         </is>
       </c>
       <c r="J291">
@@ -18386,7 +18386,7 @@
       </c>
       <c r="I292" t="inlineStr">
         <is>
-          <t>alfuran,benkfuran,berkfuran,berkfurin,ceduran,chemiofuran,cistofuran,cyantin,cystit,dantafur,fua med,fuamed,furabid,furachel,furadantin,furadantin retard,furadantina mc,furadantine,furadantine mc,furadantoin,furadoin,furadoine,furadonin,furadonine,furadoninum,furadontin,furadoxyl,furalan,furaloid,furantoin,furantoina,furatoin,furedan,furina,furobactina,furodantin,furophen t,gerofuran,io&gt;&gt;uss&gt;&gt;a&lt;&lt;ixoo,ituran,ivadantin,macpac,macrobid,macrodantin,macrodantina,macrofuran,macrofurin,nierofu,nifurantin,nifuretten,nitoin,nitrex,nitrofuradantin,nitrofurantion,nitrofurantoin,nitrofurantoin macro,nitrofurantoina,nitrofurantoine,nitrofurantoinum,novofuran,orafuran,parfuran,phenurin,piyeloseptyl,siraliden,trantoin,uerineks,urantoin,urizept,urodin,urofuran,urofurin,urolisa,urolong,uvamin,welfurin,zoofurin</t>
+          <t>alfuran,benkfuran,berkfuran,berkfurin,ceduran,chemiofuran,cistofuran,cyantin,cystit,dantafur,fua med,fuamed,furabid,furachel,furadantin,furadantin retard,furadantina,furadantine,furadantoin,furadoin,furadoine,furadonin,furadonine,furadoninum,furadontin,furadoxyl,furalan,furaloid,furantoin,furantoina,furatoin,furedan,furina,furobactina,furodantin,furophen t,gerofuran,io&gt;&gt;uss&gt;&gt;a&lt;&lt;ixoo,ituran,ivadantin,macpac,macrobid,macrodantin,macrodantina,macrofuran,macrofurin,nierofu,nifuraden,nifuradene,nifuradeno,nifuradenum,nifuradine,nifurantin,nifuretten,nitoin,nitrex,nitro macro,nitrofuradantin,nitrofurantion,nitrofurantoin macro,nitrofurantoina,nitrofurantoine,nitrofurantoinum,novofuran,orafuran,oxafuradene,oxafurandene,oxifuradene,oxyfuradene,parfuran,phenurin,piyeloseptyl,renafur,siraliden,trantoin,uerineks,urantoin,urizept,urodin,urofuran,urofurin,urolisa,urolong,uvamin,welfurin,zoofurin</t>
         </is>
       </c>
       <c r="J292">
@@ -18446,7 +18446,7 @@
       </c>
       <c r="I293" t="inlineStr">
         <is>
-          <t>acutol,aldomycin,alfucin,amifur,babrocid,becafurazone,biofuracina,biofurea,chemofuran,chixin,cocafurin,coxistat,dermofural,dymazone,dynazone,eldezol,fedacin,flavazone,fracine,furacilin,furacilinum,furacillin,furacin,furacine,furacinetten,furacoccid,furacort,furacycline,furaderm,furagent,furalcyn,furaldon,furalone,furametral,furaplast,furaseptyl,furaskin,furatsilin,furaziline,furazin,furazina,furazol w,furazone,furazyme,furesol,furfurin,furosem,fuvacillin,hemofuran,ibiofural,mammex,mastofuran,monafuracin,monafuracis,monofuracin,nfz mix,nifucin,nifurid,nifuzon,nitrofural,nitrofuralum,nitrofuran,nitrofurane,nitrofurazan,nitrofurazone,nitrofurazonum,nitrofurol,nitrozone,otofural,otofuran,rivafurazon,sanfuran,vabrocid,vadrocid,yatrocin</t>
+          <t>acutol,aldomycin,alfucin,amifur,babrocid,becafurazone,biofuracina,biofurea,chemofuran,chixin,cocafurin,coxistat,dermofural,dymazone,dynazone,eldezol,fedacin,flavazone,fracine,furacilin,furacilinum,furacillin,furacin,furacine,furacinetten,furacoccid,furacort,furacycline,furaderm,furagent,furalcyn,furaldon,furalone,furametral,furaplast,furaseptyl,furaskin,furatsilin,furaziline,furazin,furazina,furazol w,furazone,furazyme,furesol,furfurin,furosem,fuvacillin,hemofuran,ibiofural,mammex,mastofuran,monafuracin,monafuracis,monofuracin,nfz mix,nifucin,nifurid,nifuzon,nitrofural,nitrofuralum,nitrofuran,nitrofurane,nitrofurazan,nitrofurazonum,nitrofurol,nitrozone,otofural,otofuran,rivafurazon,sanfuran,vabrocid,vadrocid,yatrocin</t>
         </is>
       </c>
       <c r="J293" t="e">
@@ -18508,7 +18508,7 @@
       </c>
       <c r="I294" t="inlineStr">
         <is>
-          <t>galinok,isinok,nibiol,nicene forte,nitroxlina,nitroxolin,nitroxolina,nitroxoline,nitroxolinum,notroxoline,noxibiol</t>
+          <t>galinok,hydron iii,isinok,nibiol,nicene forte,nitroxlina,nitroxolin,nitroxolina,nitroxolinum,notroxoline,noxibiol</t>
         </is>
       </c>
       <c r="J294">
@@ -18572,7 +18572,7 @@
       </c>
       <c r="I295" t="inlineStr">
         <is>
-          <t>baccidal,barazan,chibroxin,chibroxine,chibroxol,fulgram,gonorcin,lexinor,nolicin,noracin,noraxin,norflo,norfloxacin,norfloxacine,norfloxacino,norfloxacinum,norocin,noroxin,noroxine,norxacin,sebercim,uroxacin,utinor,zoroxin</t>
+          <t>baccidal,barazan,bareon,chibroxin,chibroxine,chibroxol,fulgram,gonorcin,lexinor,logiflox,lomebact,maxaquin,maxaquine,mazaquin,nolicin,noracin,noraxin,norflo,norfloxacine,norfloxacino,norfloxacinum,norocin,noroxin,noroxine,norxacin,okacin,okacyn,sebercim,uniquin,uroxacin,utinor,zoroxin</t>
         </is>
       </c>
       <c r="J295">
@@ -18756,7 +18756,7 @@
       </c>
       <c r="I298" t="inlineStr">
         <is>
-          <t>norvancomycin</t>
+          <t>aerovanc,firvanq,firvanq kit,targocid,tecoplanina,tecoplanine,tecoplaninum,teichomycin,teicoplanina,teicoplanine,teicoplaninum</t>
         </is>
       </c>
       <c r="J298" t="e">
@@ -18814,7 +18814,7 @@
       </c>
       <c r="I299" t="inlineStr">
         <is>
-          <t>albamix,albamycin,cardelmycin,cathocin,cathomycin,crystallinic acid,inamycin,novobiocin,novobiocina,novobiocine,novobiocinum,robiocina,sirbiocina,spheromycin,stilbiocina,streptonivicin</t>
+          <t>albadry,albamast suspension,albamix,albamycin,albamycin capsules,cardelmycin,cardelmycinsalt,cathocin,cathomycin,crystallinic acid,inabiocin,inamycin,novobiocina,novobiocina bomaca,novobiocine,novobiocinsalt,novobiocinum,robiocina,salt novobiocin,sirbiocina,spheromycin,stilbiocina,streptonivicin,streptonivicinsalt,vulcamycin</t>
         </is>
       </c>
       <c r="J299" t="e">
@@ -18872,7 +18872,7 @@
       </c>
       <c r="I300" t="inlineStr">
         <is>
-          <t>biofanal,candex lotion,comycin,diastatin,herniocid,moronal,myconystatin,mycostatin,mycostatin pastilles,mykinac,mykostatyna,nilstat,nistatin,nistatina,nyamyc,nyotran,nyotrantrade mark,nystaform,nystan,nystatin,nystatin a,nystatin g,nystatin hydrate,nystatin lf,nystatine,nystatinum,nystatyna,nystavescent,nystex,nystop,stamycin,terrastatin,zydin e</t>
+          <t>biofanal,candex lotion,comycin,diastatin,herniocid,moronal,myconystatin,mycostatin,mycostatin pastilles,mykinac,mykostatyna,nilstat,nistatin,nistatina,nyamyc,nyotran,nyotrantrade mark,nystaform,nystan,nystatin a,nystatin g,nystatine,nystatinum,nystatyna,nystavescent,nystex,nystop,stamycin,terrastatin,zydin e</t>
         </is>
       </c>
       <c r="J300">
@@ -18936,7 +18936,7 @@
       </c>
       <c r="I301" t="inlineStr">
         <is>
-          <t>bactocin,danoflox,dextrofloxacin,effexin,exocin,exocine,flobacin,flodemex,flotavid,flovid,floxal,floxil,floxin,floxin otic,floxstat,fugacin,inoflox,kinflocin,kinoxacin,levofloxacin hcl,liflox,loxinter,marfloxacin,medofloxine,mergexin,monoflocet,novecin,nufafloqo,occidal,ocuflox,oflocee,oflocet,oflocin,oflodal,oflodex,oflodura,ofloxacin,ofloxacin otic,ofloxacina,ofloxacine,ofloxacino,ofloxacinum,ofloxin,onexacin,operan,orocin,otonil,oxaldin,pharflox,praxin,puiritol,qinolon,quinolon,quotavil,sinflo,tabrin,taravid,tariflox,tarivid,telbit,tructum,uro tarivid,viotisone,visiren,zanocin</t>
+          <t>bactocin,danoflox,dextrofloxacin,dextrofloxacine,effexin,exocin,exocine,flobacin,flodemex,flotavid,flovid,floxal,floxil,floxin,floxstat,fugacin,inoflox,kinflocin,kinoxacin,liflox,loxinter,marfloxacin,medofloxine,mergexin,monoflocet,novecin,nufafloqo,occidal,ocuflox,oflocee,oflocet,oflocin,oflodal,oflodex,oflodura,ofloxacin impurity e,ofloxacina,ofloxacine,ofloxacino,ofloxacinum,ofloxin,onexacin,operan,orocin,otonil,oxaldin,pharflox,praxin,puiritol,qinolon,quinolon,quotavil,sinflo,tabrin,taravid,tariflox,tarivid,telbit,tructum,uro tarivid,viotisone,visiren,zanocin</t>
         </is>
       </c>
       <c r="J301">
@@ -19064,7 +19064,7 @@
       </c>
       <c r="I303" t="inlineStr">
         <is>
-          <t>amimycin,landomycin,matromycin,oleandomicina,oleandomycin,oleandomycin a,oleandomycine,oleandomycinum,romicil</t>
+          <t>amimycin,landomycin,matromycin,oleandomicina,oleandomycin a,oleandomycine,oleandomycinum,romicil</t>
         </is>
       </c>
       <c r="J303">
@@ -19124,7 +19124,7 @@
       </c>
       <c r="I304" t="inlineStr">
         <is>
-          <t>amadacycline,omadacycline</t>
+          <t>amadacycline</t>
         </is>
       </c>
       <c r="J304">
@@ -19186,7 +19186,7 @@
       </c>
       <c r="I305" t="inlineStr">
         <is>
-          <t>numoquin,optochin,optoquine</t>
+          <t>aflukin,auriquin,biquinate,chinidin,chinidine,chinimetten,chinin,chinine,chininum muriaticum,chininum purum,conchinin,conchinine,conquinine,dentojel,dihydrochinidin,dihydroquinidine,dihydroquinine,hydroconchinine,hydroconquinine,hydroquinidine,kinder quinina,kinidin,methanol,numoquin,optoquine,pitayine,qualaquin,quinact,quinaglute,quine,quinicardine,quinidex,quinidine,quiniduran,quinindine,quinine,quinine chloride,quinine muriate,quinine tannate,quinineanhydrous,quinoline alkaloid,quinora,quinsan,rezquin</t>
         </is>
       </c>
       <c r="J305" t="e">
@@ -19244,7 +19244,7 @@
       </c>
       <c r="I306" t="inlineStr">
         <is>
-          <t>orbifloxacin</t>
+          <t>bareon,logiflox,lomebact,maxaquin,maxaquine,mazaquin,okacin,okacyn,uniquin</t>
         </is>
       </c>
       <c r="J306" t="e">
@@ -19306,7 +19306,7 @@
       </c>
       <c r="I307" t="inlineStr">
         <is>
-          <t>kimyrsa,oritavancin</t>
+          <t>aerovanc,firvanq,firvanq kit,kimyrsa</t>
         </is>
       </c>
       <c r="J307" t="e">
@@ -19426,7 +19426,7 @@
       </c>
       <c r="I309" t="inlineStr">
         <is>
-          <t>madelen,ornidal,ornidazol,ornidazole,ornidazolum,tiberal</t>
+          <t>levornidazole,madelen,ornidal,ornidazol,ornidazole isomer,ornidazolum,tiberal</t>
         </is>
       </c>
       <c r="J309">
@@ -19492,7 +19492,7 @@
       </c>
       <c r="I310" t="inlineStr">
         <is>
-          <t>oteseconazole</t>
+          <t>quilseconazole,quilseconazole?</t>
         </is>
       </c>
       <c r="J310">
@@ -19556,7 +19556,7 @@
       </c>
       <c r="I311" t="inlineStr">
         <is>
-          <t>bactocill,ossacillina,oxacilina,oxacillin,oxacillin sodium,oxacilline,oxacillinum,oxazocillin,oxazocilline,prostaphlin,prostaphlyn,sodium oxacillin</t>
+          <t>bactocill,bristopen,cryptocillin,micropenin,ossacillina,oxabel,oxabelsalt,oxacilina,oxacillin spofa,oxacillinanhydrous,oxacilline,oxacillinhydrate,oxacillinmonohydrate,oxacillinum,oxazocillin,oxazocilline,penstapho,prostaphlin,prostaphlyn,resistopen,stapenor,staphcillin v</t>
         </is>
       </c>
       <c r="J311">
@@ -19622,7 +19622,7 @@
       </c>
       <c r="I312" t="inlineStr">
         <is>
-          <t>acide oxolinique,acido ossolico,acido oxolinico,acidum oxolinicum,aqualinic,cistopax,dioxacin,emyrenil,gramurin,inoxyl,nidantin,oksaren,orthurine,ossian,oxoboi,oxolinic,oxolinic acid,pietil,prodoxal,prodoxol,starner,tiurasin,ultibid,urinox,uritrate,urotrate,uroxol,utibid</t>
+          <t>acide oxolinique,acido ossolico,acido oxolinico,acidum oxolinicum,aqualinic,cistopax,dioxacin,emyrenil,gramurin,inoxyl,nidantin,oksaren,orthurine,ossian,oxoboi,oxolinic,pietil,prodoxal,prodoxol,starner,tiurasin,ultibid,urinox,uritrate,urotrate,uroxol,utibid</t>
         </is>
       </c>
       <c r="J312">
@@ -19686,7 +19686,7 @@
       </c>
       <c r="I313" t="inlineStr">
         <is>
-          <t>adamycin,berkmycen,biostat,biostat pa,bisolvomycin,dabicycline,dalimycin,embryostat,fanterrin,galsenomycin,geomycin,geotilin,hydroxytetracyclinum,imperacin,lenocycline,macocyn,medamycin,mepatar,oksisyklin,ossitetraciclina,oxacycline,oxitetraciclina,oxitetracyclin,oxitetracycline,oxitetracyclinum,oxydon,oxymycin,oxymykoin,oxypam,oxysteclin,oxyterracin,oxyterracine,oxyterracyne,oxytetracid,oxytetracyclin,oxytetracycline,oxytetracycline base,oxytetracyclinum,proteroxyna,riomitsin,ryomycin,solkaciclina,stecsolin,stevacin,tarocyn,tarosin,teravit,terrafungine,terramitsin,terramycin,terramycin im,terramycine,tetran,unimycin,ursocyclin,ursocycline,vendarcin</t>
+          <t>abbocin,achromycin,achromycin v,actisite,adamycin,ala tet,alamycin,aquacycline,artomycin,berkmycen,bi steclin,biosolvomycin,biostat,biotet,bisolvomycin,bristacycline,cefracycline tablets,chrysocin,cyclopar,dabicycline,dalimycin,dalinmycin,diacycine,dumocyclin,elinton,embryostat,engemycin,fanterrin,galsenomycin,geomycin,geotilin,hostacycline,hydrocyclin,hydroxytetracyclinum,imperacin,intaloxin,lenocycline,liquachel,macocyn,macodyn,medamycin,mepatar,mephacyclin,neocyclin b,neocycline b,oksisyklin,ossitetraciclina,otetryn,oxacycline,oxamycen,oxatet,oxitetraciclina,oxitetracyclin,oxitetracycline,oxitetracyclinum,oxlopar,oxy,oxybiocycline,oxycycline,oxydon,oxyject,oxymycin,oxymykoin,oxypam,oxysteclin,oxyterracin,oxyterracine,oxyterracyne,oxytet,oxytetracid,oxytetracyclin,oxytetracycline.hcl,oxytetracyclinum,oxytetral,oxytetrin,oxytracyl,oxyvet,paltet,partrex,piracaps,proteroxyna,qidtet,quadracycline,quatrex,remicyclin,retet,ricycline,riomitsin,ryomycin,solkaciclina,stecsolin,stevacin,stilciclina,subamycin,sumycin,supramycin,sustamycin,tarocyn,tarosin,tefilin,teline,telotrex,teravit,terrafungine,terraject,terramitsin,terramycin,terramycine,tetrabakat,tetrabid,tetrablet,tetracaps,tetracompren,tetracycline.hcl,tetrakap,tetralution,tetramavan,tetramed,tetran,tetran hydrochloride,tetrasure,tetrosol,topicycline,toxinal,triphacyclin,unicin,unimycin,ursocyclin,ursocycline,vendarcin</t>
         </is>
       </c>
       <c r="J313">
@@ -19746,7 +19746,7 @@
       </c>
       <c r="I314" t="inlineStr">
         <is>
-          <t>ozadub,ozenoxacin,ozenoxacin cream</t>
+          <t>ozadub,ozenoxacin cream</t>
         </is>
       </c>
       <c r="J314" t="e">
@@ -19804,7 +19804,7 @@
       </c>
       <c r="I315" t="inlineStr">
         <is>
-          <t>aminopar,aminosalicylic,aminosalicylic acid,aminosalyl,aminox,apacil,deapasil,entepas,ferrosan,gabbropas,granupas,helipidyl,hellipidyl,neopasalate,osacyl,pamacyl,pamisyl,paramycin,parasal,parasalicil,parasalindon,pasalon,pasara,pascorbic,pasdium,paser granules,paskalium,pasmed,pasnodia,pasolac,propasa,rezipas,teebacin</t>
+          <t>aminacyl,aminopar,aminosalicylate,aminosalicylic,aminosalicylic acid,aminosalyl,aminosalyle,aminox,apacil,deapasil,entepas,ferrosan,gabbropas,granupas,helipidyl,hellipidyl,nemasol,neopasalate,nippas,osacyl,p.a.s.,pamacyl,pamisyl,paramisan,paramycin,parasal,parasalicil,parasalindon,pasade,pasalon,pasara,pascorbic,pasdium,paser granules,paskalium,pasmed,pasnal,pasnodia,pasolac,passodico,propasa,rezipas,salvis,sodiopas,teebacin</t>
         </is>
       </c>
       <c r="J315" t="e">
@@ -19862,7 +19862,7 @@
       </c>
       <c r="I316" t="inlineStr">
         <is>
-          <t>panipenem,panipenem/betamipron,panipenemum,penipanem</t>
+          <t>panipenam,panipenem/betamipron,panipenemum,penipanem</t>
         </is>
       </c>
       <c r="J316" t="e">
@@ -19922,7 +19922,7 @@
       </c>
       <c r="I317" t="inlineStr">
         <is>
-          <t>aminosidin,aminosidine,aminosidine i,aminosidine sulfate,amminosidin,crestomycin,estomycin,gabbromicina,gabbromycin,gabromycin,humatin,humycin,hydroxymycin,hydroxymycin sulfate,monomycin,monomycin a,neomycin e,paramomycin,paramomycin sulfate,paromomicina,paromomycin,paromomycin i,paromomycine,paromomycinum,paucimycin,paucimycinum,quintomycin c</t>
+          <t>aminosidin,aminosidine,aminosidine i,amminosidin,crestomycin,estomycin,gabbromicina,gabbromycin,gabromycin,humatin,humycin,hydroxymycin,monomycin,monomycin a,neomycin e,paramomycin,paromomicina,paromomycin i,paromomycine,paromomycinum,paucimycin,paucimycinum,quintomycin c</t>
         </is>
       </c>
       <c r="J317">
@@ -19986,7 +19986,7 @@
       </c>
       <c r="I318" t="inlineStr">
         <is>
-          <t>pazufloxacin,pazufloxacine,pazufloxacino,pazufloxacinum</t>
+          <t>pazufloxacine,pazufloxacino,pazufloxacinum</t>
         </is>
       </c>
       <c r="J318" t="e">
@@ -20050,7 +20050,7 @@
       </c>
       <c r="I319" t="inlineStr">
         <is>
-          <t>abactal,labocton,pefloxacin,pefloxacine,pefloxacinium,pefloxacino,pefloxacinum,perfloxacin,silver pefloxacin</t>
+          <t>abactal,labocton,pefloxacine,pefloxacinium,pefloxacino,pefloxacinum,perfloxacin,silver pefloxacin</t>
         </is>
       </c>
       <c r="J319">
@@ -20116,7 +20116,7 @@
       </c>
       <c r="I320" t="inlineStr">
         <is>
-          <t>hydroxymethyl,penamecilina,penamecillin,penamecillina,penamecilline,penamecillinum</t>
+          <t>alphacilina,alphacillin,bacbenzylpenicillin,berocillin,centurina,devonium,diancina,hydroxymethyl,inacilin,maxifen,penamecilina,penamecillina,penamecilline,penamecillinum,pivatil,pondocil,pondocillin,pondocillina,sanguicillin</t>
         </is>
       </c>
       <c r="J320">
@@ -20296,7 +20296,7 @@
       </c>
       <c r="I323" t="inlineStr">
         <is>
-          <t>criseocil,duamine,geotricyn,hydrocycline,penetracyne,penimepiciclina,penimepicycline,penimepicyclinum</t>
+          <t>criseocil,duamine,geotricyn,hydrocycline,penetracyne,penimepiciclina,penimepicyclinum</t>
         </is>
       </c>
       <c r="J323" t="e">
@@ -20354,7 +20354,7 @@
       </c>
       <c r="I324" t="inlineStr">
         <is>
-          <t>pentisomicin,pentisomicina,pentisomicine,pentisomicinum</t>
+          <t>pentisomicina,pentisomicine,pentisomicinum</t>
         </is>
       </c>
       <c r="J324" t="e">
@@ -20412,7 +20412,7 @@
       </c>
       <c r="I325" t="inlineStr">
         <is>
-          <t>pentizidona,pentizidone,pentizidonum</t>
+          <t>pentizidona,pentizidonum</t>
         </is>
       </c>
       <c r="J325" t="e">
@@ -20470,7 +20470,7 @@
       </c>
       <c r="I326" t="inlineStr">
         <is>
-          <t>pexiganan</t>
+          <t>cytolex,mangainin</t>
         </is>
       </c>
       <c r="J326" t="e">
@@ -20532,7 +20532,7 @@
       </c>
       <c r="I327" t="inlineStr">
         <is>
-          <t>feneticilina,feneticillin,feneticillina,feneticilline,k phenethicillin,phenethicilin,phenethicillinum,pheneticillin,pheneticilline,pheneticillinum,phenoxy pc,potassium penicillin,synthepen</t>
+          <t>alfacillin,alticina,antibiocin,apsin,arcacil,arcasin,aspin,astracillin,bendralan,beromycin,brocsil,broxil,calciopen k,chemipen,cliacil,compocillin,darcil,dramcillin s,feneticilina,feneticillin,feneticillina,feneticilline,fenocin,icipen,isocillin,ispenoral,k phenethicillin,kavepenin,ledercillin,maxipen,megacillin,optipen,oracilline,oralopen,orapen,orocillin,ospeneff,pedipen,pen v,pen,penagen,penapar,pencompren,penemve,penicillin,penicillin v,penicillin vk+,peniplus,penova,pensig,penvikal,pfizerpen,phenethicilin,phenethicillinum,pheneticilline,pheneticillinum,phenoxy,potassium penicillin,primcillin,priospen,qidpen,robicillin,roscopenin,semopen,sumapen,suspen,synapen,syncillin,synerpenin,synthecillin,synthecilline,synthepen,synthepen tabl,triospen,uticillin,vamosyn,veetids,vepen</t>
         </is>
       </c>
       <c r="J327">
@@ -20596,7 +20596,7 @@
       </c>
       <c r="I328" t="inlineStr">
         <is>
-          <t>acipen v,apocillin,apopen,beromycin,calcipen,compocillin v,crystapen v,distaquaine v,eskacillian v,eskacillin v,fenacilin,fenospen,meropenin,oracillin,oratren,pc pen vk,penicillin v,penicillinv,phenocillin,phenomycilline,phenopenicillin,robicillin,rocilin,stabicillin,vebecillin,veetids,vegacillin</t>
+          <t>acipen v,alfacillin,alticina,antibiocin,apocillin,apopen,apsin,arcacil,arcasin,aspin,astracillin,bendralan,beromycin,brocsil,broxil,calciopen k,calcipen,chemipen,cliacil,compocillin v,compocillin,crystapen v,darcil,distaquaine v,dramcillin s,eskacillian v,eskacillin v,fenacilin,feneticilline,fenocin,fenospen,icipen,isocillin,ispenoral,k phenethicillin,kavepenin,ledercillin,maxipen,megacillin,meropenin,optipen,oracillin,oracilline,oralopen,orapen,oratren,orocillin,ospeneff,pc pen,pedipen,pen v,pen,penagen,penapar,pencompren,penemve,penicillin,penicillin v,penicillin vk+,penicillinv,peniplus,penova,pensig,penvikal,pfizerpen,phenocillin,phenomycilline,phenopenicillin,potassium penicillin,primcillin,priospen,qidpen,robicillin,rocilin,roscopenin,semopen,stabicillin,sumapen,suspen,synapen,syncillin,synerpenin,synthecillin,synthecilline,synthepen,synthepen tabl,triospen,uticillin,vamosyn,vebecillin,veetids,vegacillin,vepen</t>
         </is>
       </c>
       <c r="J328">
@@ -20656,7 +20656,7 @@
       </c>
       <c r="I329" t="inlineStr">
         <is>
-          <t>delvocid,delvolan,delvopos,mycophyt,myprozine,natacyn,natafucin,natamicina,natamycin,natamycine,natamycinum,pimafucin,pimaracin,pimaricin,pimaricine,pimarizin,synogil,tennecetin</t>
+          <t>delvocid,delvolan,delvopos,mycophyt,myprozine,natacyn,natafucin,natamicina,natamycin,natamycine,natamycinum,pimafucin,pimaracin,pimaricine,pimarizin,synogil,tennecetin</t>
         </is>
       </c>
       <c r="J329" t="e">
@@ -20718,7 +20718,7 @@
       </c>
       <c r="I330" t="inlineStr">
         <is>
-          <t>acide pipemidique,acido pipemidico,acidum pipemidicum,deblaston,dolcol,filtrax,pipedac,pipemid,pipemidate,pipemidic,pipemidic acid,pipemidicacid,pipram,pipurin,tractur,uromidin,urosten,uroval</t>
+          <t>acide pipemidique,acido pipemidico,acidum pipemidicum,deblaston,dolcol,filtrax,karunomazin,pipedac,pipemid,pipemidate,pipemidic,pipemidicacid,pipram,pipurin,pyrido,tractur,uromidin,urosten,uroval</t>
         </is>
       </c>
       <c r="J330">
@@ -20782,7 +20782,7 @@
       </c>
       <c r="I331" t="inlineStr">
         <is>
-          <t>isipen,pentcillin,peperacillin,peracin,piperacilina,piperacillin,piperacillin hydrate,piperacillin na,piperacillin sodium,piperacillina,piperacilline,piperacillinum,pipercillin,pipracil,pipril,tazocin</t>
+          <t>ab piperacillin,isipen,penmalin,pentcillin,peperacillin,peracin,piperacilina,piperacillina,piperacilline,piperacillinhydrate,piperacillinsalt,piperacillinum,pipercillin,pipracil,pipracil sterile,pipril,tazocin,zosyn sterile</t>
         </is>
       </c>
       <c r="J331" t="e">
@@ -20904,7 +20904,7 @@
       </c>
       <c r="I333" t="inlineStr">
         <is>
-          <t>tazocel,tazocillin,tazocin,zosyn</t>
+          <t>piptazobactam,tazobac,tazocel,tazocillin,tazocilline,tazocin,tazonam,zobactin,zosyn</t>
         </is>
       </c>
       <c r="J333" t="e">
@@ -20964,7 +20964,7 @@
       </c>
       <c r="I334" t="inlineStr">
         <is>
-          <t>piridicillin</t>
+          <t/>
         </is>
       </c>
       <c r="J334" t="e">
@@ -21022,7 +21022,7 @@
       </c>
       <c r="I335" t="inlineStr">
         <is>
-          <t>pirlimycin,pirlimycina,pirlimycine,pirlimycinum,pirsue</t>
+          <t>pirlimycina,pirlimycine,pirlimycinum,pirsue</t>
         </is>
       </c>
       <c r="J335" t="e">
@@ -21084,7 +21084,7 @@
       </c>
       <c r="I336" t="inlineStr">
         <is>
-          <t>acide piromidique,acido piromidico,acidum piromidicum,actrun c,bactramyl,enterol,gastrurol,panacid,pirodal,piromidate,piromidic acid,piromidicacid,pyrido,reelon,septural,urisept,uropir,zaomeal</t>
+          <t>acide piromidique,acido piromidico,acidum piromidicum,actrun c,bactramyl,enterol,gastrurol,panacid,pirodal,piromidate,piromidicacid,pyrido,reelon,septural,urisept,uropir,zaomeal</t>
         </is>
       </c>
       <c r="J336">
@@ -21148,7 +21148,7 @@
       </c>
       <c r="I337" t="inlineStr">
         <is>
-          <t>berocillin,pivaloylampicillin,pivampicilina,pivampicillin,pivampicilline,pivampicillinum,pondocillin</t>
+          <t>alphacilina,alphacillin,ambacamp,ambaxin,bacacil,berocillin,centurina,devonium,diancina,inacilin,maxifen,pivaloylampicillin,pivampicilina,pivampicilline,pivampicillinum,pivatil,pondocil,pondocillin,pondocillina,sanguicillin,spectrobid,velbacil</t>
         </is>
       </c>
       <c r="J337">
@@ -21212,7 +21212,7 @@
       </c>
       <c r="I338" t="inlineStr">
         <is>
-          <t>amdinocillin pivoxil,coactabs,hydroxymethyl,pivmecilinamo,pivmecillinam,pivmecillinam hcl,pivmecillinamum</t>
+          <t>amdinocillin pivoxil,coactabs,hydroxymethyl,melysin,pivmecilinamo,pivmecillinamum,pivya,selexid</t>
         </is>
       </c>
       <c r="J338">
@@ -21272,7 +21272,7 @@
       </c>
       <c r="I339" t="inlineStr">
         <is>
-          <t>plazomicin,zemdri</t>
+          <t>zemdri</t>
         </is>
       </c>
       <c r="J339" t="e">
@@ -21334,7 +21334,7 @@
       </c>
       <c r="I340" t="inlineStr">
         <is>
-          <t>polimixina b,polumyxin b,polymixin b,polymyxine b</t>
+          <t>aerosporin,polimixina b,polumyxin b,polymixin b,polymyxine b</t>
         </is>
       </c>
       <c r="J340">
@@ -21458,7 +21458,7 @@
       </c>
       <c r="I342" t="inlineStr">
         <is>
-          <t>noxafil,posaconazole,posaconazole sp,posconazole</t>
+          <t>noxafil,posconazole</t>
         </is>
       </c>
       <c r="J342">
@@ -21520,7 +21520,7 @@
       </c>
       <c r="I343" t="inlineStr">
         <is>
-          <t>pradofloxacin,pudofloxacin,veraflox</t>
+          <t>pudofloxacin,veraflox</t>
         </is>
       </c>
       <c r="J343" t="e">
@@ -21578,7 +21578,7 @@
       </c>
       <c r="I344" t="inlineStr">
         <is>
-          <t>premafloxacin,remafloxacin</t>
+          <t>lasvic,remafloxacin</t>
         </is>
       </c>
       <c r="J344" t="e">
@@ -21640,7 +21640,7 @@
       </c>
       <c r="I345" t="inlineStr">
         <is>
-          <t>oxazine,pretomanid</t>
+          <t>oxazine</t>
         </is>
       </c>
       <c r="J345">
@@ -21700,7 +21700,7 @@
       </c>
       <c r="I346" t="inlineStr">
         <is>
-          <t>primycin</t>
+          <t>chinopricin,debrycin,guanidine,primycin a</t>
         </is>
       </c>
       <c r="J346" t="e">
@@ -21762,7 +21762,7 @@
       </c>
       <c r="I347" t="inlineStr">
         <is>
-          <t>eskalin v,mikamycin,mikamycine,mikamycinum,ostreogrycinum,pristinamycine,pristinamycinum,stafac,stafytracine,staphylomycin,starfac,streptogramin,vernamycin,virgimycin,virgimycine,virginiamycin,virginiamycina,virginiamycine,virginiamycinum</t>
+          <t>eskalin,eskalin v,micamicina,mikamycin,mikamycine,mikamycinum,ostreogricina,ostreogrycin,ostreogrycine,ostreogrycinum,pristinamicina,pristinamycine,pristinamycinum,pyostacine,stafac,stafytracine,staphylomycin,stapyocine,starfac,streptogramin,vernamycin,virgimycin,virgimycine,virginiamicina,virginiamycin,virginiamycina,virginiamycinum</t>
         </is>
       </c>
       <c r="J347">
@@ -21826,7 +21826,7 @@
       </c>
       <c r="I348" t="inlineStr">
         <is>
-          <t>depocillin,duphapen,hostacillin,hydracillin,jenacillin o,nopcaine,penicillin procaine,retardillin,vetspen,vitablend</t>
+          <t>afsillin,aquacilina,aquacillin,aquasuspen,avloprocil,bactracillin g,cilicaine,crysticillin,depocillin,despacilina,distaquaine,duphapen,duracillin,hostacillin,hydracillin,jenacillin o,kabipenin,ledercillin,millicillin,mylipen,neoproc,nopcaine,novocaine penicillin,parencillin,penaquacaine g,penicillin procaine,premocillin,procaine penicillin,procanodia,prostabillin,retardillin,sharcillin,vetspen,vitablend,wycillin</t>
         </is>
       </c>
       <c r="J348" t="e">
@@ -21890,7 +21890,7 @@
       </c>
       <c r="I349" t="inlineStr">
         <is>
-          <t>propicilina,propicillin,propicilline,propicillinum</t>
+          <t>alfacillin,alticina,antibiocin,apsin,arcacil,arcasin,aspin,astracillin,bendralan,beromycin,brocsil,broxil,calciopen k,chemipen,cliacil,compocillin,darcil,dramcillin s,feneticilline,fenocin,icipen,isocillin,ispenoral,k phenethicillin,kavepenin,ledercillin,maxipen,megacillin,optipen,oracilline,oralopen,orapen,orocillin,ospeneff,pedipen,pen v,pen,penagen,penapar,pencompren,penemve,penicillin,penicillin v,penicillin vk+,peniplus,penova,pensig,penvikal,pfizerpen,potassium penicillin,primcillin,priospen,propicilina,propicilline,propicillinum,qidpen,robicillin,roscopenin,semopen,sumapen,suspen,synapen,syncillin,synerpenin,synthecillin,synthecilline,synthepen,synthepen tabl,triospen,uticillin,vamosyn,veetids,vepen</t>
         </is>
       </c>
       <c r="J349">
@@ -21950,7 +21950,7 @@
       </c>
       <c r="I350" t="inlineStr">
         <is>
-          <t>propikacin,propikacina,propikacine,propikacinum</t>
+          <t>gentamicin a,gentamycin a,propikacina,propikacine,propikacinum</t>
         </is>
       </c>
       <c r="J350" t="e">
@@ -22012,7 +22012,7 @@
       </c>
       <c r="I351" t="inlineStr">
         <is>
-          <t>ektebin,peteha,prothionamide,prothionamidum,protion,protionamid,protionamida,protionamide,protionamidum,protionizina,tebeform,trevintix,tuberex</t>
+          <t>ektebin,peteha,prothionamide,prothionamidum,protion,protionamid,protionamida,protionamidum,protionizina,tebeform,trevintix,tuberex</t>
         </is>
       </c>
       <c r="J351">
@@ -22076,7 +22076,7 @@
       </c>
       <c r="I352" t="inlineStr">
         <is>
-          <t>prulifloxacin,pruvel,pufloxacin dioxolil,quisnon</t>
+          <t>pruvel,pufloxacin dioxolil,quisnon</t>
         </is>
       </c>
       <c r="J352">
@@ -22140,7 +22140,7 @@
       </c>
       <c r="I353" t="inlineStr">
         <is>
-          <t>aldinamid,aldinamide,braccopiral,corsazinmid,dipimide,eprazin,farmizina,isopas,lynamide,novamid,p ezetamid,pezetamid,pharozinamide,piraldina,pirazimida,pirazinamid,pirazinamida,pirazinamide,prazina,pyrafat,pyramide,pyrazide,pyrazinamdie,pyrazinamid,pyrazinamide,pyrazinamidum,pyrazine carboxamide,pyrazineamide,pyrizinamide,rifafour,rozide,tebrazid,tebrazio,tisamid,unipyranamide,zinamide,zinastat</t>
+          <t>aldinamid,aldinamide,braccopiral,corsazinmid,dipimide,eprazin,farmizina,isopas,lynamide,novamid,p ezetamid,pezetamid,pharozinamide,piraldina,pirazimida,pirazinamid,pirazinamida,pirazinamide,prazina,pyrafat,pyramide,pyrazide,pyrazinamdie,pyrazinamid,pyrazinamidum,pyrazine carboxamide,pyrazineamide,pyrizinamide,rifafour,rozide,tebrazid,tebrazio,tisamid,unipyranamide,zinamide,zinastat</t>
         </is>
       </c>
       <c r="J353">
@@ -22204,7 +22204,7 @@
       </c>
       <c r="I354" t="inlineStr">
         <is>
-          <t/>
+          <t>synercid</t>
         </is>
       </c>
       <c r="J354" t="e">
@@ -22262,7 +22262,7 @@
       </c>
       <c r="I355" t="inlineStr">
         <is>
-          <t>optaflexx,paylean,ractopamina,ractopamine,ractopaminum</t>
+          <t>bufenina,buphenin,buphenine,bupheninum,luteonin,nilidrine,nylidrin,nylidrinum,optaflexx,paylean,ractopamina,ractopaminum,ritodrin,ritodrina,ritodrine,ritodrinium,utopar,yutopar</t>
         </is>
       </c>
       <c r="J355" t="e">
@@ -22320,7 +22320,7 @@
       </c>
       <c r="I356" t="inlineStr">
         <is>
-          <t>ramoplanin</t>
+          <t/>
         </is>
       </c>
       <c r="J356" t="e">
@@ -22378,7 +22378,7 @@
       </c>
       <c r="I357" t="inlineStr">
         <is>
-          <t>razupenem</t>
+          <t/>
         </is>
       </c>
       <c r="J357" t="e">
@@ -22440,7 +22440,7 @@
       </c>
       <c r="I358" t="inlineStr">
         <is>
-          <t>altabax,altargo,retapamulin</t>
+          <t>altabax,altargo</t>
         </is>
       </c>
       <c r="J358" t="e">
@@ -22560,7 +22560,7 @@
       </c>
       <c r="I360" t="inlineStr">
         <is>
-          <t>kisqali,ribociclib</t>
+          <t>kisqali</t>
         </is>
       </c>
       <c r="J360">
@@ -22624,7 +22624,7 @@
       </c>
       <c r="I361" t="inlineStr">
         <is>
-          <t>dekamycin iv,hetangmycin,ribastamin,ribostamicina,ribostamycin,ribostamycine,ribostamycinum,vistamycin,xylostatin</t>
+          <t>dekamycin,exaluren,hetangmycin,ribastamin,ribostamicina,ribostamycine,ribostamycinum,vistamycin,xylostatin</t>
         </is>
       </c>
       <c r="J361" t="e">
@@ -22684,7 +22684,7 @@
       </c>
       <c r="I362" t="inlineStr">
         <is>
-          <t>ridinilazole</t>
+          <t/>
         </is>
       </c>
       <c r="J362" t="e">
@@ -22746,7 +22746,7 @@
       </c>
       <c r="I363" t="inlineStr">
         <is>
-          <t>alfacid,ansamicin,ansamycin,ansatipin,ansatipine,assatipin,mycobutin,rifabutin,rifabutina,rifabutine,rifabutinum</t>
+          <t>alfacid,ansamicin,ansamycin,ansatipin,ansatipine,assatipin,mycobutin,rifabutina,rifabutine,rifabutinum</t>
         </is>
       </c>
       <c r="J363">
@@ -22810,7 +22810,7 @@
       </c>
       <c r="I364" t="inlineStr">
         <is>
-          <t>abrifam,archidyn,arficin,arzide,azt + rifampin,benemicin,benemycin,dipicin,doloresum,eremfat,famcin,fenampicin,rifadin,rifadin i.v,rifadin i.v.,rifadine,rifagen,rifaldazin,rifaldazine,rifaldin,rifamate,rifamicin amp,rifamor,rifampicin,rifampicin sv,rifampicina,rifampicine,rifampicinum,rifampin,rifamsolin,rifamycin amp,rifapiam,rifaprodin,rifcin,rifinah,rifobac,rifoldin,rifoldine,riforal,rimactan,rimactane,rimactazid,rimactizid,rimazid,rimycin,sinerdol,tubocin</t>
+          <t>abrifam,archidyn,arficin,arzide,azt + rifampin,benemicin,benemycin,dipicin,doloresum,eremfat,famcin,fenampicin,rifadin,rifadine,rifagen,rifaldazin,rifaldazine,rifaldin,rifamate,rifamicin amp,rifamor,rifampicina,rifampicine,rifampicinum,rifampin,rifamsolin,rifamycin amp,rifapiam,rifaprodin,rifcin,rifinah,rifobac,rifoldin,rifoldine,riforal,rimactan,rimactane,rimactazid,rimactizid,rimazid,rimycin,sinerdol,tubocin</t>
         </is>
       </c>
       <c r="J364">
@@ -22876,7 +22876,7 @@
       </c>
       <c r="I365" t="inlineStr">
         <is>
-          <t/>
+          <t>isonarif,macox plus,rifamate,rifamazid,rifamazid i,rifinah,rimactazid</t>
         </is>
       </c>
       <c r="J365" t="e">
@@ -23124,7 +23124,7 @@
       </c>
       <c r="I369" t="inlineStr">
         <is>
-          <t>aemcolo,rifacin,rifamicina,rifamicine sv,rifamycin,rifamycine,rifamycinum,rifocin,rifocyn,rifomycin,rifomycin sv,tuborin</t>
+          <t>acetic acid,aemcolo,nacimycin,nancimycin,otofa,rifacin,rifamastene,rifamicina,rifamicine,rifamycin b,rifamycin svsalt,rifamycine,rifamycinimpurity a,rifamycinum,rifamycinum natricum,rifaximin impurity b,rifocin,rifocyn,rifomycin,rifomycin b,tuborin</t>
         </is>
       </c>
       <c r="J369">
@@ -23190,7 +23190,7 @@
       </c>
       <c r="I370" t="inlineStr">
         <is>
-          <t>cyclopentyl rifampin,prifitin,priftin,rifapentin,rifapentina,rifapentine,rifapentinum</t>
+          <t>cyclopentyl rifampin,prifitin,priftin,rifapentin,rifapentina,rifapentinum</t>
         </is>
       </c>
       <c r="J370">
@@ -23254,7 +23254,7 @@
       </c>
       <c r="I371" t="inlineStr">
         <is>
-          <t>fatroximin,flonorm,lormyx,lumenax,normix,redactiv,rifacol,rifamixin,rifaxidin,rifaximin,rifaximina,rifaximine,rifaximinum,rifaxin,ritacol,spiraxin,xifaxan,xifaxsan</t>
+          <t>fatroximin,flonorm,lormyx,lumenax,normix,redactiv,rifacol,rifamixin,rifaxidin,rifaximina,rifaximine,rifaximinum,rifaxin,ritacol,spiraxin,xifaxan,xifaxsan</t>
         </is>
       </c>
       <c r="J371">
@@ -23314,7 +23314,7 @@
       </c>
       <c r="I372" t="inlineStr">
         <is>
-          <t>ritipenem</t>
+          <t>ritipenemsalt</t>
         </is>
       </c>
       <c r="J372" t="e">
@@ -23372,7 +23372,7 @@
       </c>
       <c r="I373" t="inlineStr">
         <is>
-          <t>ritipenem acoxil</t>
+          <t>penemac</t>
         </is>
       </c>
       <c r="J373" t="e">
@@ -23434,7 +23434,7 @@
       </c>
       <c r="I374" t="inlineStr">
         <is>
-          <t>propionylleucomycin,ricamycin,rokicid,rokital,rokitamicina,rokitamycin,rokitamycine,rokitamycinum</t>
+          <t>medemycin,mydecamycin,propionylleucomycin,ricamycin,rokicid,rokital,rokitamicina,rokitamycine,rokitamycinum</t>
         </is>
       </c>
       <c r="J374">
@@ -23498,7 +23498,7 @@
       </c>
       <c r="I375" t="inlineStr">
         <is>
-          <t>bristacin,kinteto,reverin,rolitetraciclina,rolitetracycline,rolitetracyclinum,solvocillin,superciclin,synotodecin,synterin,syntetrex,syntetrin,transcycline,velacicline,velacycline</t>
+          <t>bristacin,colbiocin,kinteto,pyrrocycline n,reverin,rolitetraciclina,rolitetracyclinum,solvocillin,superciclin,synotodecin,synterin,syntetrex,syntetrin,syntetrin nitrate,tetraverin,tetrex pmt,tetrim,tetriv,transcycline,velacicline,velacycline</t>
         </is>
       </c>
       <c r="J375" t="e">
@@ -23562,7 +23562,7 @@
       </c>
       <c r="I376" t="inlineStr">
         <is>
-          <t>acrosoxacin,eracine,eradacil,eradacin,eradicin,rosoxacin,rosoxacine,rosoxacino,rosoxacinum,roxadyl,winoxacin,winuron</t>
+          <t>acrosoxacin,eracine,eradacil,eradacin,eradicin,rosoxacine,rosoxacino,rosoxacinum,roxadyl,winoxacin,winuron</t>
         </is>
       </c>
       <c r="J376">
@@ -23626,7 +23626,7 @@
       </c>
       <c r="I377" t="inlineStr">
         <is>
-          <t>roxithromycin,roxithromycine,roxithromycinum,roxitromicina,rulide</t>
+          <t>roxithromycine,roxithromycinum,roxitromicina,rulide</t>
         </is>
       </c>
       <c r="J377">
@@ -23690,7 +23690,7 @@
       </c>
       <c r="I378" t="inlineStr">
         <is>
-          <t>rufloxacin,rufloxacin hcl,rufloxacine,rufloxacino,rufloxacinum</t>
+          <t>monos,rufloxacine,rufloxacino,rufloxacinum,tebraxin</t>
         </is>
       </c>
       <c r="J378">
@@ -23750,7 +23750,7 @@
       </c>
       <c r="I379" t="inlineStr">
         <is>
-          <t>coxistac,procoxacin,salinomicina,salinomycin,salinomycine,salinomycinum</t>
+          <t>coxistac,procoxacin,salinomicina,salinomycine,salinomycinum</t>
         </is>
       </c>
       <c r="J379" t="e">
@@ -23808,7 +23808,7 @@
       </c>
       <c r="I380" t="inlineStr">
         <is>
-          <t>difloxacine,difloxacino,difloxacinum,quinolone der.,saraflox,sarafloxacin,sarafloxacine,sarafloxacino,sarafloxacinum</t>
+          <t>difloxacine,difloxacino,difloxacinum,quinolone der.,sarafin,saraflox,saraflox injectable,saraflox wsp,sarafloxacine,sarafloxacino,sarafloxacinum</t>
         </is>
       </c>
       <c r="J380" t="e">
@@ -23870,7 +23870,7 @@
       </c>
       <c r="I381" t="inlineStr">
         <is>
-          <t>sarecycline,seysara</t>
+          <t>sarecycline?,seysara</t>
         </is>
       </c>
       <c r="J381">
@@ -23930,7 +23930,7 @@
       </c>
       <c r="I382" t="inlineStr">
         <is>
-          <t>sarmoxicillin</t>
+          <t>sarmoxillina,sarmoxilline,sarmoxillinum</t>
         </is>
       </c>
       <c r="J382" t="e">
@@ -23988,7 +23988,7 @@
       </c>
       <c r="I383" t="inlineStr">
         <is>
-          <t>flagentyl,secnidal,secnidazol,secnidazole,secnidazolum,secnil,sindose,solosec</t>
+          <t>flagentyl,secnidal,secnidazol,secnidazolum,secnil,sindose,solosec</t>
         </is>
       </c>
       <c r="J383">
@@ -24114,7 +24114,7 @@
       </c>
       <c r="I385" t="inlineStr">
         <is>
-          <t>rickamicin,salvamina,siseptin sulfate,sisomicin,sisomicin sulfate,sisomicina,sisomicine,sisomicinum,sisomin,sisomycin,sissomicin,sizomycin</t>
+          <t>rickamicin,salvamina,siseptin,sisomicina,sisomicine,sisomicinum,sisomin,sisomycin,sissomicin,sizomycin</t>
         </is>
       </c>
       <c r="J385" t="e">
@@ -24174,7 +24174,7 @@
       </c>
       <c r="I386" t="inlineStr">
         <is>
-          <t>gracevit,sitafloxacin,sitafloxacinisomer</t>
+          <t>clinafoxacin,gracevit,sitafloxacinisomer,spifloxacin</t>
         </is>
       </c>
       <c r="J386">
@@ -24238,7 +24238,7 @@
       </c>
       <c r="I387" t="inlineStr">
         <is>
-          <t>bactylan,decapasil,lepasen,monopas,nippas,p.a.s. sodium,pamisyl sodium,parasal sodium,pas sodium,pasade,pasnal,passodico,salvis,sanipirol,sodiopas,sodium p.a.s,sodium pas,teebacin,tubersan</t>
+          <t>aminacyl,aminosalicylate,aminosalyle,bactylan,decapasil,lepasen,monopas,nemasol,nippas,p.a.s.,pamisyl,paramisan,parasal,pas,pasade,paskalium,pasnal,passodico,salvis,sanipirol,sodiopas,p.a.s,teebacin,tubersan</t>
         </is>
       </c>
       <c r="J387">
@@ -24300,7 +24300,7 @@
       </c>
       <c r="I388" t="inlineStr">
         <is>
-          <t>solithera,solithromycin</t>
+          <t>solithera</t>
         </is>
       </c>
       <c r="J388" t="e">
@@ -24362,7 +24362,7 @@
       </c>
       <c r="I389" t="inlineStr">
         <is>
-          <t>esparfloxacino,sparfloxacin,sparfloxacine,sparfloxacinum</t>
+          <t>esparfloxacino,sparfloxacine,sparfloxacinum</t>
         </is>
       </c>
       <c r="J389">
@@ -24426,7 +24426,7 @@
       </c>
       <c r="I390" t="inlineStr">
         <is>
-          <t>actinospectacina,adspec,espectinomicina,prospec,specitinomycin,spectam,spectinomicina,spectinomycin,spectinomycin di hcl,spectinomycine,spectinomycinum,stanilo,togamycin,trobicin</t>
+          <t>actinospectacina,adspec,espectinomicina,prospec,specitinomycin,spectam,spectam scour halt,spectinomicina,spectinomycin dihcl,spectinomycine,spectinomycinum,spectogard,stanilo,togamycin,trobicin</t>
         </is>
       </c>
       <c r="J390" t="e">
@@ -24490,7 +24490,7 @@
       </c>
       <c r="I391" t="inlineStr">
         <is>
-          <t>espiramicin,provamycin,rovamycin,rovamycine,sequamycin,spiramycine,spiramycinum</t>
+          <t>espiramicin,formacidine,foromacidin,foromacidin a,provamycin,rovamicina,rovamycin,rovamycine,sequamycin,spiramycin i,spiramycine,spiramycinum</t>
         </is>
       </c>
       <c r="J391">
@@ -24680,7 +24680,7 @@
       </c>
       <c r="I394" t="inlineStr">
         <is>
-          <t>agrept,agrimycin,chemform,estreptomicina,neodiestreptopab,strepcen,streptomicina,streptomycin,streptomycin a,streptomycin spx,streptomycin sulfate,streptomycine,streptomycinum,streptomyzin,vetstrep</t>
+          <t>agrept,agrimycin,chemform,estreptomicina,hydroxystreptomycin,neodiestreptopab,reticulin,strepcen,streptomicina,streptomycin a,streptomycin b,streptomycin c,streptomycin spx,streptomycine,streptomycinum,streptomyzin,vetstrep</t>
         </is>
       </c>
       <c r="J394" t="e">
@@ -24864,7 +24864,7 @@
       </c>
       <c r="I397" t="inlineStr">
         <is>
-          <t>betamaze,sulbactam,sulbactam acid,sulbactam free acid,sulbactamum</t>
+          <t>betamaze,sulbactam acid,sulbactam free acid,sulbactamum</t>
         </is>
       </c>
       <c r="J397" t="e">
@@ -24928,7 +24928,7 @@
       </c>
       <c r="I398" t="inlineStr">
         <is>
-          <t>kedacillina,sulbenicilina,sulbenicillin,sulbenicilline,sulbenicillinum</t>
+          <t>kedacillina,penicillin sulfoxide,sulbenicilina,sulbenicilline,sulbenicillinum</t>
         </is>
       </c>
       <c r="J398" t="e">
@@ -24988,7 +24988,7 @@
       </c>
       <c r="I399" t="inlineStr">
         <is>
-          <t>sulconazol,sulconazole,sulconazolum</t>
+          <t>sulconazol,sulconazolum</t>
         </is>
       </c>
       <c r="J399" t="e">
@@ -25046,7 +25046,7 @@
       </c>
       <c r="I400" t="inlineStr">
         <is>
-          <t>cluricol,cosulid,cosumix,durasulf,nefrosul,nsulfanilamide,prinzone vet,prinzone vet.,solfaclorpiridazina,sonilyn,sulfachlorpyridazine,sulfacloropiridazina,vetisulid</t>
+          <t>cluricol,cosulid,cosumix,durasulf,nefrosul,nsulfanilamide,prinzone,solfaclorpiridazina,sonilyn,sulfacloropiridazina,vetisulid</t>
         </is>
       </c>
       <c r="J400" t="e">
@@ -25108,7 +25108,7 @@
       </c>
       <c r="I401" t="inlineStr">
         <is>
-          <t>adiazin,adiazine,cocodiazine,codiazine,cremodiazine,cremotres,debenal,deltazina,diazin,diazolone,diazovit,diazyl,eskadiazine,honey diazine,liquadiazine,microsulfon,neazine,neotrizine,nsulfanilamide,palatrize,piridisir,pirimal,pyrimal,quadetts,quadramoid,sanodiazine,sildaflo,silvadene,solfadiazina,spofadrizine,sterazine,sulfacombin,sulfadiazene,sulfadiazin,sulfadiazina,sulfadiazine,sulfadiazinum,sulfapirimidin,sulfapyrimidin,sulfapyrimidine,sulfatryl,sulfazine,sulfolex,sulfonamides duplex,sulfonsol,sulfose,sulphadiazine,sulphadiazine e,terfonyl,theradiazine,thermazene,trifonamide,triple sulfa,triple sulfas,trisem,truozine,zinc sulfadiazine</t>
+          <t>adiazin,adiazine,cocodiazine,codiazine,cremodiazine,cremotres,debenal,deltazina,dermazin,dermazine,diazin,diazolone,diazovit,diazyl,eskadiazine,flamazine,geben,honey diazine,liquadiazine,microsulfon,n salt,neazine,neotrizine,nsulfanilamide,palatrize,piridisir,pirimal,pyrimal,quadetts,quadramoid,rayasore kit,sanodiazine,silbertone,sildaflo,silvadene,silvazine,silver  sulfadiazine,silver sulfadazine,silver sulfadiazene,silver sulfadiazine,silver sulfafdiazine,silver sulphadiazine,silveramide,sliverex,solfadiazina,spofadrizine,ssd cream,sterazine,sulfacombin,sulfadiazene,sulfadiazin,sulfadiazin silber,sulfadiazina,sulfadiazine silver,sulfadiazinum,sulfapirimidin,sulfapyrimidin,sulfapyrimidine,sulfatryl,sulfazine,sulfolex,sulfonamides duplex,sulfonsol,sulfose,sulphadiazine,sulphadiazine e,terfonyl,theradiazine,thermazene,trifonamide,triple sulfa,triple sulfas,trisem,truozine,zinc sulfadiazine</t>
         </is>
       </c>
       <c r="J401">
@@ -25172,7 +25172,7 @@
       </c>
       <c r="I402" t="inlineStr">
         <is>
-          <t>cotetroxazine</t>
+          <t>berlocombin,cotetroxazine,potesept,trimerazine</t>
         </is>
       </c>
       <c r="J402" t="e">
@@ -25234,7 +25234,7 @@
       </c>
       <c r="I403" t="inlineStr">
         <is>
-          <t>antastmon,cotrimazine,diaziprim forte,ditrim,ditrivet,sultrisan,triglobe,trimin,tucoprim,uniprim</t>
+          <t>antastmon,berlocombin,cotrimazine,diaziprim forte,ditrim,ditrivet,potesept,sultrisan,triglobe,trimerazine,trimin,tucoprim,uniprim</t>
         </is>
       </c>
       <c r="J403" t="e">
@@ -25296,7 +25296,7 @@
       </c>
       <c r="I404" t="inlineStr">
         <is>
-          <t>agribon,arnosulfan,bactrovet,deposul,diasulfa,diasulfyl,dimetazina,dinosol,dorisul,lasibon,madribon,madrigid,madriqid,madroxin,madroxine,maxulvet,mecozine,memcozine,metoxidon,neostrepal,neostreptal,nsulfanilamide,omnibon,persulfen,primor,radonin,redifal,rofenaid,roscosulf,scandisil,solfadimetossina,sudine,suldixine,sulfabon,sulfadimethoxin,sulfadimethoxine,sulfadimethoxinum,sulfadimetossina,sulfadimetoxin,sulfadimetoxina,sulfadimetoxine,sulfadimoxine,sulfastop,sulfdimethoxine,sulfoplan,sulphadimethoxine,sulxin,sumbio,symbio,theracanzan,ultrasulfon</t>
+          <t>agribon,arnosulfan,bactotril,bactrovet,deposul,diasulfa,diasulfyl,dimetazina,dinosol,dorisul,lasibon,madribon,madrigid,madriqid,madroxin,madroxine,maxulvet,mecozine,memcozine,metoxidon,neostrepal,neostreptal,nsulfanilamide,nsulfanilamidesalt,nsulphanilamide,omnibon,persulfen,primor,radonin,redifal,rofenaid,roscosulf,scandisil,solfadimetossina,sudine,suldixine,sulfabon,sulfadimethoxin,sulfadimethoxinesalt,sulfadimethoxinum,sulfadimetossina,sulfadimetoxin,sulfadimetoxina,sulfadimetoxine,sulfadimoxine,sulfamoprine,sulfastop,sulfdimethoxine,sulfoplan,sulphadimethoxine,sulxin,sumbio,symbio,theracanzan,ultrasulfon</t>
         </is>
       </c>
       <c r="J404">
@@ -25360,7 +25360,7 @@
       </c>
       <c r="I405" t="inlineStr">
         <is>
-          <t>azolmetazin,benzene sulfonamide,calfspan,calfspan tablets,cremomethazine,diazil,diazilsulfadine,dimezathine,intradine,kelametazine,mermeth,metazin,neasina,neazina,nsulfanilamide,panazin,pirmazin,primazin,sa iii,solfadimidina,spanbolet,sulfadimerazine,sulfadimesin,sulfadimesine,sulfadimethyldiazine,sulfadimezin,sulfadimezine,sulfadimezinum,sulfadimidin,sulfadimidina,sulfadimidine,sulfadimidinum,sulfadine,sulfametazina,sulfametazyny,sulfamethazine,sulfamethiazine,sulfamezathine,sulfamidine,sulfasure sr bolus,sulfodimesin,sulfodimezine,sulka k boluses,sulka s boluses,sulmet,sulphadimidine,sulphamethasine,sulphamethazine,sulphamezathine,sulphamidine,sulphodimezine,superseptil,superseptyl,vertolan</t>
+          <t>azolmetazin,benzene sulfonamide,bovibol,calfspan,calfspan tablets,cremomethazine,diazil,diazilsulfadine,dimezathine,intradine,kelametazine,mermeth,metazin,neasina,neazina,nsulfanilamide,nsulfanilamidesalt,panazin,pirmazin,primazin,sa iii,solfadimidina,spanbolet,sulfadimerazine,sulfadimesin,sulfadimesine,sulfadimethyldiazine,sulfadimetine,sulfadimezin,sulfadimezine,sulfadimezinum,sulfadimidin,sulfadimidina,sulfadimidinum,sulfadine,sulfametazina,sulfametazyny,sulfamethazinesalt,sulfamethiazine,sulfamezathine,sulfamidine,sulfasure sr bolus,sulfisomidin,sulfisomidine,sulfodimesin,sulfodimezine,sulka k boluses,sulka s boluses,sulmet,sulphadimidine,sulphamethasine,sulphamethazine,sulphamezathine,sulphamidine,sulphodimezine,superseptil,superseptyl,vertolan,vesadin</t>
         </is>
       </c>
       <c r="J405">
@@ -25486,7 +25486,7 @@
       </c>
       <c r="I407" t="inlineStr">
         <is>
-          <t>accuzole,alphazole,amidoxal,astrazolo,azo gantrisin,azosulfizin,bactesulf,barazae,chemouag,cosoxazole,dorsulfan,dorsulfan warthausen,entusil,entusul,eryzole,gantrisin,gantrisine,gantrisona,gantrizin,gantrosan,isoxamin,neazolin,neoxazoi,neoxazol,novazolo,novosaxazole,nsulfanilamide,nsulphanilamide,pancid,pediazole,renosulfan,resoxol,roxosul,roxosul tablets,roxoxol,saxosozine,sodizole,solfafurazolo,soxamide,soxazole,soxisol,soxitabs,soxomide,stansin,sulbio,sulfafuraz ole,sulfafurazol,sulfafurazole,sulfafurazolum,sulfagan,sulfagen,sulfaisoxazole,sulfalar,sulfapolar,sulfasol,sulfasoxazole,sulfasoxizole,sulfazin,sulfisin,sulfisonazole,sulfisoxasole,sulfisoxazol,sulfisoxazole,sulfisoxazolum,sulfizin,sulfizol,sulfizole,sulfofurazole,sulfoxol,suloxsol,sulphafuraz,sulphafurazol,sulphafurazole,sulphafurazolum,sulphaisoxazole,sulphisoxazol,sulphisoxazole,sulphofurazole,sulsoxin,thiasin,unisulf,urisoxin,uritrisin,urogan,vagilia</t>
+          <t>accuzole,alphazole,amidoxal,astrazolo,azo gantrisin,azosulfizin,bactesulf,barazae,chemouag,cosoxazole,dorsulfan,dorsulfan warthausen,entusil,entusul,eryzole,gantrisin,gantrisine,gantrisona,gantrizin,gantrosan,isoxamin,neazolin,neoxazoi,neoxazol,novazolo,novosaxazole,nsulfanilamide,nsulfanilamidesalt,nsulphanilamide,pancid,pediazole,renosulfan,resoxol,roxosul,roxosul tablets,roxoxol,saxosozine,sodizole,solfafurazolo,soxamide,soxazole,soxisol,soxitabs,soxomide,stansin,sulbio,sulfafuraz ole,sulfafurazol,sulfafurazolum,sulfagan,sulfagen,sulfaisoxazole,sulfalar,sulfapolar,sulfasol,sulfasoxazole,sulfasoxizole,sulfazin,sulfisin,sulfisonazole,sulfisoxasole,sulfisoxazol,sulfisoxazolesalt,sulfisoxazolum,sulfizin,sulfizol,sulfizole,sulfofurazole,sulfoxol,suloxsol,sulphafuraz,sulphafurazol,sulphafurazole,sulphafurazolum,sulphaisoxazole,sulphisoxazol,sulphisoxazole,sulphofurazole,sulsoxin,thiasin,unisulf,urisoxin,uritrisin,urogan,vagilia</t>
         </is>
       </c>
       <c r="J407">
@@ -25552,7 +25552,7 @@
       </c>
       <c r="I408" t="inlineStr">
         <is>
-          <t>aristamid,aristamide,aristogyn,domain,domian,elcosin,elcosine,elkosil,elkosin,elkosine,erycon,isosulf,mefenal,nsulfanilamide,solfisomidina,sulfadimetine,sulfaisodimerazine,sulfaisodimidine,sulfaisodimidinum,sulfaisomidine,sulfamethin,sulfasomidine,sulfisomidina,sulfisomidine,sulfisomidine sodium,sulfisomidinum,sulphasomidine</t>
+          <t>aristamid,aristamid augensalbe,aristamide,aristogyn,bovibol,domain,domian,elcosin,elcosine,elkosil,elkosin,elkosine,erycon,intradine,isosulf,mefenal,nsulfanilamide,nsulfanilamidesalt,solfisomidina,sulfadimetine,sulfadimidin,sulfaisodimerazine,sulfaisodimidinum,sulfaisomidine,sulfamethazinesalt,sulfamethin,sulfasomidine,sulfisomidin,sulfisomidina,sulfisomidine,sulfisomidinum,sulphasomidine,vesadin</t>
         </is>
       </c>
       <c r="J408">
@@ -25618,7 +25618,7 @@
       </c>
       <c r="I409" t="inlineStr">
         <is>
-          <t>dalysep,kelfizin,kelfizina,kelfizine,kelfizine w,longum,nsulfanilamide,policydal,polycidal,solfametopirazina,sulfalen,sulfalene,sulfaleno,sulfalenum,sulfamethopyrazine,sulfamethoxypyrazine,sulfametopyrazine,sulfametoxypyridazin,sulphalene,sulphametopyrazine,vetkelfizina</t>
+          <t>dalysep,kelfizin,kelfizina,kelfizine,kelfizine w,longum,nsulfanilamide,policydal,polycidal,solfametopirazina,sulfalen,sulfaleno,sulfalenum,sulfamethopyrazine,sulfamethoxypyrazine,sulfametopyrazine,sulfametoxypyridazin,sulphalene,sulphametopyrazine,vetkelfizina</t>
         </is>
       </c>
       <c r="J409">
@@ -25682,7 +25682,7 @@
       </c>
       <c r="I410" t="inlineStr">
         <is>
-          <t>sulfamazon,sulfamazona,sulfamazone,sulfamazonum</t>
+          <t>marespin,sulfamazon,sulfamazona,sulfamazonum</t>
         </is>
       </c>
       <c r="J410">
@@ -25746,7 +25746,7 @@
       </c>
       <c r="I411" t="inlineStr">
         <is>
-          <t>cremomerazine,kelamerazine,mebacid,mesulfa,methylpyrimal,methylsulfazin,methylsulfazine,metilsulfadiazin,metilsulfazin,nsulfanilamide,percoccide,pyralcid,pyrimal m,romezin,septacil,septosyl,solfamerazina,solumedin,solumedine,sulfameradine,sulfamerazin,sulfamerazina,sulfamerazine,sulfamerazinum,sulfamethyldiazine,sulphamerazine,sumedine,susfamerazine</t>
+          <t>cremomerazine,dermazin,dermazine,flamazine,geben,kelamerazine,mebacid,mesulfa,methylpyrimal,methylsulfazin,methylsulfazine,metilsulfadiazin,metilsulfazin,n salt,nsulfanilamide,percoccide,pyralcid,pyrimal m,rayasore kit,romezin,septacil,septosyl,silbertone,sildaflo,silvadene,silvazine,silver  sulfadiazine,silver sulfadazine,silver sulfadiazene,silver sulfadiazine,silver sulfafdiazine,silver sulphadiazine,silveramide,sliverex,solfamerazina,solumedin,solumedine,ssd cream,sulfadiazin silber,sulfadiazine silver,sulfameradine,sulfamerazin,sulfamerazina,sulfamerazinum,sulfamethyldiazine,sulphamerazine,sumedine,susfamerazine,thermazene</t>
         </is>
       </c>
       <c r="J411">
@@ -25868,7 +25868,7 @@
       </c>
       <c r="I413" t="inlineStr">
         <is>
-          <t>azolmetazin,benzene sulfonamide,calfspan,calfspan tablets,cremomethazine,diazil,diazilsulfadine,dimezathine,intradine,kelametazine,mermeth,metazin,neasina,neazina,nsulfanilamide,panazin,pirmazin,primazin,sa iii,solfadimidina,spanbolet,sulfadimerazine,sulfadimesin,sulfadimesine,sulfadimethyldiazine,sulfadimezin,sulfadimezine,sulfadimezinum,sulfadimidin,sulfadimidina,sulfadimidine,sulfadimidinum,sulfadine,sulfametazina,sulfametazyny,sulfamethazine,sulfamethiazine,sulfamezathine,sulfamidine,sulfasure sr bolus,sulfodimesin,sulfodimezine,sulka k boluses,sulka s boluses,sulmet,sulphadimidine,sulphamethasine,sulphamethazine,sulphamezathine,sulphamidine,sulphodimezine,superseptil,superseptyl,vertolan</t>
+          <t>azolmetazin,benzene sulfonamide,bovibol,calfspan,calfspan tablets,cremomethazine,diazil,diazilsulfadine,dimezathine,intradine,kelametazine,mermeth,metazin,neasina,neazina,nsulfanilamide,nsulfanilamidesalt,panazin,pirmazin,primazin,sa iii,solfadimidina,spanbolet,sulfadimerazine,sulfadimesin,sulfadimesine,sulfadimethyldiazine,sulfadimetine,sulfadimezin,sulfadimezine,sulfadimezinum,sulfadimidin,sulfadimidina,sulfadimidinum,sulfadine,sulfametazina,sulfametazyny,sulfamethazinesalt,sulfamethiazine,sulfamezathine,sulfamidine,sulfasure sr bolus,sulfisomidin,sulfisomidine,sulfodimesin,sulfodimezine,sulka k boluses,sulka s boluses,sulmet,sulphadimidine,sulphamethasine,sulphamethazine,sulphamezathine,sulphamidine,sulphodimezine,superseptil,superseptyl,vertolan,vesadin</t>
         </is>
       </c>
       <c r="J413" t="e">
@@ -25930,7 +25930,7 @@
       </c>
       <c r="I414" t="inlineStr">
         <is>
-          <t>ayerlucil,lucosil,methazol,microsul,nsulfanilamide,proklar,renasul,salimol,solfametizolo,sulamethizole,sulfa gram,sulfamethizol,sulfamethizole,sulfamethizolum,sulfametizol,sulfapyelon,sulfstat,sulfurine,sulphamethizole,tetracid,thidicur,thiosulfil,thiosulfil forte,ultrasul,urocydal,urodiaton,urolucosil,urosulfin</t>
+          <t>aethazol,aethazolum,ayerlucil,berlophen,etazol,etazole,ethazole,gliprotiazol,globucid,globucin,globuzid,glyprothiazol,glyprothiazole,glyprothiazolum,glyprothizol,glyprothizolum,lucosil,methazol,microsul,nsulfanilamide,pasit,proklar,renasul,salimol,sethadil,solfametizolo,solfetidolo,sulamethizole,sulfa gram,sulfaethidiole,sulfaethidol,sulfaethidole,sulfaethidolum,sulfaetidol,sulfamethizol,sulfamethizolum,sulfametizol,sulfapyelon,sulfstat,sulfurine,sulphaethidole,sulphamethizole,tardipyrine,tetracid,thidicur,thiosulfil,thiosulfil forte,ultrasul,urocydal,urodiaton,urolucosil,urosulfin</t>
         </is>
       </c>
       <c r="J414">
@@ -25994,7 +25994,7 @@
       </c>
       <c r="I415" t="inlineStr">
         <is>
-          <t>azo gantanol,gamazole,gantanol,gantanol ds,metoxal,nsulfanilamide,nsulphanilamide,radonil,septran,simsinomin,sinomin,solfametossazolo,sulfamethalazole,sulfamethoxazol,sulfamethoxazole,sulfamethoxazolum,sulfamethoxizole,sulfamethylisoxazole,sulfametoxazol,sulfisomezole,sulmeprim,sulphamethalazole,sulphamethoxazol,sulphamethoxazole,sulphisomezole,urobak</t>
+          <t>azo gantanol,gamazole,gantanol,metoxal,nsulfanilamide,nsulphanilamide,radonil,septran,simsinomin,sinomin,solfametossazolo,sulfamethalazole,sulfamethoxazol,sulfamethoxazolum,sulfamethoxizole,sulfamethylisoxazole,sulfametoxazol,sulfiodizole,sulfisomezole,sulmeprim,sulphamethalazole,sulphamethoxazol,sulphamethoxazole,sulphisomezole,urobak</t>
         </is>
       </c>
       <c r="J415">
@@ -26058,7 +26058,7 @@
       </c>
       <c r="I416" t="inlineStr">
         <is>
-          <t>altezol,davosin,depovernil,kineks,lederkyn,lentac,lisulfen,longin,medicel,midicel,midikel,myasul,nsulfanilamide,opinsul,paramid,paramid supra,petrisul,piridolo,quinoseptyl,retamid,retasulfin,retasulphine,slosul,spofadazine,sulfalex,sulfapyridazine,sulfdurazin,sulfozona,sultirene,vinces</t>
+          <t>altezol,cysul,davosin,depovernil,kineks,lederkyn,lentac,lisulfen,longin,medicel,midicel,midikel,myasul,nsulfanilamide,nsulphanilamide,opinsul,paramid,paramid supra,petrisul,piridolo,quinoseptyl,retamid,retasulfin,retasulphine,slosul,spofadazine,sulfalex,sulfapiridazin,sulfapyridazine,sulfdurazin,sulfozona,sultirene,vinces</t>
         </is>
       </c>
       <c r="J416">
@@ -26122,7 +26122,7 @@
       </c>
       <c r="I417" t="inlineStr">
         <is>
-          <t>duroprocin,methofadin,methofazine,nsulfanilamide,solfametomidina,sulfamethomidine,sulfametomidin,sulfametomidina,sulfametomidine,sulfametomidinum</t>
+          <t>bactotril,duroprocin,methofadin,methofazine,nsulfanilamide,nsulfanilamidesalt,solfametomidina,sulfadimethoxinesalt,sulfamethomidine,sulfametomidin,sulfametomidina,sulfametomidinum,sulphadimethoxine</t>
         </is>
       </c>
       <c r="J417" t="e">
@@ -26184,7 +26184,7 @@
       </c>
       <c r="I418" t="inlineStr">
         <is>
-          <t>bayrena,berlicid,dairena,durenat,juvoxin,kinecid,kirocid,longasulf,methoxypyrimal,nsulfanilamide,solfametossidiazina,sulfameter,sulfamethorine,sulfamethoxine,sulfamethoxydiazin,sulfamethoxydiazine,sulfamethoxydin,sulfamethoxydine,sulfametin,sulfametinum,sulfametorin,sulfametorine,sulfametorinum,sulfametoxidiazina,sulfametoxidine,sulfametoxydiazine,sulfametoxydiazinum,sulphameter,sulphamethoxydiazine,supramid,ultrax</t>
+          <t>bayrena,berlicid,dairena,durenat,juvoxin,kinecid,kirocid,longasulf,methoxypyrimal,nsulfanilamide,solfametossidiazina,sulfameter,sulfametersalt,sulfamethorine,sulfamethoxine,sulfamethoxydiazin,sulfamethoxydiazine,sulfamethoxydin,sulfamethoxydine,sulfametin,sulfametinum,sulfametorin,sulfametorine,sulfametorinum,sulfametoxidiazina,sulfametoxidine,sulfametoxydiazinum,sulphameter,sulphamethoxydiazine,supramid,ultrax</t>
         </is>
       </c>
       <c r="J418">
@@ -26310,7 +26310,7 @@
       </c>
       <c r="I420" t="inlineStr">
         <is>
-          <t>justamil,nsulfanilamide,oxasulfa,solfamossolo,sulfadimethyloxazole,sulfamoxol,sulfamoxole,sulfamoxolum,sulfano,sulfavigor,sulfmidil,sulfono,sulfune,sulfuno,sulphamoxole,tardamid,tardamide</t>
+          <t>enterocura,justamil,nsulfanilamide,oxasulfa,solfaguanolo,solfamossolo,sulfadimethyloxazole,sulfaguanol,sulfaguanole,sulfaguanolum,sulfamoxol,sulfamoxolum,sulfano,sulfavigor,sulfmidil,sulfono,sulfune,sulfuno,sulphamoxole,tardamid,tardamide</t>
         </is>
       </c>
       <c r="J420">
@@ -26438,7 +26438,7 @@
       </c>
       <c r="I422" t="inlineStr">
         <is>
-          <t>albexan,albosal,ambeside,antistrept,astreptine,astrocid,bacteramid,bactesid,collomide,colsulanyde,copticide,deseptyl,desseptyl,dipron,ergaseptine,erysipan,estreptocida,exoseptoplix,gerison,gombardol,infepan,lysococcine,neococcyl,orgaseptine,prontalbin,prontosil album,prontosil i,prontosil white,prontylin,pronzin album,proseptal,proseptine,proseptol,pysococcine,rubiazol a,sanamid,septamide album,septanilam,septinal,septolix,septoplex,septoplix,solfanilamide,stopton album,stramid,strepamide,strepsan,streptagol,streptamid,streptamin,streptasol,streptocid,streptocid album,streptocide,streptocide white,streptocidum,streptoclase,streptocom,streptol,strepton,streptopan,streptosil,streptozol,streptozone,streptrocide,sulfamidyl,sulfamine,sulfana,sulfanalone,sulfanidyl,sulfanil,sulfanilamida,sulfanilamide,sulfanilamidum,sulfanilimidic acid,sulfanimide,sulfocidin,sulfocidine,sulfonamide,sulfonamide p,sulfonylamide,sulphanilamide,sulphanilamide gr,sulphanilamidum,sulphonamide,therapol,tolder,white streptocide</t>
+          <t>albexan,albosal,ambeside,antistrept,astreptine,astrocid,bacteramid,bactesid,collomide,colsulanyde,copticide,deseptyl,desseptyl,dipron,ergaseptine,erysipan,estreptocida,exoseptoplix,gerison,gombardol,infepan,lysococcine,neococcyl,orgaseptine,prontalbin,prontosil album,prontosil i,prontosil white,prontylin,pronzin album,proseptal,proseptine,proseptol,pysococcine,rubiazol a,sanamid,septamide album,septanilam,septinal,septolix,septoplex,septoplix,solfanilamide,stopton album,stramid,strepamide,strepsan,streptagol,streptamid,streptamin,streptasol,streptocid,streptocid album,streptocide,streptocide white,streptocidum,streptoclase,streptocom,streptol,strepton,streptopan,streptosil,streptozol,streptozone,streptrocide,sulfamidyl,sulfamine,sulfana,sulfanalone,sulfanidyl,sulfanil,sulfanilamid,sulfanilamida,sulfanilamidomethan,sulfanilamidum,sulfanilimidic acid,sulfanimide,sulfocidin,sulfocidine,sulfonamide p,sulfonylamide,sulphanilamide,sulphanilamidum,sulphonamide,therapol,tolder,white streptocide</t>
         </is>
       </c>
       <c r="J422" t="e">
@@ -26500,7 +26500,7 @@
       </c>
       <c r="I423" t="inlineStr">
         <is>
-          <t>anastaf,archisulfa,avissul,chemiopen,demosulfan,durisan saft,ipersulfidin sirup,isosulfamerazine,methylsulfadiazin,methylsulfadiazine,novosul,nsulfanilamide,orosulfan,pallidin,retardon,risulfasens,sulfaperin,sulfaperina,sulfaperine,sulfaperinum,sulfatreis,sulfopirimidine,sulpenta,ultrasulfon sirup</t>
+          <t>anastaf,archisulfa,avissul,chemiopen,demosulfan,durisan saft,ipersulfidin sirup,isosulfamerazine,methylsulfadiazin,methylsulfadiazine,novosul,nsulfanilamide,orosulfan,pallidin,retardon,risulfasens,sulfaperina,sulfaperine,sulfaperinum,sulfatreis,sulfopirimidine,sulpenta,ultrasulfon sirup</t>
         </is>
       </c>
       <c r="J423">
@@ -26564,7 +26564,7 @@
       </c>
       <c r="I424" t="inlineStr">
         <is>
-          <t>depocid,depotsulfonamide,eftolon,firmazolo,inamil,isarol,isarol v,merian,microtan pirazolo,nsulfanilamide,orisul,orisulf,paidazolo,phenylsulfapyrazole,plisulfan,raziosulfa,solfafenazolo,sulfabid,sulfafenazol,sulfafenazolo,sulfaphenazol,sulfaphenazole,sulfaphenazolum,sulfaphenazon,sulfaphenylpipazol,sulfaphenylpyrazol,sulfaphenylpyrazole,sulfonylpyrazol,sulphaphenazole,sulphenazole</t>
+          <t>depocid,depotsulfonamide,eftolon,firmazolo,inamil,isarol,isarol v,merian,microtan pirazolo,nsulfanilamide,orisul,orisulf,paidazolo,phenylsulfapyrazole,plisulfan,raziosulfa,solfafenazolo,sulfabid,sulfafenazol,sulfafenazolo,sulfaphenazol,sulfaphenazolum,sulfaphenazon,sulfaphenylpipazol,sulfaphenylpyrazol,sulfaphenylpyrazole,sulfonylpyrazol,sulphaphenazole,sulphenazole</t>
         </is>
       </c>
       <c r="J424">
@@ -26628,7 +26628,7 @@
       </c>
       <c r="I425" t="inlineStr">
         <is>
-          <t>adiplon,coccoclase,dagenan,eubasin,eubasinum,haptocil,piridazol,plurazol,pyriamid,pyridazol,relbapiridina,septipulmon,solfapiridina,streptosilpyridine,sulfapiridina,sulfapyridin,sulfapyridine,sulfapyridinum,sulfidin,sulfidine,sulphapyridin,sulphapyridine,thioseptal,trianon</t>
+          <t>adiplon,coccoclase,dagenan,eubasin,eubasinum,haptocil,piridazol,plurazol,pyriamid,pyridazol,relbapiridina,septipulmon,solfapiridina,soludagenan,streptosilpyridine,sulfapiridina,sulfapyridin,sulfapyridinum,sulfidin,sulfidine,sulphapyridin,sulphapyridine,thioseptal,trianon</t>
         </is>
       </c>
       <c r="J425">
@@ -26688,7 +26688,7 @@
       </c>
       <c r="I426" t="inlineStr">
         <is>
-          <t>ambesid,derganil,sulfasuccinamid,sulfasuccinamida,sulfasuccinamide,sulfasuccinamidum</t>
+          <t>ambesid,derganil,sulfasuccinamid,sulfasuccinamida,sulfasuccinamidum</t>
         </is>
       </c>
       <c r="J426" t="e">
@@ -26750,7 +26750,7 @@
       </c>
       <c r="I427" t="inlineStr">
         <is>
-          <t>azoquimiol,azoseptale,cerazol,cerazole,chemosept,cibazol,duatok,dulana,eleudron,enterobiocine,estafilol,formosulfathiazole,neostrepsan,norsulfasol,norsulfazol,norsulfazole,norsulfazolum,nsulfanilamide,planomide,poliseptil,sanotiazol,septozol,sodium sulfathiazole,solfatiazolo,streptosilthiazole,sulfamul,sulfathiazol,sulfathiazole,sulfathiazolum,sulfatiazol,sulfavitina,sulfocerol,sulphathiazole,sulzol,thiacoccine,thiasulfol,thiazamide,thiozamide,triple sulfa,wintrazole</t>
+          <t>azoquimiol,azoseptale,cerazol,cerazole,chemosept,cibazol,duatok,dulana,eleudron,enterobiocine,estafilol,formosulfathiazole,neostrepsan,norsulfasol,norsulfazol,norsulfazole,norsulfazolum,nsulfanilamide,planomide,poliseptil,sanotiazol,septozol,silver sulfathiazole,solfatiazolo,soluthiazomide,streptosilthiazole,sulfamul,sulfathiazol,sulfathiazole silver,sulfathiazolesalt,sulfathiazolum,sulfatiazol,sulfavitina,sulfocerol,sulphathiazole,sulzol,thiacoccine,thiasulfol,thiazamide,thiozamide,triple sulfa,wintrazole</t>
         </is>
       </c>
       <c r="J427" t="e">
@@ -26812,7 +26812,7 @@
       </c>
       <c r="I428" t="inlineStr">
         <is>
-          <t>badional,baldinol,fontamide,salvoseptyl,solfatiourea,solufontamide,sulfanilthiourea,sulfathiocarbamid,sulfathiocarbamide,sulfathiocarbamidum,sulfathiourea,sulfathiouree,sulfatiourea,sulphathiourea</t>
+          <t>badional,baldinol,fontamide,salvoseptyl,solfatiourea,solufontamide,sulfanilthiourea,sulfathiocarbamid,sulfathiocarbamide,sulfathiocarbamidum,sulfathioureasalt,sulfathiouree,sulfatiourea,sulphathiourea</t>
         </is>
       </c>
       <c r="J428">
@@ -26872,7 +26872,7 @@
       </c>
       <c r="I429" t="inlineStr">
         <is>
-          <t>accuzole,alphazole,amidoxal,astrazolo,azo gantrisin,azosulfizin,bactesulf,barazae,chemouag,cosoxazole,dorsulfan,dorsulfan warthausen,entusil,entusul,eryzole,gantrisin,gantrisine,gantrisona,gantrizin,gantrosan,isoxamin,neazolin,neoxazoi,neoxazol,novazolo,novosaxazole,nsulfanilamide,nsulphanilamide,pancid,pediazole,renosulfan,resoxol,roxosul,roxosul tablets,roxoxol,saxosozine,sodizole,solfafurazolo,soxamide,soxazole,soxisol,soxitabs,soxomide,stansin,sulbio,sulfafuraz ole,sulfafurazol,sulfafurazole,sulfafurazolum,sulfagan,sulfagen,sulfaisoxazole,sulfalar,sulfapolar,sulfasol,sulfasoxazole,sulfasoxizole,sulfazin,sulfisin,sulfisonazole,sulfisoxasole,sulfisoxazol,sulfisoxazole,sulfisoxazolum,sulfizin,sulfizol,sulfizole,sulfofurazole,sulfoxol,suloxsol,sulphafuraz,sulphafurazol,sulphafurazole,sulphafurazolum,sulphaisoxazole,sulphisoxazol,sulphisoxazole,sulphofurazole,sulsoxin,thiasin,unisulf,urisoxin,uritrisin,urogan,vagilia</t>
+          <t>accuzole,alphazole,amidoxal,astrazolo,azo gantrisin,azosulfizin,bactesulf,barazae,chemouag,cosoxazole,dorsulfan,dorsulfan warthausen,entusil,entusul,eryzole,gantrisin,gantrisine,gantrisona,gantrizin,gantrosan,isoxamin,neazolin,neoxazoi,neoxazol,novazolo,novosaxazole,nsulfanilamide,nsulfanilamidesalt,nsulphanilamide,pancid,pediazole,renosulfan,resoxol,roxosul,roxosul tablets,roxoxol,saxosozine,sodizole,solfafurazolo,soxamide,soxazole,soxisol,soxitabs,soxomide,stansin,sulbio,sulfafuraz ole,sulfafurazol,sulfafurazolum,sulfagan,sulfagen,sulfaisoxazole,sulfalar,sulfapolar,sulfasol,sulfasoxazole,sulfasoxizole,sulfazin,sulfisin,sulfisonazole,sulfisoxasole,sulfisoxazol,sulfisoxazolesalt,sulfisoxazolum,sulfizin,sulfizol,sulfizole,sulfofurazole,sulfoxol,suloxsol,sulphafuraz,sulphafurazol,sulphafurazole,sulphafurazolum,sulphaisoxazole,sulphisoxazol,sulphisoxazole,sulphofurazole,sulsoxin,thiasin,unisulf,urisoxin,uritrisin,urogan,vagilia</t>
         </is>
       </c>
       <c r="J429" t="e">
@@ -26988,7 +26988,7 @@
       </c>
       <c r="I431" t="inlineStr">
         <is>
-          <t>sulopenem</t>
+          <t/>
         </is>
       </c>
       <c r="J431" t="e">
@@ -27050,7 +27050,7 @@
       </c>
       <c r="I432" t="inlineStr">
         <is>
-          <t>sultamicilina,sultamicillin,sultamicillinum</t>
+          <t>sultamicilina,sultamicillinum</t>
         </is>
       </c>
       <c r="J432">
@@ -27110,7 +27110,7 @@
       </c>
       <c r="I433" t="inlineStr">
         <is>
-          <t>surotomycin</t>
+          <t>cidecin,cubicin,dapcin,daptomicina,daptomycin for,daptomycine,daptomycinum,dapzura,deptomycin</t>
         </is>
       </c>
       <c r="J433" t="e">
@@ -27172,7 +27172,7 @@
       </c>
       <c r="I434" t="inlineStr">
         <is>
-          <t>talampicilina,talampicillin,talampicilline,talampicillinum</t>
+          <t>aseocillin,talampicilina,talampicilline,talampicillinum,talpen,tamampicillin,yamacillin</t>
         </is>
       </c>
       <c r="J434">
@@ -27232,7 +27232,7 @@
       </c>
       <c r="I435" t="inlineStr">
         <is>
-          <t>talmetoprim</t>
+          <t/>
         </is>
       </c>
       <c r="J435" t="e">
@@ -27294,7 +27294,7 @@
       </c>
       <c r="I436" t="inlineStr">
         <is>
-          <t>tazobactam,tazobactam acid,tazobactamum,tazobactum</t>
+          <t>enmetazobactam,tazobactam acid,tazobactamsalt,tazobactamum,tazobactum</t>
         </is>
       </c>
       <c r="J436" t="e">
@@ -27416,7 +27416,7 @@
       </c>
       <c r="I438" t="inlineStr">
         <is>
-          <t>sivextro,tedizolid,torezolid</t>
+          <t>sivextro,torezolid</t>
         </is>
       </c>
       <c r="J438">
@@ -27482,7 +27482,7 @@
       </c>
       <c r="I439" t="inlineStr">
         <is>
-          <t>targocid,tecoplanina,tecoplanine,tecoplaninum,teichomycin,teicoplanin,teicoplanina,teicoplanine,teicoplaninum</t>
+          <t>aerovanc,firvanq,firvanq kit,targocid,tecoplanina,tecoplanine,tecoplaninum,teichomycin,teicoplanina,teicoplanine,teicoplaninum</t>
         </is>
       </c>
       <c r="J439" t="e">
@@ -27604,7 +27604,7 @@
       </c>
       <c r="I441" t="inlineStr">
         <is>
-          <t>telavancin,televancin,vibativ</t>
+          <t>aerovanc,firvanq,firvanq kit,televancin,vibativ</t>
         </is>
       </c>
       <c r="J441" t="e">
@@ -27666,7 +27666,7 @@
       </c>
       <c r="I442" t="inlineStr">
         <is>
-          <t>levviax,telithromycin</t>
+          <t>ketek,levviax</t>
         </is>
       </c>
       <c r="J442">
@@ -27730,7 +27730,7 @@
       </c>
       <c r="I443" t="inlineStr">
         <is>
-          <t>omniflox,temafloxacin,temafloxacina,temafloxacine,temafloxacinum</t>
+          <t>omniflox,sarafin,saraflox,saraflox injectable,saraflox wsp,temafloxacina,temafloxacine,temafloxacinum</t>
         </is>
       </c>
       <c r="J443">
@@ -27794,7 +27794,7 @@
       </c>
       <c r="I444" t="inlineStr">
         <is>
-          <t>negaban,temocilina,temocillin,temocillina,temocilline,temocillinum</t>
+          <t>negaban,temocilina,temocillin disalt,temocillina,temocilline,temocillinum</t>
         </is>
       </c>
       <c r="J444" t="e">
@@ -27858,7 +27858,7 @@
       </c>
       <c r="I445" t="inlineStr">
         <is>
-          <t>corbinal,lamasil,lamisil,lamisil at,lamisil tablet,terbinafina,terbinafine,terbinafinum,terbinex</t>
+          <t>afogan,antifungal foot,athletes foot,bramazil,bramizil,corbinal,innonyx,krogerantifungal,lamasil,lamisil,lamisil at cream,lamisil krem,lamisil tablet,lamisilat jock itch,muzonal,mycova,shopkoathletes foot,shoprite,silkaantifungal,silkagel,silkajock itch,terbifoam,terbina,terbinafina,terbinafine hcl?,terbinafinum,terbine,terbinex,terbisil,zabel</t>
         </is>
       </c>
       <c r="J445">
@@ -27918,7 +27918,7 @@
       </c>
       <c r="I446" t="inlineStr">
         <is>
-          <t>fungistat,panlomyc,terazol,terconazol,terconazole,terconazolum,tercospor,triaconazole,zazole</t>
+          <t>fungistat,panlomyc,terazol,terconazol,terconazolum,tercospor,triaconazole,zazole</t>
         </is>
       </c>
       <c r="J446" t="e">
@@ -27980,7 +27980,7 @@
       </c>
       <c r="I447" t="inlineStr">
         <is>
-          <t>terivalidin,terizidon,terizidona,terizidone,terizidonum</t>
+          <t>terivalidin,terizidon,terizidona,terizidonum</t>
         </is>
       </c>
       <c r="J447" t="e">
@@ -28042,7 +28042,7 @@
       </c>
       <c r="I448" t="inlineStr">
         <is>
-          <t>abramycin,abricycline,achromycin,achromycin v,actisite,agromicina,ambramicina,ambramycin,amycin,biocycline,bristaciclin,bristaciclina,bristacycline,brodspec,cefracycline,centet,ciclibion,copharlan,criseociclina,cyclomycin,cyclopar,cytome,democracin,deschlorobiomycin,dumocyclin,economycin,enterocycline,hostacyclin,lexacycline,limecycline,liquamycin,medocycline,mericycline,micycline,neocycline,oletetrin,omegamycin,orlycycline,panmycin,piracaps,polycycline,polyotic,purocyclina,resteclin,robitet,roviciclina,sigmamycin,solvocin,sumycin,sumycin syrup,supramycin,sustamycin,tetrabid organon,tetrabon,tetrachel,tetraciclina,tetracycl,tetracyclin,tetracycline,tetracycline base,tetracycline i,tetracycline ii,tetracyclinehydrate,tetracyclinum,tetracyn,tetradecin,tetrafil,tetramed,tetrasure,tetraverine,tetrazyklin,tetrex,topicycline,tsiklomistsin,tsiklomitsin,veracin,vetacyclinum,vetquamycin</t>
+          <t>abbocin,abramycin,abricycline,achromycin,achromycin v,acromicina,actisite,agromicina,ala tet,alamycin,ambramicina,ambramycin,amycin,aquacycline,artomycin,bi steclin,biocycline,biosolvomycin,biotet,bisolvomycin,bristaciclin,bristaciclin .alpha.,bristaciclina,bristacycline,brodspec,cefracycline,cefracycline tablets,centet,chrysocin,ciclibion,copharlan,criseociclina,cyclomycin,cyclopar,cytome,dalimycin,dalinmycin,democracin,deschlorobiomycin,diacycine,dispatetrin,dumocyclin,economycin,elinton,engemycin,enterocycline,hostacyclin,hostacycline,hydrocyclin,ibicyn,imperacin,intaloxin,lemtrex,lexacycline,limecycline,liquachel,liquamycin,macodyn,medocycline,mepatar,mephacyclin,mericycline,micycline,neocyclin b,neocycline,neocycline b,oletetrin,omegamycin,orlycycline,otetryn,oxacycline,oxamycen,oxatet,oxlopar,oxy,oxybiocycline,oxycycline,oxydon,oxyject,oxymykoin,oxysteclin,oxytet,oxytetracycline.hcl,oxytetral,oxytetrin,oxytracyl,oxyvet,paltet,panmycin,partrex,piracaps,polycycline,polyotic,purocyclina,qidtet,quadracycline,quatrex,remicyclin,resteclin,retet,ricycline,robitet,roviciclina,sigmamycin,solvocin,steclin,stecsolin,stilciclina,subamycin,sumycin,supramycin,sustamycin,talsutin,tefilin,teline,telotrex,terraject,terramycin,tetrabakat,tetrabid,tetrabid organon,tetrablet,tetrabon,tetracaps,tetrachel,tetraciclina,tetracompren,tetracycl,tetracyclin,tetracyclinbase,tetracycline i,tetracycline.hcl,tetracyclinehydrate,tetracyclinum,tetracyn,tetradecin,tetrafil,tetrakap,tetralution,tetramavan,tetramed,tetran hydrochloride,tetraseptine,tetrasure,tetraverine,tetrazyklin,tetrex,tetrosol,topicycline,toxinal,triphacyclin,tsiklomistsin,tsiklomitsin,unicin,unimycin,vendarcin,veracin,vetacyclinum,vetquamycin</t>
         </is>
       </c>
       <c r="J448">
@@ -28166,7 +28166,7 @@
       </c>
       <c r="I450" t="inlineStr">
         <is>
-          <t>tetroxoprim,tetroxoprima,tetroxoprime,tetroxoprimum</t>
+          <t>primsol,tetroxoprima,tetroxoprime,tetroxoprimum,trimpex,trimplex</t>
         </is>
       </c>
       <c r="J450" t="e">
@@ -28224,7 +28224,7 @@
       </c>
       <c r="I451" t="inlineStr">
         <is>
-          <t>aktivan,ambathizon,amithiozone,amithizone,amitiozon,benthiozone,benzothiozane,benzothiozon,berculon a,berkazon,citazone,conteben,diasan,diazan,domakol,ilbion,livazone,mirizone neustab,mivizon,myvizone,neotibil,neustab,novakol,nuclon argentinian,panrone,parazone,seroden,siocarbazone,tebalon,tebecure,tebemar,tebesone i,tebethion,tebethione,tebezon,thiacetazone,thiacetone,thiacetozone,thibon,thibone,thioacetazon,thioacetazone,thioacetazonum,thioazetazone,thiocarbazil,thiomicid,thionicid,thioparamizon,thioparamizone,thiosemicarbarzone,thiosemicarbazone,thiotebesin,thiotebezin,thiotebicina,thizone,tiacetazon,tibicur,tibion,tibione,tibizan,tibone,tioacetazon,tioacetazona,tioatsetazon,tiobicina,tiocarone,tiosecolo,tubercazon,tubigal</t>
+          <t>aktivan,ambathizon,amithiozone,amithizone,amitiozon,benthiozone,benzothiozane,benzothiozon,berculon a,berkazon,citazone,conteben,diasan,diazan,domakol,ilbion,livazone,mirizone neustab,mivizon,myvizone,neotibil,neustab,novakol,nuclon argentinian,panrone,parazone,seroden,siocarbazone,tebalon,tebecure,tebemar,tebesone i,tebethion,tebethione,tebezon,thiacetazone?,thiacetone,thiacetozone,thibon,thibone,thioacetazon,thioacetazonum,thioazetazone,thiocarbazil,thiomicid,thionicid,thioparamizon,thioparamizone,thiosemicarbarzone,thiosemicarbazone,thiotebesin,thiotebezin,thiotebicina,thizone,tiacetazon,tibicur,tibion,tibione,tibizan,tibone,tioacetazon,tioacetazona,tioatsetazon,tiobicina,tiocarone,tiosecolo,tubercazon,tubigal</t>
         </is>
       </c>
       <c r="J451" t="e">
@@ -28286,7 +28286,7 @@
       </c>
       <c r="I452" t="inlineStr">
         <is>
-          <t>descocin,dexawin,dextrosulfenidol,dextrosulphenidol,efnicol,hyrazin,igralin,macphenicol,masatirin,neomyson,racefenicol,racefenicolo,racefenicolum,raceophenidol,racephenicol,rincrol,thiamcol,thiamphenicol,thiamphenicolum,thiocymetin,thiomycetin,thiophenicol,tiamfenicol,tiamfenicolo,urfamicina,urfamycine,vicemycetin</t>
+          <t>descocin,dexawin,dextrosulfenidol,dextrosulphenidol,efnicol,fricol,hyrazin,igralin,macphenicol,masatirin,neomyson,racefenicol,racefenicolo,racefenicolum,raceophenidol,racephenicol,rincrol,thiamcol,thiamphenicol epimer,thiamphenicolum,thiocymetin,thiomycetin,thiophenicol,tiamfenicol,tiamfenicolo,urfamicina,urfamycine,urophenyl,vicemycetin</t>
         </is>
       </c>
       <c r="J452">
@@ -28352,7 +28352,7 @@
       </c>
       <c r="I453" t="inlineStr">
         <is>
-          <t>aktivan,ambathizon,amithiozone,amitiozon,benthiozone,benzothiozane,benzothiozon,berculon a,berkazon,citazone,conteben,diasan,domakol,ilbion,livazone,mirizone neustab,mivizon,myvizone,neotibil,neustab,novakol,nuclon argentinian,panrone,parazone,seroden,siocarbazone,tebalon,tebecure,tebemar,tebesone i,tebethion,tebethione,tebezon,thiacetone,thiacetozone,thibon,thibone,thioacetazon,thioacetazone,thioacetazonum,thioazetazone,thiocarbazil,thiomicid,thionicid,thioparamizon,thioparamizone,thiosemicarbarzone,thiosemicarbazone,thiotebesin,thiotebezin,thiotebicina,thizone,tiacetazon,tibicur,tibion,tibione,tibizan,tibone,tioacetazon,tioacetazona,tioatsetazon,tiobicina,tiocarone,tiosecolo,tubercazon,tubigal</t>
+          <t>aktivan,ambathizon,amithiozone,amitiozon,benthiozone,benzothiozane,benzothiozon,berculon a,berkazon,citazone,conteben,diasan,domakol,ilbion,livazone,mirizone neustab,mivizon,myvizone,neotibil,neustab,novakol,nuclon argentinian,panrone,parazone,seroden,siocarbazone,tebalon,tebecure,tebemar,tebesone i,tebethion,tebethione,tebezon,thiacetazone?,thiacetone,thiacetozone,thibon,thibone,thioacetazon,thioacetazonum,thioazetazone,thiocarbazil,thiomicid,thionicid,thioparamizon,thioparamizone,thiosemicarbarzone,thiosemicarbazone,thiotebesin,thiotebezin,thiotebicina,thizone,tiacetazon,tibicur,tibion,tibione,tibizan,tibone,tioacetazon,tioacetazona,tioatsetazon,tiobicina,tiocarone,tiosecolo,tubercazon,tubigal</t>
         </is>
       </c>
       <c r="J453" t="e">
@@ -28472,7 +28472,7 @@
       </c>
       <c r="I455" t="inlineStr">
         <is>
-          <t>denagard,thiamutilin,tiamulin,tiamulin pamoate,tiamulina,tiamuline,tiamulinum,tiavet p</t>
+          <t>denagard,thiamutilin,tiamulin pamoate,tiamulina,tiamuline,tiamulinum,tiavet p</t>
         </is>
       </c>
       <c r="J455" t="e">
@@ -28534,7 +28534,7 @@
       </c>
       <c r="I456" t="inlineStr">
         <is>
-          <t>ticarcilina,ticarcillin,ticarcilline,ticarcillinum,ticillin,timentin</t>
+          <t>ticarcilina,ticarcilline,ticarcillinum,ticillin,timentin</t>
         </is>
       </c>
       <c r="J456" t="e">
@@ -28598,7 +28598,7 @@
       </c>
       <c r="I457" t="inlineStr">
         <is>
-          <t>timentin</t>
+          <t>augpenin,timentin</t>
         </is>
       </c>
       <c r="J457" t="e">
@@ -28662,7 +28662,7 @@
       </c>
       <c r="I458" t="inlineStr">
         <is>
-          <t>haizheng li xing,tigeciclina,tigecyclin,tigecycline,tigecycline hydrate,tigecyclinum,tigilcycline,tygacil</t>
+          <t>haizheng li xing,tigeciclina,tigecyclin,tigecyclinehydrate,tigecyclinum,tigilcycline,tygacil</t>
         </is>
       </c>
       <c r="J458" t="e">
@@ -28722,7 +28722,7 @@
       </c>
       <c r="I459" t="inlineStr">
         <is>
-          <t>tilbroquinol,tilbroquinolum</t>
+          <t>tilbroquinolum</t>
         </is>
       </c>
       <c r="J459" t="e">
@@ -28780,7 +28780,7 @@
       </c>
       <c r="I460" t="inlineStr">
         <is>
-          <t>tildipirosin,zuprevo</t>
+          <t>zuprevo</t>
         </is>
       </c>
       <c r="J460" t="e">
@@ -28838,7 +28838,7 @@
       </c>
       <c r="I461" t="inlineStr">
         <is>
-          <t>micotil,pulmotil,tilmicosin,tilmicosina,tilmicosine,tilmicosinum</t>
+          <t>micotil,pulmotil,tilmicosina,tilmicosine,tilmicosinum</t>
         </is>
       </c>
       <c r="J461" t="e">
@@ -28900,7 +28900,7 @@
       </c>
       <c r="I462" t="inlineStr">
         <is>
-          <t>amtiba,bioshik,ethyl sulfone,fasigin,fasigyn,fasigyntrade mark,fasygin,glongyn,haisigyn,pletil,simplotan,simplotantrade mark,sorquetan,symplotan,tindamax,tindamaxtrade mark,tinidazol,tinidazole,tinidazolum,tricolam,trimonase</t>
+          <t>amtiba,bioshik,ethyl sulfone,fasigin,fasigyn,fasigyntrade mark,fasygin,glongyn,haisigyn,isotinidazole,pletil,simplotan,simplotantrade mark,sorquetan,symplotan,tindamax,tindamaxtrade mark,tinidazol,tinidazolum,tricolam,trimonase</t>
         </is>
       </c>
       <c r="J462">
@@ -28966,7 +28966,7 @@
       </c>
       <c r="I463" t="inlineStr">
         <is>
-          <t>amixyl,datanil,disocarban,disoxyl,isoxyl,thiocarlide,tiocarlid,tiocarlida,tiocarlide,tiocarlidum</t>
+          <t>aethoksid,aethoxyd,aethoxydum,amixyl,datanil,disocarban,disoxyl,ethoxide,ethoxyd,etocarlid,etocarlida,etocarlide,etocarlidum,etoksid,isoxyl,thiocarlide,tiocarlid,tiocarlida,tiocarlidum</t>
         </is>
       </c>
       <c r="J463">
@@ -29026,7 +29026,7 @@
       </c>
       <c r="I464" t="inlineStr">
         <is>
-          <t>cloruro de tiodonio,tiodonii chloridum,tiodonium chloride</t>
+          <t>cloruro de tiodonio,tiodonii chloridum,tiodonium,tiodonium cation</t>
         </is>
       </c>
       <c r="J464" t="e">
@@ -29084,7 +29084,7 @@
       </c>
       <c r="I465" t="inlineStr">
         <is>
-          <t>tioxacin,tioxacine,tioxacino,tioxacinum,tioxic acid</t>
+          <t>tioxacine,tioxacino,tioxacinum,tioxic acid</t>
         </is>
       </c>
       <c r="J465" t="e">
@@ -29204,7 +29204,7 @@
       </c>
       <c r="I467" t="inlineStr">
         <is>
-          <t>bethkis,brulamycin,deoxykanamycin b,distobram,gernebcin,gotabiotic,kitabis,kitabis pak,nebcin,nebicin,nebramycin,nebramycin vi,obramycin,sybryx,tenebrimycin,tenemycin,tobacin,tobi podhaler,tobracin,tobradex,tobradistin,tobralex,tobramaxin,tobramicin,tobramicina,tobramitsetin,tobramycetin,tobramycin,tobramycin base,tobramycin sulfate,tobramycine,tobramycinum,tobrased,tobrasone,tobrex</t>
+          <t>bethkis,brulamycin,deoxykanamycin b,distobram,gernebcin,gotabiotic,kitabis,kitabis pak,nebcin,nebicin,nebramycin,obramycin,sybryx,tenebrimycin,tenemycin,tobacin,tobi podhaler,tobracin,tobradex,tobradistin,tobralex,tobramaxin,tobramicin,tobramicina,tobramitsetin,tobramycetin,tobramycine,tobramycinum,tobrased,tobrasone,tobrex</t>
         </is>
       </c>
       <c r="J467" t="e">
@@ -29322,7 +29322,7 @@
       </c>
       <c r="I469" t="inlineStr">
         <is>
-          <t>tosufloxacin</t>
+          <t/>
         </is>
       </c>
       <c r="J469">
@@ -29386,7 +29386,7 @@
       </c>
       <c r="I470" t="inlineStr">
         <is>
-          <t>abaprim,alprim,anitrim,antrima,antrimox,bacdan,bacidal,bacide,bacterial,bacticel,bactifor,bactin,bactoprim,bactramin,bactrim,bencole,bethaprim,biosulten,briscotrim,chemotrin,colizole,colizole ds,conprim,cotrimel,cotrimoxizole,deprim,dosulfin,duocide,esbesul,espectrin,euctrim,exbesul,fermagex,fortrim,idotrim,ikaprim,infectotrimet,instalac,kombinax,lagatrim,lagatrim forte,lastrim,lescot,methoprim,metoprim,monoprim,monotrim,monotrimin,novotrimel,omstat,oraprim,pancidim,polytrim,priloprim,primosept,primsol,proloprim,protrin,purbal,resprim,resprim forte,roubac,roubal,salvatrim,septrin ds,septrin forte,septrin s,setprin,sinotrim,stopan,streptoplus,sugaprim,sulfamar,sulfamethoprim,sulfoxaprim,sulthrim,sultrex,syraprim,tiempe,tmp smx,toprim,trimanyl,trimethioprim,trimethopim,trimethoprim,trimethoprime,trimethoprimum,trimethopriom,trimetoprim,trimetoprima,trimexazole,trimexol,trimezol,trimogal,trimono,trimopan,trimpex,triprim,trisul,trisulcom,trisulfam,trisural,uretrim,urobactrim,utetrin,velaten,wellcoprim,wellcoprin,xeroprim,zamboprim</t>
+          <t>abaprim,alprim,anitrim,antrima,antrimox,bacdan,bacidal,bacide,bacterial,bacticel,bactifor,bactin,bactoprim,bactramin,bactrim,bencole,bethaprim,biosulten,briscotrim,chemotrin,colizole,conprim,cotrimel,cotrimoxizole,deprim,dosulfin,duocide,esbesul,espectrin,euctrim,exbesul,fermagex,fortrim,idotrim,ikaprim,infectotrimet,instalac,kombinax,lagatrim,lagatrim forte,lastrim,lescot,methoprim,metoprim,monoprim,monotrim,monotrimin,novotrimel,omstat,oraprim,pancidim,polytrim,priloprim,primosept,primsol,proloprim,protrin,purbal,resprim,resprim forte,roubac,roubal,salvatrim,septrin,septrin forte,septrin s,setprin,sinotrim,stopan,streptoplus,sugaprim,sulfamar,sulfamethoprim,sulfoxaprim,sulthrim,sultrex,syraprim,tiempe,tmp smx,toprim,trimanyl,trimethioprim,trimethopim,trimethoprime,trimethoprimum,trimethopriom,trimetoprim,trimetoprima,trimexazole,trimexol,trimezol,trimogal,trimono,trimopan,trimpex,triprim,trisul,trisulcom,trisulfam,trisural,uretrim,urobactrim,utetrin,velaten,wellcoprim,wellcoprin,xeroprim,zamboprim</t>
         </is>
       </c>
       <c r="J470">
@@ -29452,7 +29452,7 @@
       </c>
       <c r="I471" t="inlineStr">
         <is>
-          <t>abacin,abactrim,agoprim,alfatrim,aposulfatrim,bacteral,bacterial forte,bactilen,bactiver,bacton,bactoreduct,bactrim,bactrim ds,bactrim forte,bactrim pediatric,bactrimel,bactrizol,bactromin,bactropin,baktar,belcomycine,berlocid,bibacrim,biseptol,chemitrim,chemotrim,ciplin,colimycin,colimycin sulphate,colisticin,colistimethate,colistimethate sodium,colistin sulfate,colistin sulphate,colomycin,coly-mycin,cotribene,cotrim d.s.,cotrim eu rho,cotrim holsen,cotrim.l.u.t.,cotrimaxazol,cotrimazole,cotrimhexal,cotrimoxazol,cotrimoxazol al,cotrimoxazole,cotrimstada,cotriver,dibaprim,drylin,duratrimet,eltrianyl,escoprim,esteprim,eusaprim,fectrim,gantaprim,gantaprin,gantrim,groprim,helveprim,imexim,jenamoxazol,kemoprim,kepinol,kepinol forte,laratrim,linaris,maxtrim,microtrim,microtrim forte,mikrosid,momentol,oecotrim,oriprim,oxaprim,pantoprim,polymyxin e,polymyxin e. sulfate,primazole,promixin,septra,septra ds,septra grape,septrim,septrin,servitrim,sigaprim,sigaprin,sulfatrim pediatric,sulfotrim,sulfotrimin,sulmeprim pediatric,sulprim,sumetrolim,supracombin,suprim,tacumil,teleprim,teleprin,thiocuran,totazina,tribakin,trifen,trigonyl,trimesulf,trimetho comp,trimethoprimsulfa,trimetoger,trimexazol,trimforte,trimosulfa,uroplus,uroplus ds,uroplus ss</t>
+          <t>abacin,abactrim,agoprim,alfatrim,aposulfatrim,bacteral,bacterial forte,bactilen,bactiver,bacton,bactoreduct,bactrim,bactrim forte,bactrimel,bactrizol,bactromin,bactropin,baktar,belcomycine,berlocid,bibacrim,biseptol,chemitrim,chemotrim,ciplin,colimycin,colisticin,colistimethate,colomycin,coly-mycin,cotribene,cotrim,cotrim eu rho,cotrim holsen,cotrim.l.u.t.,cotrimaxazol,cotrimazole,cotrimhexal,cotrimoxazol,cotrimoxazole,cotrimstada,cotriver,dibaprim,drylin,duratrimet,eltrianyl,escoprim,esteprim,eusaprim,fectrim,gantaprim,gantaprin,gantrim,groprim,helveprim,imexim,jenamoxazol,kemoprim,kepinol,kepinol forte,laratrim,linaris,maxtrim,microtrim,microtrim forte,mikrosid,momentol,oecotrim,oriprim,oxaprim,pantoprim,polymyxin e,polymyxin e.,potrox,primazole,promixin,septra,septra grape,septrim,septrin,servitrim,sigaprim,sigaprin,sulfatrim,sulfotrim,sulfotrimin,sulmeprim,sulprim,sumetrolim,supracombin,suprim,tacumil,teleprim,teleprin,thiocuran,totazina,tribakin,trifen,trigonyl,trimesulf,trimetho comp,trimethoprimsulfa,trimetoger,trimexazol,trimforte,trimosulfa,uroplus</t>
         </is>
       </c>
       <c r="J471" t="e">
@@ -29514,7 +29514,7 @@
       </c>
       <c r="I472" t="inlineStr">
         <is>
-          <t>acetyloleandomycin,aovine,cyclamycin,evramicina,matromicina,matromycin t,micotil,oleandocetine,oleandomycin,t.a.o.,treolmicina,tribiocillina,triocetin,triolan,troleandomicina,troleandomycin,troleandomycine,troleandomycinum,viamicina,wytrion</t>
+          <t>acetyloleandomycin,aovine,cyclamycin,evramicina,matromicina,matromycin t,micotil,oleandocetin,oleandocetine,t.a.o.,treolmicina,tribiocillina,triocetin,triolan,troleandomicina,troleandomycine,troleandomycinum,viamicina,wytrion</t>
         </is>
       </c>
       <c r="J472">
@@ -29574,7 +29574,7 @@
       </c>
       <c r="I473" t="inlineStr">
         <is>
-          <t>rubidiumnitrate,trospectinomycin,trospectomicina,trospectomycin,trospectomycine,trospectomycinum</t>
+          <t>rubidiumnitrate,trospectinomycin,trospectomicina,trospectomycine,trospectomycinum</t>
         </is>
       </c>
       <c r="J473" t="e">
@@ -29636,7 +29636,7 @@
       </c>
       <c r="I474" t="inlineStr">
         <is>
-          <t>trovafloxacin,trovan</t>
+          <t>trovan</t>
         </is>
       </c>
       <c r="J474">
@@ -29698,7 +29698,7 @@
       </c>
       <c r="I475" t="inlineStr">
         <is>
-          <t>draxxin,tulathrmycin a,tulathromycin,tulathromycin a</t>
+          <t>draxxin,tulathrmycin a,tulathromycin a</t>
         </is>
       </c>
       <c r="J475" t="e">
@@ -29756,7 +29756,7 @@
       </c>
       <c r="I476" t="inlineStr">
         <is>
-          <t>fradizine,tilosina,tylocine,tylosin,tylosin a,tylosine,tylosinum</t>
+          <t>fradizine,tilosina,tylocine,tylosin a,tylosine,tylosinum</t>
         </is>
       </c>
       <c r="J476" t="e">
@@ -29814,7 +29814,7 @@
       </c>
       <c r="I477" t="inlineStr">
         <is>
-          <t>tylvalosin</t>
+          <t/>
         </is>
       </c>
       <c r="J477" t="e">
@@ -29934,7 +29934,7 @@
       </c>
       <c r="I479" t="inlineStr">
         <is>
-          <t>vancocin,vancocin hcl,vancoled,vancomicina,vancomycin,vancomycin hcl,vancomycine,vancomycinum,vancor,viomycin derivative</t>
+          <t>aerovanc,firvanq,firvanq kit,targocid,vancocin,vancoled,vancomicina,vancomycine,vancomycinum,vancor,viomycin derivative</t>
         </is>
       </c>
       <c r="J479">
@@ -30054,7 +30054,7 @@
       </c>
       <c r="I481" t="inlineStr">
         <is>
-          <t>celiomycin,florimycin,floromycin,tuberactinomycin b,vinacetin a,vioactane,viomicina,viomycin,viomycine,viomycinum</t>
+          <t>celiomycin,florimycin,floromycin,solfato di viomicina,tuberactinomycin b,vinacetin a,vioactane,viocin,viomicina,viomycine,viomycinum</t>
         </is>
       </c>
       <c r="J481" t="e">
@@ -30112,7 +30112,7 @@
       </c>
       <c r="I482" t="inlineStr">
         <is>
-          <t>eskalin,eskalin v,micamicina,mikamycin,mikamycine,mikamycinum,ostreogricina,ostreogrycin,ostreogrycine,ostreogrycinum,pristinamicina,pristinamycin,pristinamycine,pristinamycinum,pyostacine,stafac,stafytracine,staphylomycin,stapyocine,starfac,streptogramin,vernamycin,virgimycin,virgimycine,virginiamicina,virginiamycin,virginiamycina,virginiamycine,virginiamycinum</t>
+          <t>eskalin,eskalin v,micamicina,mikamycin,mikamycine,mikamycinum,ostreogricina,ostreogrycin,ostreogrycine,ostreogrycinum,pristinamicina,pristinamycine,pristinamycinum,pyostacine,stafac,stafytracine,staphylomycin,stapyocine,starfac,streptogramin,vernamycin,virgimycin,virgimycine,virginiamicina,virginiamycin,virginiamycina,virginiamycinum</t>
         </is>
       </c>
       <c r="J482" t="e">
@@ -30174,7 +30174,7 @@
       </c>
       <c r="I483" t="inlineStr">
         <is>
-          <t>pfizer,vfend i.v.,voriconazol,voriconazole,voriconazole vfend,voriconazolum,voriconzole,vorikonazole</t>
+          <t>pfizer,vfend,voriconazol,voriconazole vfend,voriconazolum,voriconzole,vorikonazole</t>
         </is>
       </c>
       <c r="J483">
@@ -30240,7 +30240,7 @@
       </c>
       <c r="I484" t="inlineStr">
         <is>
-          <t>bactacine,bracen,nanbacine,xibornol,xibornolo,xibornolum</t>
+          <t>bactacine,bracen,nanbacine,xibornolo,xibornolum</t>
         </is>
       </c>
       <c r="J484" t="e">
@@ -30298,7 +30298,7 @@
       </c>
       <c r="I485" t="inlineStr">
         <is>
-          <t>zidebactam</t>
+          <t>zidebactamsalt</t>
         </is>
       </c>
       <c r="J485" t="e">
@@ -30354,7 +30354,7 @@
       </c>
       <c r="I486" t="inlineStr">
         <is>
-          <t>zoliflodacin</t>
+          <t/>
         </is>
       </c>
       <c r="J486" t="e">

</xml_diff>

<commit_message>
(v2.1.1.9141) new AMR selectors, eucast overwrite arg
</commit_message>
<xml_diff>
--- a/data-raw/antibiotics.xlsx
+++ b/data-raw/antibiotics.xlsx
@@ -369,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:N487"/>
+  <dimension ref="A1:N488"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="1" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
@@ -730,7 +730,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>amicacin,amikacillin,amikacinbase,amikacindihydrate,amikacinfreebase,amikacinsulfate,amikacina,amikacine,amikacinum,amikavet,amikin,amiklin,amikozit,amukin,arikace,arikayceliposomal,briclin,kaminax,lukadin,mikavir,pierami,potentox</t>
+          <t>amicacin,amikacillin,amikacina,amikacinbase,amikacindihydrate,amikacine,amikacinfreebase,amikacinsulfate,amikacinum,amikavet,amikin,amiklin,amikozit,amukin,arikace,arikayceliposomal,briclin,kaminax,lukadin,mikavir,pierami,potentox</t>
         </is>
       </c>
       <c r="J6" t="e">
@@ -914,7 +914,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>actimoxi,amoclen,amolin,amopen,amopenixin,amoxibiotic,amoxicaps,amoxicilina,amoxicillinhydrate,amoxicilline,amoxicillinum,amoxiden,amoxil,amoxivet,amoxy,amoxycillin,amoxyke,anemolin,aspenil,atoksilin,biomox,bristamox,cemoxin,clamoxyl,damoxy,delacillin,demoksil,dispermox,efpenix,flemoxin,hiconcil,histocillin,hydroxyampicillin,ibiamox,imacillin,lamoxy,largopen,metafarmacapsules,metifarmacapsules,moksilin,moxacin,moxatag,ospamox,pamoxicillin,piramox,promoxil,remoxil,robamox,sawamoxpm,tolodina,topramoxin,unicillin,utimox,vetramox</t>
+          <t>actimoxi,amoclen,amolin,amopen,amopenixin,amoxibiotic,amoxicaps,amoxicilina,amoxicilline,amoxicillinhydrate,amoxicillinum,amoxiden,amoxil,amoxivet,amoxy,amoxycillin,amoxyke,anemolin,aspenil,atoksilin,biomox,bristamox,cemoxin,clamoxyl,damoxy,delacillin,demoksil,dispermox,efpenix,flemoxin,hiconcil,histocillin,hydroxyampicillin,ibiamox,imacillin,lamoxy,largopen,metafarmacapsules,metifarmacapsules,moksilin,moxacin,moxatag,ospamox,pamoxicillin,piramox,promoxil,remoxil,robamox,sawamoxpm,tolodina,topramoxin,unicillin,utimox,vetramox</t>
         </is>
       </c>
       <c r="J9">
@@ -980,7 +980,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>amocla,amoclan,amoclav,amoksiclav,amoxsiklav,amoxyclav,augmentan,augmentin,augmentinxr,augmentine,auspilic,clamentin,clamobit,clavamox,clavinex,clavoxilinplus,clavulin,clavumox,coamoxiclav,eumetinex,kmoxilin,spectramox,spektramox,synulox,viaclav,xiclav</t>
+          <t>amocla,amoclan,amoclav,amoksiclav,amoxsiklav,amoxyclav,augmentan,augmentin,augmentine,augmentinxr,auspilic,clamentin,clamobit,clavamox,clavinex,clavoxilinplus,clavulin,clavumox,coamoxiclav,eumetinex,kmoxilin,spectramox,spektramox,synulox,viaclav,xiclav</t>
         </is>
       </c>
       <c r="J10">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>acillin,adobacillin,amblosin,amcill,amfipen,amfipenv,amipenixs,ampichel,ampicil,ampicilina,ampicillina,ampicillinacid,ampicillinanhydrate,ampicillinanhydrous,ampicillinbase,ampicillinhydrate,ampicillinsodium,ampicilline,ampicillinum,ampicin,ampifarm,ampikel,ampimed,ampipenin,ampiscel,ampisyn,ampivax,ampivet,amplacilina,amplin,amplipenyl,amplisom,amplital,anhydrousampicillin,austrapen,binotal,bonapicillin,britacil,campicillin,copharcilin,delcillin,deripen,divercillin,doktacillin,duphacillin,grampenil,guicitrina,guicitrine,lifeampil,marcillin,morepen,norobrittin,nuvapen,olinkid,omnipen,orbicilina,penaoral,penampil,penbristol,penbritin,penbritinpaediatric,penbritinsyrup,penbrock,penicline,penimic,pensyn,pentrex,pentrexl,pentrexyl,pentritin,pfizerpena,polycillin,polyflex,ponecil,princillin,principen,qidamp,racenacillin,redicilin,rosampline,roscillin,semicillin,semicillinr,servicillin,sumipanto,synpenin,texcillin,tokiocillin,tolomol,totacillin,totalciclina,totapen,trifacilina,ukapen,ultrabion,ultrabron,vampen,viccillin,viccillins,vidocillin,wypicil</t>
+          <t>acillin,adobacillin,amblosin,amcill,amfipen,amfipenv,amipenixs,ampichel,ampicil,ampicilina,ampicillina,ampicillinacid,ampicillinanhydrate,ampicillinanhydrous,ampicillinbase,ampicilline,ampicillinhydrate,ampicillinsodium,ampicillinum,ampicin,ampifarm,ampikel,ampimed,ampipenin,ampiscel,ampisyn,ampivax,ampivet,amplacilina,amplin,amplipenyl,amplisom,amplital,anhydrousampicillin,austrapen,binotal,bonapicillin,britacil,campicillin,copharcilin,delcillin,deripen,divercillin,doktacillin,duphacillin,grampenil,guicitrina,guicitrine,lifeampil,marcillin,morepen,norobrittin,nuvapen,olinkid,omnipen,orbicilina,penampil,penaoral,penbristol,penbritin,penbritinpaediatric,penbritinsyrup,penbrock,penicline,penimic,pensyn,pentrex,pentrexl,pentrexyl,pentritin,pfizerpena,polycillin,polyflex,ponecil,princillin,principen,qidamp,racenacillin,redicilin,rosampline,roscillin,semicillin,semicillinr,servicillin,sumipanto,synpenin,texcillin,tokiocillin,tolomol,totacillin,totalciclina,totapen,trifacilina,ukapen,ultrabion,ultrabron,vampen,viccillin,viccillins,vidocillin,wypicil</t>
         </is>
       </c>
       <c r="J14">
@@ -2179,7 +2179,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Beta-lactams/penicillins</t>
+          <t>Monobactams</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -2243,7 +2243,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Beta-lactams/penicillins</t>
+          <t>Monobactams</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Beta-lactams/penicillins</t>
+          <t>Monobactams</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -2754,7 +2754,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>abbocillin,ayercillin,bencilpenicilina,benzopenicillin,benzylpenicilling,benzylpenicilline,benzylpenicillinum,bicillin,cillora,cilloral,cilopen,compocilling,cosmopen,dropcillin,freepenicilling,freepenicillinii,galofak,gelacillin,liquacillin,megacillin,pencilling,penicillin,penicilling,pentids,permapen,pfizerpen,pfizerpeng,pharmacillin,pradupen,specillineg,ursopen</t>
+          <t>abbocillin,ayercillin,bencilpenicilina,benzopenicillin,benzylpenicilline,benzylpenicilling,benzylpenicillinum,bicillin,cillora,cilloral,cilopen,compocilling,cosmopen,dropcillin,freepenicilling,freepenicillinii,galofak,gelacillin,liquacillin,megacillin,pencilling,penicillin,penicilling,pentids,permapen,pfizerpen,pfizerpeng,pharmacillin,pradupen,specillineg,ursopen</t>
         </is>
       </c>
       <c r="J39" t="e">
@@ -3405,7 +3405,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Other antibacterials</t>
+          <t>Monobactams</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -3744,7 +3744,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>alcephin,alexin,alsporin,amplex,anhydrouscefalexin,anhydrouscephalexin,biocef,carnosporin,cefablan,cefadal,cefadin,cefadina,cefaleksin,cefalessina,cefalexinanhydrous,cefalexina,cefalexine,cefalexinum,cefalin,cefaloto,cefaseptin,ceffanex,ceflax,ceforal,cefovit,celexin,cepastar,cepexin,cephacillin,cephalexin,cephalexinanhydrous,cephalexine,cephalexinum,cephanasten,cephaxin,cephin,ceporex,ceporexforte,ceporexin,ceporexine,cerexin,cerexins,cophalexin,durantel,durantelds,erocetin,factagard,felexin,ibilex,ibrexin,inphalex,kefalospes,keflet,keflex,kefolan,keforal,keftab,kekrinal,kidolex,lafarine,larixin,lenocef,lexibiotico,lonflex,lopilexin,madlexin,mamalexin,mamlexin,medoxine,neokef,neolexina,novolexin,optocef,oracef,oriphex,oroxin,ortisporina,ospexin,palitrex,panixinedisperdose,pectril,pyassan,roceph,rocephdistab,sanaxin,sartosona,sencephalin,sepexin,servispor,sialexin,sinthecillin,sporicef,sporidex,syncle,synecl,tepaxin,tokiolexin,uphalexin,voxxim,winlex,zozarine</t>
+          <t>alcephin,alexin,alsporin,amplex,anhydrouscefalexin,anhydrouscephalexin,biocef,carnosporin,cefablan,cefadal,cefadin,cefadina,cefaleksin,cefalessina,cefalexina,cefalexinanhydrous,cefalexine,cefalexinum,cefalin,cefaloto,cefaseptin,ceffanex,ceflax,ceforal,cefovit,celexin,cepastar,cepexin,cephacillin,cephalexin,cephalexinanhydrous,cephalexine,cephalexinum,cephanasten,cephaxin,cephin,ceporex,ceporexforte,ceporexin,ceporexine,cerexin,cerexins,cophalexin,durantel,durantelds,erocetin,factagard,felexin,ibilex,ibrexin,inphalex,kefalospes,keflet,keflex,kefolan,keforal,keftab,kekrinal,kidolex,lafarine,larixin,lenocef,lexibiotico,lonflex,lopilexin,madlexin,mamalexin,mamlexin,medoxine,neokef,neolexina,novolexin,optocef,oracef,oriphex,oroxin,ortisporina,ospexin,palitrex,panixinedisperdose,pectril,pyassan,roceph,rocephdistab,sanaxin,sartosona,sencephalin,sepexin,servispor,sialexin,sinthecillin,sporicef,sporidex,syncle,synecl,tepaxin,tokiolexin,uphalexin,voxxim,winlex,zozarine</t>
         </is>
       </c>
       <c r="J55">
@@ -4192,7 +4192,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>atirin,cefamezin,cefamezine,cefazina,cefazolinacid,cefazolina,cefazoline,cefazolinum,cephamezine,cephazolidin,cephazolin,cephazoline,elzogram,firmacef,kefzol,liviclina,totacef</t>
+          <t>atirin,cefamezin,cefamezine,cefazina,cefazolina,cefazolinacid,cefazoline,cefazolinum,cephamezine,cephazolidin,cephazolin,cephazoline,elzogram,firmacef,kefzol,liviclina,totacef</t>
         </is>
       </c>
       <c r="J62" t="e">
@@ -4659,7 +4659,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Other antibacterials</t>
+          <t>Cephalosporins (4th gen.)</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -4779,7 +4779,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Beta-lactams/penicillins</t>
+          <t>Cephalosporins (4th gen.)</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -4895,7 +4895,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Other antibacterials</t>
+          <t>Cephalosporins (4th gen.)</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -5968,7 +5968,7 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>cefotaxim,cefotaximhikma,cefotaxima,cefotaximaacid,cefotaximeacid,cefotaximum,cephotaxime,claforan,omnatax</t>
+          <t>cefotaxim,cefotaxima,cefotaximaacid,cefotaximeacid,cefotaximhikma,cefotaximum,cephotaxime,claforan,omnatax</t>
         </is>
       </c>
       <c r="J91" t="e">
@@ -6762,7 +6762,7 @@
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>cefpodoximacid,cefpodoxima,cefpodoximeacid,cefpodoximum,epoxim</t>
+          <t>cefpodoxima,cefpodoximacid,cefpodoximeacid,cefpodoximum,epoxim</t>
         </is>
       </c>
       <c r="J104">
@@ -7736,7 +7736,7 @@
       </c>
       <c r="I120" t="inlineStr">
         <is>
-          <t>ceftem,ceftibutendihydrate,ceftibutenhydrate,ceftibutene,ceftibuteno,ceftibutenum,ceftibutin,cephem,ceprifran,isocef,keimax</t>
+          <t>ceftem,ceftibutendihydrate,ceftibutene,ceftibutenhydrate,ceftibuteno,ceftibutenum,ceftibutin,cephem,ceprifran,isocef,keimax</t>
         </is>
       </c>
       <c r="J120">
@@ -8476,7 +8476,7 @@
       </c>
       <c r="I132" t="inlineStr">
         <is>
-          <t>cefuzonamsodium,cefuzoname,cefuzonamum</t>
+          <t>cefuzoname,cefuzonamsodium,cefuzonamum</t>
         </is>
       </c>
       <c r="J132" t="e">
@@ -8662,7 +8662,7 @@
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>alficetyn,ambofen,amphenicol,amphicol,amseclor,anacetin,aquamycetin,austracil,austracol,biocetin,biophenicol,catilan,chloramex,chemiceticol,chemicetin,chemicetina,chlomin,chlomycol,chloramfenikol,chloramficin,chloramfilin,chloramphenicole,chloramphenicolum,chloramsaar,chlorasol,chlorbiotic,chloricol,chlormycetinr,chlornitromycin,chloroamphenicol,chlorocaps,chlorocid,chlorocids,chlorocide,chlorocidinc,chlorocidinctetran,chlorocin,chlorocol,chlorofair,chlorojectl,chloromax,chloromycetin,chloromycetny,chloromyxin,chloronitrin,chloroptic,chloropticsop,chlorovules,chlorsig,cidocetine,ciplamycetin,cloramfen,cloramfenicol,cloramfenicolo,cloramficin,cloramical,cloramicol,cloramidina,cloranfenicol,cloroamfenicolo,clorocyn,cloromisan,cloromissan,clorosintex,comycetin,cylphenicol,desphen,detreomycin,detreomycine,dextromycetin,doctamicina,duphenicol,econochlor,embacetin,emetren,enicol,enteromycetin,erbaplast,ertilen,farmicetina,fenicol,globenicol,glorous,gloveticol,halcetin,halomycetin,hortfenicol,interomycetine,intramycetin,intramyctin,isicetin,ismicetina,isophenicol,isoptofenicol,juvamycetin,kamaver,kemicetina,kemicetine,kloramfenikol,klorita,klorocids,laevomycetinum,leukamycin,leukomyan,leukomycin,levocin,levomicetina,levomitsetin,levomycetin,levoplast,levosin,levovetin,loromicetina,loromisan,loromisin,mastiphen,mediamycetine,medichol,micloretin,micochlorine,micoclorina,microcetina,mychel,mycinol,myclocin,mycochlorin,myscel,normimycinv,novochlorocap,novomycetin,novophenicol,ocuphenicol,oftalent,oleomycetin,opclor,opelor,ophthochlor,ophthocort,ophtochlor,optomycin,otachron,otophen,pantovernil,paraxin,pentamycetin,quemicetina,rivomycin,romphenil,ronfenil,ronphenil,septicol,sificetina,sintomicetin,sintomicetina,sintomicetiner,snophenicol,soluthor,stanomycetin,synthomycetin,synthomycetine,synthomycine,syntomycin,tevcocin,tevcosin,tifomycin,tifomycine,tiromycetin,treomicetina,tyfomycine,unimycetin,veticol,viceton</t>
+          <t>alficetyn,ambofen,amphenicol,amphicol,amseclor,anacetin,aquamycetin,austracil,austracol,biocetin,biophenicol,catilan,chemiceticol,chemicetin,chemicetina,chlomin,chlomycol,chloramex,chloramfenikol,chloramficin,chloramfilin,chloramphenicole,chloramphenicolum,chloramsaar,chlorasol,chlorbiotic,chloricol,chlormycetinr,chlornitromycin,chloroamphenicol,chlorocaps,chlorocid,chlorocide,chlorocidinc,chlorocidinctetran,chlorocids,chlorocin,chlorocol,chlorofair,chlorojectl,chloromax,chloromycetin,chloromycetny,chloromyxin,chloronitrin,chloroptic,chloropticsop,chlorovules,chlorsig,cidocetine,ciplamycetin,cloramfen,cloramfenicol,cloramfenicolo,cloramficin,cloramical,cloramicol,cloramidina,cloranfenicol,cloroamfenicolo,clorocyn,cloromisan,cloromissan,clorosintex,comycetin,cylphenicol,desphen,detreomycin,detreomycine,dextromycetin,doctamicina,duphenicol,econochlor,embacetin,emetren,enicol,enteromycetin,erbaplast,ertilen,farmicetina,fenicol,globenicol,glorous,gloveticol,halcetin,halomycetin,hortfenicol,interomycetine,intramycetin,intramyctin,isicetin,ismicetina,isophenicol,isoptofenicol,juvamycetin,kamaver,kemicetina,kemicetine,kloramfenikol,klorita,klorocids,laevomycetinum,leukamycin,leukomyan,leukomycin,levocin,levomicetina,levomitsetin,levomycetin,levoplast,levosin,levovetin,loromicetina,loromisan,loromisin,mastiphen,mediamycetine,medichol,micloretin,micochlorine,micoclorina,microcetina,mychel,mycinol,myclocin,mycochlorin,myscel,normimycinv,novochlorocap,novomycetin,novophenicol,ocuphenicol,oftalent,oleomycetin,opclor,opelor,ophthochlor,ophthocort,ophtochlor,optomycin,otachron,otophen,pantovernil,paraxin,pentamycetin,quemicetina,rivomycin,romphenil,ronfenil,ronphenil,septicol,sificetina,sintomicetin,sintomicetina,sintomicetiner,snophenicol,soluthor,stanomycetin,synthomycetin,synthomycetine,synthomycine,syntomycin,tevcocin,tevcosin,tifomycin,tifomycine,tiromycetin,treomicetina,tyfomycine,unimycetin,veticol,viceton</t>
         </is>
       </c>
       <c r="J135">
@@ -8976,7 +8976,7 @@
       </c>
       <c r="I140" t="inlineStr">
         <is>
-          <t>alconcilox,auripro,bacquinor,baflox,baycip,bernoflox,cetraxal,ciflox,cifloxin,ciloxan,ciplus,ciprecu,ciprine,ciprinol,ciproiv,ciproxl,ciproxr,ciprobay,ciprobayuro,ciprocinol,ciprodar,ciproflox,ciprofloxacina,ciprofloxacine,ciprofloxacino,ciprofloxacinum,ciprogis,ciprolin,ciprolon,cipromycin,ciproquinol,ciprowin,ciproxan,ciproxin,ciproxina,ciproxine,ciriax,citopcin,corsacin,cyprobay,fimoflox,flociprin,ipiflox,italnik,linhaliq,otiprio,probiox,proflaxin,quinolid,quintor,rancif,roxytal,septicide,sophixinofteno,spitacin,superocin,velmonit,velomonit,zumaflox</t>
+          <t>alconcilox,auripro,bacquinor,baflox,baycip,bernoflox,cetraxal,ciflox,cifloxin,ciloxan,ciplus,ciprecu,ciprine,ciprinol,ciprobay,ciprobayuro,ciprocinol,ciprodar,ciproflox,ciprofloxacina,ciprofloxacine,ciprofloxacino,ciprofloxacinum,ciprogis,ciproiv,ciprolin,ciprolon,cipromycin,ciproquinol,ciprowin,ciproxan,ciproxin,ciproxina,ciproxine,ciproxl,ciproxr,ciriax,citopcin,corsacin,cyprobay,fimoflox,flociprin,ipiflox,italnik,linhaliq,otiprio,probiox,proflaxin,quinolid,quintor,rancif,roxytal,septicide,sophixinofteno,spitacin,superocin,velmonit,velomonit,zumaflox</t>
         </is>
       </c>
       <c r="J140">
@@ -9784,7 +9784,7 @@
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>canesten,canestencream,canestensolution,canestene,canestine,canifug,chlotrimazole,cimitidine,clomatin,clotrimaderm,clotrimadermcream,clotrimazol,clotrimazolum,cutistad,desamixf,diphenylmethane,empecid,esparol,femcare,gynelotrimin,jidesheng,kanesten,klotrimazole,lotrimax,lotrimin,lotriminaf,lotriminafcream,lotriminaflotion,lotriminafsolution,lotrimincream,lotriminlotion,lotriminsolution,monobaycuten,mycelax,mycelex,mycelexcream,mycelexg,mycelexotc,mycelexsolution,mycelextroches,mycelextwinpack,myclocream,myclosolution,myclospraysolution,mycofug,mycosporin,mykosporin,nalbix,otomax,pedisafe,rimazole,stiemazol,tibatin,trimysten,trivagizole,veltrim</t>
+          <t>canesten,canestencream,canestene,canestensolution,canestine,canifug,chlotrimazole,cimitidine,clomatin,clotrimaderm,clotrimadermcream,clotrimazol,clotrimazolum,cutistad,desamixf,diphenylmethane,empecid,esparol,femcare,gynelotrimin,jidesheng,kanesten,klotrimazole,lotrimax,lotrimin,lotriminaf,lotriminafcream,lotriminaflotion,lotriminafsolution,lotrimincream,lotriminlotion,lotriminsolution,monobaycuten,mycelax,mycelex,mycelexcream,mycelexg,mycelexotc,mycelexsolution,mycelextroches,mycelextwinpack,myclocream,myclosolution,myclospraysolution,mycofug,mycosporin,mykosporin,nalbix,otomax,pedisafe,rimazole,stiemazol,tibatin,trimysten,trivagizole,veltrim</t>
         </is>
       </c>
       <c r="J153" t="e">
@@ -9846,7 +9846,7 @@
       </c>
       <c r="I154" t="inlineStr">
         <is>
-          <t>chloroxacillin,clossacillina,cloxacilina,cloxacillinsodium,cloxacilline,cloxacillinna,cloxacillinum,cloxapen,methocillins,orbenin,syntarpen,tegopen</t>
+          <t>chloroxacillin,clossacillina,cloxacilina,cloxacilline,cloxacillinna,cloxacillinsodium,cloxacillinum,cloxapen,methocillins,orbenin,syntarpen,tegopen</t>
         </is>
       </c>
       <c r="J154">
@@ -10222,7 +10222,7 @@
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>aczone,aralditeht,atrisone,avlosulfon,avlosulfone,avlosulphone,avsulfor,bissulfone,bissulphone,croysulfone,croysulphone,dapson,dapsona,dapsonum,disulfone,diaphenylsulfone,diaphenylsulfon,diaphenylsulphon,diaphenylsulphone,dimitone,diphenasone,diphone,disulone,disulphone,dubronax,dubronaz,dumitone,eporal,metabolitec,novophone,protogen,servidapson,slphadione,sulfadione,sulfona,sulfoneucb,sulfonyldianiline,sulphadione,sulphonyldianiline,sumicures,tarimyl,udolac</t>
+          <t>aczone,aralditeht,atrisone,avlosulfon,avlosulfone,avlosulphone,avsulfor,bissulfone,bissulphone,croysulfone,croysulphone,dapson,dapsona,dapsonum,diaphenylsulfon,diaphenylsulfone,diaphenylsulphon,diaphenylsulphone,dimitone,diphenasone,diphone,disulfone,disulone,disulphone,dubronax,dubronaz,dumitone,eporal,metabolitec,novophone,protogen,servidapson,slphadione,sulfadione,sulfona,sulfoneucb,sulfonyldianiline,sulphadione,sulphonyldianiline,sumicures,tarimyl,udolac</t>
         </is>
       </c>
       <c r="J160">
@@ -10540,7 +10540,7 @@
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>debecacin,dibekacinsulfate,dibekacina,dibekacine,dibekacinum,dideoxykanamycinb,kappati,orbicin,panamicin</t>
+          <t>debecacin,dibekacina,dibekacine,dibekacinsulfate,dibekacinum,dideoxykanamycinb,kappati,orbicin,panamicin</t>
         </is>
       </c>
       <c r="J165" t="e">
@@ -10604,7 +10604,7 @@
       </c>
       <c r="I166" t="inlineStr">
         <is>
-          <t>dichloroxacillin,diclossacillina,dicloxaciclin,dicloxacilin,dicloxacilina,dicloxacillinsodium,dicloxacillina,dicloxacilline,dicloxacillinum,dicloxacycline,dycill,dynapen,maclicine,nmdicloxacillin,pathocil</t>
+          <t>dichloroxacillin,diclossacillina,dicloxaciclin,dicloxacilin,dicloxacilina,dicloxacillina,dicloxacilline,dicloxacillinsodium,dicloxacillinum,dicloxacycline,dycill,dynapen,maclicine,nmdicloxacillin,pathocil</t>
         </is>
       </c>
       <c r="J166">
@@ -10856,7 +10856,7 @@
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>atridox,azudoxat,deoxymykoin,dossiciclina,doxcyclineanhydrous,doxiciclina,doxirobe,doxitard,doxivetin,doxycen,doxychel,doxycin,doxycyclin,doxycyclinecalcium,doxycyclinehyclate,doxycyclinum,doxylin,doxysol,doxytec,doxytetracycline,hydramycin,investin,jenacyclin,liviatin,monodox,oracea,periostat,ronaxan,spanor,supracyclin,vibramycin,vibramycinnovum,vibramycine,vibravenos,zenavod</t>
+          <t>atridox,azudoxat,deoxymykoin,dossiciclina,doxcyclineanhydrous,doxiciclina,doxirobe,doxitard,doxivetin,doxycen,doxychel,doxycin,doxycyclin,doxycyclinecalcium,doxycyclinehyclate,doxycyclinum,doxylin,doxysol,doxytec,doxytetracycline,hydramycin,investin,jenacyclin,liviatin,monodox,oracea,periostat,ronaxan,spanor,supracyclin,vibramycin,vibramycine,vibramycinnovum,vibravenos,zenavod</t>
         </is>
       </c>
       <c r="J170">
@@ -11534,7 +11534,7 @@
       </c>
       <c r="I181" t="inlineStr">
         <is>
-          <t>abboticin,abomacetin,acneryne,acnesol,aknecordeslosung,aknedermerygel,aknemycin,austrias,benzamycin,bristamycin,derimer,deripil,dotycin,dumotrycin,emuvin,emycin,endoeritrin,erecin,erisone,eritomicina,eritrocina,eritromicina,ermycin,eryacne,eryacnen,erycsprinkles,erycen,erycette,erycin,erycinum,eryderm,erydermer,erygel,eryhexal,erymax,erymed,erypar,erysafe,erytab,erythrocin,erythrocinstearate,erythroderm,erythrogran,erythroguent,erythromid,erythromycina,erythromycinbase,erythromycinlactate,erythromycine,erythromycines,erythromycinum,erytop,erytrociclin,ilocaps,ilosone,iloticina,ilotycin,ilotycingluceptate,ilotycints,inderm,indermgel,indermretcin,latotryd,lederpax,mephamycin,mercina,oftamolets,paediathrocin,pantoderm,pantodrin,pantomicina,pcedispertab,pharyngocin,primacine,propiocine,proterytrin,retcin,robimycin,romycin,sansac,skidgele,staticin,stiemicyn,stiemycin,theramycinz,tiloryth,tiprocin,torlamicina,udimaerygel,wyamycins</t>
+          <t>abboticin,abomacetin,acneryne,acnesol,aknecordeslosung,aknedermerygel,aknemycin,austrias,benzamycin,bristamycin,derimer,deripil,dotycin,dumotrycin,emuvin,emycin,endoeritrin,erecin,erisone,eritomicina,eritrocina,eritromicina,ermycin,eryacne,eryacnen,erycen,erycette,erycin,erycinum,erycsprinkles,eryderm,erydermer,erygel,eryhexal,erymax,erymed,erypar,erysafe,erytab,erythrocin,erythrocinstearate,erythroderm,erythrogran,erythroguent,erythromid,erythromycina,erythromycinbase,erythromycine,erythromycines,erythromycinlactate,erythromycinum,erytop,erytrociclin,ilocaps,ilosone,iloticina,ilotycin,ilotycingluceptate,ilotycints,inderm,indermgel,indermretcin,latotryd,lederpax,mephamycin,mercina,oftamolets,paediathrocin,pantoderm,pantodrin,pantomicina,pcedispertab,pharyngocin,primacine,propiocine,proterytrin,retcin,robimycin,romycin,sansac,skidgele,staticin,stiemicyn,stiemycin,theramycinz,tiloryth,tiprocin,torlamicina,udimaerygel,wyamycins</t>
         </is>
       </c>
       <c r="J181">
@@ -12714,7 +12714,7 @@
       </c>
       <c r="I200" t="inlineStr">
         <is>
-          <t>calciumfosfomycin,fosfocina,fosfomicin,fosfomicina,fosfomycinsodium,fosfomycine,fosfomycinum,fosfonomycin,infectophos,monuril,monurol,phosphonemycin,phosphonomycin,veramina</t>
+          <t>calciumfosfomycin,fosfocina,fosfomicin,fosfomicina,fosfomycine,fosfomycinsodium,fosfomycinum,fosfonomycin,infectophos,monuril,monurol,phosphonemycin,phosphonomycin,veramina</t>
         </is>
       </c>
       <c r="J200">
@@ -12834,7 +12834,7 @@
       </c>
       <c r="I202" t="inlineStr">
         <is>
-          <t>actilin,actiline,antibiotique,bycomycin,dekamyciniii,endomixin,enterfram,fradiomycin,fradiomycinb,fradiomycinum,framicetina,framidal,framycetinsulfate,framycetine,framycetinum,framycin,framygen,francetin,fraquinol,jernadex,myacine,myacyne,mycerin,mycifradin,neobrettin,neolate,neomas,neomcin,neomicina,neomin,neomycinb,neomycinbsulfate,neomycinsolution,neomycinsulfate,neomycinsulphate,neomycine,neomycinum,nivemycin,pimavecort,soframycin,soframycine,tuttomycin,vonamycin,vonamycinpowderv</t>
+          <t>actilin,actiline,antibiotique,bycomycin,dekamyciniii,endomixin,enterfram,fradiomycin,fradiomycinb,fradiomycinum,framicetina,framidal,framycetine,framycetinsulfate,framycetinum,framycin,framygen,francetin,fraquinol,jernadex,myacine,myacyne,mycerin,mycifradin,neobrettin,neolate,neomas,neomcin,neomicina,neomin,neomycinb,neomycinbsulfate,neomycine,neomycinsolution,neomycinsulfate,neomycinsulphate,neomycinum,nivemycin,pimavecort,soframycin,soframycine,tuttomycin,vonamycin,vonamycinpowderv</t>
         </is>
       </c>
       <c r="J202" t="e">
@@ -13202,7 +13202,7 @@
       </c>
       <c r="I208" t="inlineStr">
         <is>
-          <t>gatiflo,gatifloxacinhydrate,gatifloxacine,gatifloxcin,gatilox,gatiquin,gatispan,tequin,tequinandzymar,zymaxid</t>
+          <t>gatiflo,gatifloxacine,gatifloxacinhydrate,gatifloxcin,gatilox,gatiquin,gatispan,tequin,tequinandzymar,zymaxid</t>
         </is>
       </c>
       <c r="J208">
@@ -13574,7 +13574,7 @@
       </c>
       <c r="I214" t="inlineStr">
         <is>
-          <t>amudane,curlingfactor,delmofulvina,fulcin,fulcine,fulvicangrisactin,fulvicin,fulvicinbolus,fulvidex,fulvina,fulvinil,fulvistatin,fungivin,greosin,gresfeed,gricin,grifulin,grifulvin,grifulvinv,grisactin,grisactinultra,grisactinv,griscofulvin,griseostatin,grisefuline,griseo,griseoflulvin,griseofulvinforte,griseofulvina,griseofulvine,griseofulvinum,griseomix,grisetin,grisofulvin,grisovin,grisovinfp,grizeofulvin,grysio,guservin,lamoryl,likuden,likunden,murfulvin,poncyl,spirofulvin,sporostatinxan,xuanjing</t>
+          <t>amudane,curlingfactor,delmofulvina,fulcin,fulcine,fulvicangrisactin,fulvicin,fulvicinbolus,fulvidex,fulvina,fulvinil,fulvistatin,fungivin,greosin,gresfeed,gricin,grifulin,grifulvin,grifulvinv,grisactin,grisactinultra,grisactinv,griscofulvin,grisefuline,griseo,griseoflulvin,griseofulvina,griseofulvine,griseofulvinforte,griseofulvinum,griseomix,griseostatin,grisetin,grisofulvin,grisovin,grisovinfp,grizeofulvin,grysio,guservin,lamoryl,likuden,likunden,murfulvin,poncyl,spirofulvin,sporostatinxan,xuanjing</t>
         </is>
       </c>
       <c r="J214">
@@ -13996,7 +13996,7 @@
       </c>
       <c r="I221" t="inlineStr">
         <is>
-          <t>imipemide,imipenemanhydrous,imipenemhydrate,imipenemcilastatin,imipenemum,imipenen,primaxin,recarbrio,tienamycin</t>
+          <t>imipemide,imipenemanhydrous,imipenemcilastatin,imipenemhydrate,imipenemum,imipenen,primaxin,recarbrio,tienamycin</t>
         </is>
       </c>
       <c r="J221" t="e">
@@ -14366,7 +14366,7 @@
       </c>
       <c r="I227" t="inlineStr">
         <is>
-          <t>abdizide,andrazide,anidrasona,antimicina,antituberkulosum,armacide,armazid,armazide,atcotibine,aztisoniazid,azuren,bacillin,cemidon,chemiazid,chemidon,continazine,cortinazine,cotinazin,cotinizin,defonin,dianicotyl,dibutin,diforin,dinacrin,ditubin,ebidene,eralon,ertuban,eutizon,evalon,fetefu,fimalene,hidrasonil,hidranizil,hidrulta,hidrun,hycozid,hydrazid,hydrazide,hyozid,iai,idrazil,inizid,ipcazide,iscotin,isidrina,ismazide,isobicina,isocid,isocidene,isocotin,isohydrazide,isokin,isolyn,isonerit,isonex,isoniacid,isoniazidsa,isoniazida,isoniazide,isoniazidum,isonicazide,isonicid,isonico,isonicotan,isonicotil,isonicotinhydrazid,isonicotinohydrazide,isonide,isonidrin,isonikazid,isonilex,isonin,isonindon,isonirit,isoniton,isonizida,isonizide,isotamine,isotebe,isotebezid,isotinyl,isozid,isozide,isozyd,laniazid,laniozid,lanizid,mayambutol,mybasan,neoteben,neoxin,neumandin,niadrin,nicazide,nicetal,nicizina,niconyl,nicotibina,nicotibine,nicotisan,nicozide,nidaton,nidrazid,nikozid,niplen,nitadon,niteban,nydrazid,nyscozid,pelazid,percin,phthisen,pycazide,pyreazid,pyricidin,pyridicin,pyrizidin,raumanon,razide,retozide,rifater,rimicid,rimifon,rimiphone,rimitsid,robiselin,robisellin,roxifen,sanohidrazina,sauterazid,sauterzid,stanozide,tebecid,tebenic,tebexin,tebilon,teebaconin,tekazin,tibazide,tibemid,tibiazide,tibinide,tibison,tibivis,tibizide,tibusan,tisiodrazida,tizide,tubazid,tubazide,tubeco,tubecotubercid,tuberian,tubicon,tubilysin,tubizid,tubomel,unicocyde,unicozyde,vazadrine,vederon,zidafimia,zinadon,zonazide</t>
+          <t>abdizide,andrazide,anidrasona,antimicina,antituberkulosum,armacide,armazid,armazide,atcotibine,aztisoniazid,azuren,bacillin,cemidon,chemiazid,chemidon,continazine,cortinazine,cotinazin,cotinizin,defonin,dianicotyl,dibutin,diforin,dinacrin,ditubin,ebidene,eralon,ertuban,eutizon,evalon,fetefu,fimalene,hidranizil,hidrasonil,hidrulta,hidrun,hycozid,hydrazid,hydrazide,hyozid,iai,idrazil,inizid,ipcazide,iscotin,isidrina,ismazide,isobicina,isocid,isocidene,isocotin,isohydrazide,isokin,isolyn,isonerit,isonex,isoniacid,isoniazida,isoniazide,isoniazidsa,isoniazidum,isonicazide,isonicid,isonico,isonicotan,isonicotil,isonicotinhydrazid,isonicotinohydrazide,isonide,isonidrin,isonikazid,isonilex,isonin,isonindon,isonirit,isoniton,isonizida,isonizide,isotamine,isotebe,isotebezid,isotinyl,isozid,isozide,isozyd,laniazid,laniozid,lanizid,mayambutol,mybasan,neoteben,neoxin,neumandin,niadrin,nicazide,nicetal,nicizina,niconyl,nicotibina,nicotibine,nicotisan,nicozide,nidaton,nidrazid,nikozid,niplen,nitadon,niteban,nydrazid,nyscozid,pelazid,percin,phthisen,pycazide,pyreazid,pyricidin,pyridicin,pyrizidin,raumanon,razide,retozide,rifater,rimicid,rimifon,rimiphone,rimitsid,robiselin,robisellin,roxifen,sanohidrazina,sauterazid,sauterzid,stanozide,tebecid,tebenic,tebexin,tebilon,teebaconin,tekazin,tibazide,tibemid,tibiazide,tibinide,tibison,tibivis,tibizide,tibusan,tisiodrazida,tizide,tubazid,tubazide,tubeco,tubecotubercid,tuberian,tubicon,tubilysin,tubizid,tubomel,unicocyde,unicozyde,vazadrine,vederon,zidafimia,zinadon,zonazide</t>
         </is>
       </c>
       <c r="J227">
@@ -14624,7 +14624,7 @@
       </c>
       <c r="I231" t="inlineStr">
         <is>
-          <t>kanamicina,kanamycina,kanamycinbase,kanamycinsulfate,kanamycine,kanamycins,kanamycinum,kantrex,kenamycina,klebcil,liposomalkanamycin</t>
+          <t>kanamicina,kanamycina,kanamycinbase,kanamycine,kanamycins,kanamycinsulfate,kanamycinum,kantrex,kenamycina,klebcil,liposomalkanamycin</t>
         </is>
       </c>
       <c r="J231">
@@ -15168,7 +15168,7 @@
       </c>
       <c r="I240" t="inlineStr">
         <is>
-          <t>lenampicilina,lenampicillinhcl,lenampicilline,lenampicillinum</t>
+          <t>lenampicilina,lenampicilline,lenampicillinhcl,lenampicillinum</t>
         </is>
       </c>
       <c r="J240" t="e">
@@ -15230,7 +15230,7 @@
       </c>
       <c r="I241" t="inlineStr">
         <is>
-          <t>aeroquin,anhydrousofloxacin,cravit,cravithydrate,cravitiv,cravitophthalmic,elequine,floxacin,floxel,fluoroquinolone,iquixhydrate,leroxacin,lesacin,levaquin,levaquinhydrate,levofiexacin,levofloxacinhydrate,levofloxacine,levofloxacino,levofloxacinum,levokacin,levoxacin,mosardal,nofaxin,ofloxcacin,oftaquix,quinsair,quixin,reskuin,tavanic,unibiotic,venaxan,volequin</t>
+          <t>aeroquin,anhydrousofloxacin,cravit,cravithydrate,cravitiv,cravitophthalmic,elequine,floxacin,floxel,fluoroquinolone,iquixhydrate,leroxacin,lesacin,levaquin,levaquinhydrate,levofiexacin,levofloxacine,levofloxacinhydrate,levofloxacino,levofloxacinum,levokacin,levoxacin,mosardal,nofaxin,ofloxcacin,oftaquix,quinsair,quixin,reskuin,tavanic,unibiotic,venaxan,volequin</t>
         </is>
       </c>
       <c r="J241">
@@ -16468,7 +16468,7 @@
       </c>
       <c r="I261" t="inlineStr">
         <is>
-          <t>blomopen,bonopen,celinmicina,elatocilline,fedacilinakapseln,filorex,italcinakapseln,magnipen,metabacterampullen,metambac,metampicilina,metampicillinsodium,metampicillina,metampicilline,metampicillinum,methampicillin,metiskiaampullen,micinovo,micinovoampullen,pangocilin,probiotic,rastomycink,relyothenate,ruticina,rutizina,rutizinaampullen,sedomycin,suvipen,suvipenampullen,tampilenampullen,teonicontrofen,viderpen,viderpin,vioplex</t>
+          <t>blomopen,bonopen,celinmicina,elatocilline,fedacilinakapseln,filorex,italcinakapseln,magnipen,metabacterampullen,metambac,metampicilina,metampicillina,metampicilline,metampicillinsodium,metampicillinum,methampicillin,metiskiaampullen,micinovo,micinovoampullen,pangocilin,probiotic,rastomycink,relyothenate,ruticina,rutizina,rutizinaampullen,sedomycin,suvipen,suvipenampullen,tampilenampullen,teonicontrofen,viderpen,viderpin,vioplex</t>
         </is>
       </c>
       <c r="J261">
@@ -16534,7 +16534,7 @@
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>acetohmt,aminoform,aminoformaldehyde,ammoform,ammonioformaldehyde,antihydral,cystamin,cystex,cystogen,duirexol,ekagomh,esametilentetramina,formamine,formin,hmt,heksak,heraxuts,heterin,hexab,hexaform,hexaloids,hexamethylamine,hexamethylenamine,hexamethyleneamine,hexamethylentetramin,hexamine,hexaminesilver,hexaminesuperfine,hexaminum,hexasan,hexilmethylenamine,mandelamine,metenamina,metenamine,methamin,methenamin,methenaminesilver,methenaminum,metramine,naphthamine,noccelerh,preparationaf,resotropin,sancelerh,sancelerht,silvermethenamine,uramin,uratrine,urisol,uritone,urodeine,urotropin,urotropine,vesaloin,vesalvine,xametrin</t>
+          <t>acetohmt,aminoform,aminoformaldehyde,ammoform,ammonioformaldehyde,antihydral,cystamin,cystex,cystogen,duirexol,ekagomh,esametilentetramina,formamine,formin,heksak,heraxuts,heterin,hexab,hexaform,hexaloids,hexamethylamine,hexamethylenamine,hexamethyleneamine,hexamethylentetramin,hexamine,hexaminesilver,hexaminesuperfine,hexaminum,hexasan,hexilmethylenamine,hmt,mandelamine,metenamina,metenamine,methamin,methenamin,methenaminesilver,methenaminum,metramine,naphthamine,noccelerh,preparationaf,resotropin,sancelerh,sancelerht,silvermethenamine,uramin,uratrine,urisol,uritone,urodeine,urotropin,urotropine,vesaloin,vesalvine,xametrin</t>
         </is>
       </c>
       <c r="J262">
@@ -16778,7 +16778,7 @@
       </c>
       <c r="I266" t="inlineStr">
         <is>
-          <t>acromona,anagiardil,arilin,atrivyl,danizol,deflamon,donnan,efloran,elyzol,entizol,flagemona,flagesol,flagil,flagyl,flagyler,flagyliv,flagylivrtu,flazol,flegyl,florazole,fossyol,giatricol,gineflavir,helidac,mepagyl,meronidal,methronidazole,metric,metrocream,metrogel,metroiv,metrodzhil,metrogyl,metrolag,metrolotion,metrolyl,metromidol,metronidaz,metronidazol,metronidazoleusp,metronidazolo,metronidazolum,metrotop,metrozine,metryl,mexibol,mexibolsilanes,monagyl,monasin,nidagel,nidagyl,noritate,novonidazol,nuvessa,orvagil,polibiotic,protostat,rathimed,rosased,sanatrichom,satric,takimetol,trichazol,trichex,trichocordes,trichobrol,trichocide,trichomol,trichopal,trichopol,tricocet,tricom,tricowasb,trikacide,trikamon,trikhopol,trikojol,trikozol,trimeks,trivazol,vagilen,vagimid,vandazole,vertisal,wagitran,zadstat,zidoval</t>
+          <t>acromona,anagiardil,arilin,atrivyl,danizol,deflamon,donnan,efloran,elyzol,entizol,flagemona,flagesol,flagil,flagyl,flagyler,flagyliv,flagylivrtu,flazol,flegyl,florazole,fossyol,giatricol,gineflavir,helidac,mepagyl,meronidal,methronidazole,metric,metrocream,metrodzhil,metrogel,metrogyl,metroiv,metrolag,metrolotion,metrolyl,metromidol,metronidaz,metronidazol,metronidazoleusp,metronidazolo,metronidazolum,metrotop,metrozine,metryl,mexibol,mexibolsilanes,monagyl,monasin,nidagel,nidagyl,noritate,novonidazol,nuvessa,orvagil,polibiotic,protostat,rathimed,rosased,sanatrichom,satric,takimetol,trichazol,trichex,trichobrol,trichocide,trichocordes,trichomol,trichopal,trichopol,tricocet,tricom,tricowasb,trikacide,trikamon,trikhopol,trikojol,trikozol,trimeks,trivazol,vagilen,vagimid,vandazole,vertisal,wagitran,zadstat,zidoval</t>
         </is>
       </c>
       <c r="J266">
@@ -16844,7 +16844,7 @@
       </c>
       <c r="I267" t="inlineStr">
         <is>
-          <t>mezlin,mezlocilina,mezlocillinacid,mezlocillinsodium,mezlocilline,mezlocillinum,multocillin</t>
+          <t>mezlin,mezlocilina,mezlocillinacid,mezlocilline,mezlocillinsodium,mezlocillinum,multocillin</t>
         </is>
       </c>
       <c r="J267" t="e">
@@ -17764,7 +17764,7 @@
       </c>
       <c r="I282" t="inlineStr">
         <is>
-          <t>nafcilina,nafcillinsodium,nafcilline,nafcillinum,nallpen,naphcillin,unipen</t>
+          <t>nafcilina,nafcilline,nafcillinsodium,nafcillinum,nallpen,naphcillin,unipen</t>
         </is>
       </c>
       <c r="J282" t="e">
@@ -18070,7 +18070,7 @@
       </c>
       <c r="I287" t="inlineStr">
         <is>
-          <t>actilin,actiline,antibiotique,bycomycin,dekamyciniii,endomixin,enterfram,fradiomycin,fradiomycinb,fradiomycinum,framicetina,framidal,framycetinsulfate,framycetine,framycetinum,framycin,framygen,francetin,fraquinol,jernadex,myacine,myacyne,mycerin,mycifradin,neobrettin,neolate,neomas,neomcin,neomicina,neomin,neomycinb,neomycinbsulfate,neomycinsolution,neomycinsulfate,neomycinsulphate,neomycine,neomycinum,nivemycin,pimavecort,soframycin,soframycine,tuttomycin,vonamycin,vonamycinpowderv</t>
+          <t>actilin,actiline,antibiotique,bycomycin,dekamyciniii,endomixin,enterfram,fradiomycin,fradiomycinb,fradiomycinum,framicetina,framidal,framycetine,framycetinsulfate,framycetinum,framycin,framygen,francetin,fraquinol,jernadex,myacine,myacyne,mycerin,mycifradin,neobrettin,neolate,neomas,neomcin,neomicina,neomin,neomycinb,neomycinbsulfate,neomycine,neomycinsolution,neomycinsulfate,neomycinsulphate,neomycinum,nivemycin,pimavecort,soframycin,soframycine,tuttomycin,vonamycin,vonamycinpowderv</t>
         </is>
       </c>
       <c r="J287">
@@ -18136,7 +18136,7 @@
       </c>
       <c r="I288" t="inlineStr">
         <is>
-          <t>netillin,netilmicinsulfate,netilmicina,netilmicine,netilmicinum,netilyn,netira,nettacin,vectacin</t>
+          <t>netillin,netilmicina,netilmicine,netilmicinsulfate,netilmicinum,netilyn,netira,nettacin,vectacin</t>
         </is>
       </c>
       <c r="J288">
@@ -18442,7 +18442,7 @@
       </c>
       <c r="I293" t="inlineStr">
         <is>
-          <t>alfuran,benkfuran,berkfuran,berkfurin,ceduran,chemiofuran,cistofuran,cyantin,cystit,dantafur,fuamed,furabid,furachel,furadantin,furadantinretard,furadantinamc,furadantine,furadantinemc,furadantoin,furadoin,furadoine,furadonin,furadonine,furadoninum,furadontin,furadoxyl,furalan,furaloid,furantoin,furantoina,furatoin,furedan,furina,furobactina,furodantin,furophent,gerofuran,ioussaixoo,ituran,ivadantin,macpac,macrobid,macrodantin,macrodantina,macrofuran,macrofurin,nierofu,nifurantin,nifuretten,nitoin,nitrex,nitrofuradantin,nitrofurantion,nitrofurantoinmacro,nitrofurantoina,nitrofurantoine,nitrofurantoinum,novofuran,orafuran,parfuran,phenurin,piyeloseptyl,siraliden,trantoin,uerineks,urantoin,urizept,urodin,urofuran,urofurin,urolisa,urolong,uvamin,welfurin,zoofurin</t>
+          <t>alfuran,benkfuran,berkfuran,berkfurin,ceduran,chemiofuran,cistofuran,cyantin,cystit,dantafur,fuamed,furabid,furachel,furadantin,furadantinamc,furadantine,furadantinemc,furadantinretard,furadantoin,furadoin,furadoine,furadonin,furadonine,furadoninum,furadontin,furadoxyl,furalan,furaloid,furantoin,furantoina,furatoin,furedan,furina,furobactina,furodantin,furophent,gerofuran,ioussaixoo,ituran,ivadantin,macpac,macrobid,macrodantin,macrodantina,macrofuran,macrofurin,nierofu,nifurantin,nifuretten,nitoin,nitrex,nitrofuradantin,nitrofurantion,nitrofurantoina,nitrofurantoine,nitrofurantoinmacro,nitrofurantoinum,novofuran,orafuran,parfuran,phenurin,piyeloseptyl,siraliden,trantoin,uerineks,urantoin,urizept,urodin,urofuran,urofurin,urolisa,urolong,uvamin,welfurin,zoofurin</t>
         </is>
       </c>
       <c r="J293">
@@ -18928,7 +18928,7 @@
       </c>
       <c r="I301" t="inlineStr">
         <is>
-          <t>biofanal,candexlotion,comycin,diastatin,herniocid,moronal,myconystatin,mycostatin,mycostatinpastilles,mykinac,mykostatyna,nilstat,nistatin,nistatina,nyamyc,nyotran,nyotrantrademark,nystaform,nystan,nystatina,nystating,nystatinhydrate,nystatinlf,nystatine,nystatinum,nystatyna,nystavescent,nystex,nystop,stamycin,terrastatin,zydine</t>
+          <t>biofanal,candexlotion,comycin,diastatin,herniocid,moronal,myconystatin,mycostatin,mycostatinpastilles,mykinac,mykostatyna,nilstat,nistatin,nistatina,nyamyc,nyotran,nyotrantrademark,nystaform,nystan,nystatina,nystatine,nystating,nystatinhydrate,nystatinlf,nystatinum,nystatyna,nystavescent,nystex,nystop,stamycin,terrastatin,zydine</t>
         </is>
       </c>
       <c r="J301">
@@ -18992,7 +18992,7 @@
       </c>
       <c r="I302" t="inlineStr">
         <is>
-          <t>bactocin,danoflox,dextrofloxacin,effexin,exocin,exocine,flobacin,flodemex,flotavid,flovid,floxal,floxil,floxin,floxinotic,floxstat,fugacin,inoflox,kinflocin,kinoxacin,levofloxacinhcl,liflox,loxinter,marfloxacin,medofloxine,mergexin,monoflocet,novecin,nufafloqo,occidal,ocuflox,oflocee,oflocet,oflocin,oflodal,oflodex,oflodura,ofloxacinotic,ofloxacina,ofloxacine,ofloxacino,ofloxacinum,ofloxin,onexacin,operan,orocin,otonil,oxaldin,pharflox,praxin,puiritol,qinolon,quinolon,quotavil,sinflo,tabrin,taravid,tariflox,tarivid,telbit,tructum,urotarivid,viotisone,visiren,zanocin</t>
+          <t>bactocin,danoflox,dextrofloxacin,effexin,exocin,exocine,flobacin,flodemex,flotavid,flovid,floxal,floxil,floxin,floxinotic,floxstat,fugacin,inoflox,kinflocin,kinoxacin,levofloxacinhcl,liflox,loxinter,marfloxacin,medofloxine,mergexin,monoflocet,novecin,nufafloqo,occidal,ocuflox,oflocee,oflocet,oflocin,oflodal,oflodex,oflodura,ofloxacina,ofloxacine,ofloxacino,ofloxacinotic,ofloxacinum,ofloxin,onexacin,operan,orocin,otonil,oxaldin,pharflox,praxin,puiritol,qinolon,quinolon,quotavil,sinflo,tabrin,taravid,tariflox,tarivid,telbit,tructum,urotarivid,viotisone,visiren,zanocin</t>
         </is>
       </c>
       <c r="J302">
@@ -19612,7 +19612,7 @@
       </c>
       <c r="I312" t="inlineStr">
         <is>
-          <t>bactocill,ossacillina,oxacilina,oxacillinsodium,oxacilline,oxacillinum,oxazocillin,oxazocilline,prostaphlin,prostaphlyn,sodiumoxacillin</t>
+          <t>bactocill,ossacillina,oxacilina,oxacilline,oxacillinsodium,oxacillinum,oxazocillin,oxazocilline,prostaphlin,prostaphlyn,sodiumoxacillin</t>
         </is>
       </c>
       <c r="J312">
@@ -19742,7 +19742,7 @@
       </c>
       <c r="I314" t="inlineStr">
         <is>
-          <t>adamycin,berkmycen,biostat,biostatpa,bisolvomycin,dabicycline,dalimycin,embryostat,fanterrin,galsenomycin,geomycin,geotilin,hydroxytetracyclinum,imperacin,lenocycline,macocyn,medamycin,mepatar,oksisyklin,ossitetraciclina,oxacycline,oxitetraciclina,oxitetracyclin,oxitetracycline,oxitetracyclinum,oxydon,oxymycin,oxymykoin,oxypam,oxysteclin,oxyterracin,oxyterracine,oxyterracyne,oxytetracid,oxytetracyclin,oxytetracyclinebase,oxytetracyclinum,proteroxyna,riomitsin,ryomycin,solkaciclina,stecsolin,stevacin,tarocyn,tarosin,teravit,terrafungine,terramitsin,terramycin,terramycinim,terramycine,tetran,unimycin,ursocyclin,ursocycline,vendarcin</t>
+          <t>adamycin,berkmycen,biostat,biostatpa,bisolvomycin,dabicycline,dalimycin,embryostat,fanterrin,galsenomycin,geomycin,geotilin,hydroxytetracyclinum,imperacin,lenocycline,macocyn,medamycin,mepatar,oksisyklin,ossitetraciclina,oxacycline,oxitetraciclina,oxitetracyclin,oxitetracycline,oxitetracyclinum,oxydon,oxymycin,oxymykoin,oxypam,oxysteclin,oxyterracin,oxyterracine,oxyterracyne,oxytetracid,oxytetracyclin,oxytetracyclinebase,oxytetracyclinum,proteroxyna,riomitsin,ryomycin,solkaciclina,stecsolin,stevacin,tarocyn,tarosin,teravit,terrafungine,terramitsin,terramycin,terramycine,terramycinim,tetran,unimycin,ursocyclin,ursocycline,vendarcin</t>
         </is>
       </c>
       <c r="J314">
@@ -19978,7 +19978,7 @@
       </c>
       <c r="I318" t="inlineStr">
         <is>
-          <t>aminosidin,aminosidine,aminosidinei,aminosidinesulfate,amminosidin,crestomycin,estomycin,gabbromicina,gabbromycin,gabromycin,humatin,humycin,hydroxymycin,hydroxymycinsulfate,monomycin,monomycina,neomycine,paramomycin,paramomycinsulfate,paromomicina,paromomycini,paromomycine,paromomycinum,paucimycin,paucimycinum,quintomycinc</t>
+          <t>aminosidin,aminosidine,aminosidinei,aminosidinesulfate,amminosidin,crestomycin,estomycin,gabbromicina,gabbromycin,gabromycin,humatin,humycin,hydroxymycin,hydroxymycinsulfate,monomycin,monomycina,neomycine,paramomycin,paramomycinsulfate,paromomicina,paromomycine,paromomycini,paromomycinum,paucimycin,paucimycinum,quintomycinc</t>
         </is>
       </c>
       <c r="J318">
@@ -20838,7 +20838,7 @@
       </c>
       <c r="I332" t="inlineStr">
         <is>
-          <t>isipen,pentcillin,peperacillin,peracin,piperacilina,piperacillinhydrate,piperacillinna,piperacillinsodium,piperacillina,piperacilline,piperacillinum,pipercillin,pipracil,pipril,tazocin</t>
+          <t>isipen,pentcillin,peperacillin,peracin,piperacilina,piperacillina,piperacilline,piperacillinhydrate,piperacillinna,piperacillinsodium,piperacillinum,pipercillin,pipracil,pipril,tazocin</t>
         </is>
       </c>
       <c r="J332" t="e">
@@ -22196,7 +22196,7 @@
       </c>
       <c r="I354" t="inlineStr">
         <is>
-          <t>aldinamid,aldinamide,braccopiral,corsazinmid,dipimide,eprazin,farmizina,isopas,lynamide,novamid,pezetamid,pharozinamide,piraldina,pirazimida,pirazinamid,pirazinamida,pirazinamide,prazina,pyrafat,pyramide,pyrazide,pyrazinamdie,pyrazinamid,pyrazinamidum,pyrazinecarboxamide,pyrazineamide,pyrizinamide,rifafour,rozide,tebrazid,tebrazio,tisamid,unipyranamide,zinamide,zinastat</t>
+          <t>aldinamid,aldinamide,braccopiral,corsazinmid,dipimide,eprazin,farmizina,isopas,lynamide,novamid,pezetamid,pharozinamide,piraldina,pirazimida,pirazinamid,pirazinamida,pirazinamide,prazina,pyrafat,pyramide,pyrazide,pyrazinamdie,pyrazinamid,pyrazinamidum,pyrazineamide,pyrazinecarboxamide,pyrizinamide,rifafour,rozide,tebrazid,tebrazio,tisamid,unipyranamide,zinamide,zinastat</t>
         </is>
       </c>
       <c r="J354">
@@ -22866,7 +22866,7 @@
       </c>
       <c r="I365" t="inlineStr">
         <is>
-          <t>abrifam,archidyn,arficin,arzide,aztrifampin,benemicin,benemycin,dipicin,doloresum,eremfat,famcin,fenampicin,rifadin,rifadiniv,rifadine,rifagen,rifaldazin,rifaldazine,rifaldin,rifamate,rifamicinamp,rifamor,rifampicinsv,rifampicina,rifampicine,rifampicinum,rifampin,rifamsolin,rifamycinamp,rifapiam,rifaprodin,rifcin,rifinah,rifobac,rifoldin,rifoldine,riforal,rimactan,rimactane,rimactazid,rimactizid,rimazid,rimycin,sinerdol,tubocin</t>
+          <t>abrifam,archidyn,arficin,arzide,aztrifampin,benemicin,benemycin,dipicin,doloresum,eremfat,famcin,fenampicin,rifadin,rifadine,rifadiniv,rifagen,rifaldazin,rifaldazine,rifaldin,rifamate,rifamicinamp,rifamor,rifampicina,rifampicine,rifampicinsv,rifampicinum,rifampin,rifamsolin,rifamycinamp,rifapiam,rifaprodin,rifcin,rifinah,rifobac,rifoldin,rifoldine,riforal,rimactan,rimactane,rimactazid,rimactizid,rimazid,rimycin,sinerdol,tubocin</t>
         </is>
       </c>
       <c r="J365">
@@ -23746,7 +23746,7 @@
       </c>
       <c r="I379" t="inlineStr">
         <is>
-          <t>rufloxacinhcl,rufloxacine,rufloxacino,rufloxacinum</t>
+          <t>rufloxacine,rufloxacinhcl,rufloxacino,rufloxacinum</t>
         </is>
       </c>
       <c r="J379">
@@ -24170,7 +24170,7 @@
       </c>
       <c r="I386" t="inlineStr">
         <is>
-          <t>rickamicin,salvamina,siseptinsulfate,sisomicinsulfate,sisomicina,sisomicine,sisomicinum,sisomin,sisomycin,sissomicin,sizomycin</t>
+          <t>rickamicin,salvamina,siseptinsulfate,sisomicina,sisomicine,sisomicinsulfate,sisomicinum,sisomin,sisomycin,sissomicin,sizomycin</t>
         </is>
       </c>
       <c r="J386" t="e">
@@ -24294,7 +24294,7 @@
       </c>
       <c r="I388" t="inlineStr">
         <is>
-          <t>bactylan,decapasil,lepasen,monopas,nippas,passodium,pamisylsodium,parasalsodium,pasade,pasnal,passodico,salvis,sanipirol,sodiopas,sodiumpas,teebacin,tubersan</t>
+          <t>bactylan,decapasil,lepasen,monopas,nippas,pamisylsodium,parasalsodium,pasade,pasnal,passodico,passodium,salvis,sanipirol,sodiopas,sodiumpas,teebacin,tubersan</t>
         </is>
       </c>
       <c r="J388">
@@ -24736,7 +24736,7 @@
       </c>
       <c r="I395" t="inlineStr">
         <is>
-          <t>agrept,agrimycin,chemform,estreptomicina,neodiestreptopab,strepcen,streptomicina,streptomycina,streptomycinspx,streptomycinsulfate,streptomycine,streptomycinum,streptomyzin,vetstrep</t>
+          <t>agrept,agrimycin,chemform,estreptomicina,neodiestreptopab,strepcen,streptomicina,streptomycina,streptomycine,streptomycinspx,streptomycinsulfate,streptomycinum,streptomyzin,vetstrep</t>
         </is>
       </c>
       <c r="J395" t="e">
@@ -28098,7 +28098,7 @@
       </c>
       <c r="I449" t="inlineStr">
         <is>
-          <t>abramycin,abricycline,achromycin,achromycinv,actisite,agromicina,ambramicina,ambramycin,amycin,biocycline,bristaciclin,bristaciclina,bristacycline,brodspec,cefracycline,centet,ciclibion,copharlan,criseociclina,cyclomycin,cyclopar,cytome,democracin,deschlorobiomycin,dumocyclin,economycin,enterocycline,hostacyclin,lexacycline,limecycline,liquamycin,medocycline,mericycline,micycline,neocycline,oletetrin,omegamycin,orlycycline,panmycin,piracaps,polycycline,polyotic,purocyclina,resteclin,robitet,roviciclina,sigmamycin,solvocin,sumycin,sumycinsyrup,supramycin,sustamycin,tetrabidorganon,tetrabon,tetrachel,tetraciclina,tetracycl,tetracyclin,tetracyclinebase,tetracyclinei,tetracyclineii,tetracyclinehydrate,tetracyclinum,tetracyn,tetradecin,tetrafil,tetramed,tetrasure,tetraverine,tetrazyklin,tetrex,topicycline,tsiklomistsin,tsiklomitsin,veracin,vetacyclinum,vetquamycin</t>
+          <t>abramycin,abricycline,achromycin,achromycinv,actisite,agromicina,ambramicina,ambramycin,amycin,biocycline,bristaciclin,bristaciclina,bristacycline,brodspec,cefracycline,centet,ciclibion,copharlan,criseociclina,cyclomycin,cyclopar,cytome,democracin,deschlorobiomycin,dumocyclin,economycin,enterocycline,hostacyclin,lexacycline,limecycline,liquamycin,medocycline,mericycline,micycline,neocycline,oletetrin,omegamycin,orlycycline,panmycin,piracaps,polycycline,polyotic,purocyclina,resteclin,robitet,roviciclina,sigmamycin,solvocin,sumycin,sumycinsyrup,supramycin,sustamycin,tetrabidorganon,tetrabon,tetrachel,tetraciclina,tetracycl,tetracyclin,tetracyclinebase,tetracyclinehydrate,tetracyclinei,tetracyclineii,tetracyclinum,tetracyn,tetradecin,tetrafil,tetramed,tetrasure,tetraverine,tetrazyklin,tetrex,topicycline,tsiklomistsin,tsiklomitsin,veracin,vetacyclinum,vetquamycin</t>
         </is>
       </c>
       <c r="J449">
@@ -28528,7 +28528,7 @@
       </c>
       <c r="I456" t="inlineStr">
         <is>
-          <t>denagard,thiamutilin,tiamulinpamoate,tiamulina,tiamuline,tiamulinum,tiavetp</t>
+          <t>denagard,thiamutilin,tiamulina,tiamuline,tiamulinpamoate,tiamulinum,tiavetp</t>
         </is>
       </c>
       <c r="J456" t="e">
@@ -28744,25 +28744,25 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>TBQ</t>
-        </is>
-      </c>
-      <c r="B460">
-        <v>65592</v>
+          <t>TMN</t>
+        </is>
+      </c>
+      <c r="B460" t="e">
+        <v>#N/A</v>
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>Tilbroquinol</t>
+          <t>Tigemonam</t>
         </is>
       </c>
       <c r="D460" t="inlineStr">
         <is>
-          <t>Quinolones</t>
+          <t>Monobactams</t>
         </is>
       </c>
       <c r="E460" t="inlineStr">
         <is>
-          <t>P01AA05</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="F460" t="e">
@@ -28778,7 +28778,7 @@
       </c>
       <c r="I460" t="inlineStr">
         <is>
-          <t>tilbroquinolum</t>
+          <t/>
         </is>
       </c>
       <c r="J460" t="e">
@@ -28802,25 +28802,25 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>TIP</t>
+          <t>TBQ</t>
         </is>
       </c>
       <c r="B461">
-        <v>24860548</v>
+        <v>65592</v>
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>Tildipirosin</t>
+          <t>Tilbroquinol</t>
         </is>
       </c>
       <c r="D461" t="inlineStr">
         <is>
-          <t>Macrolides/lincosamides</t>
+          <t>Quinolones</t>
         </is>
       </c>
       <c r="E461" t="inlineStr">
         <is>
-          <t>QJ01FA96</t>
+          <t>P01AA05</t>
         </is>
       </c>
       <c r="F461" t="e">
@@ -28836,7 +28836,7 @@
       </c>
       <c r="I461" t="inlineStr">
         <is>
-          <t>zuprevo</t>
+          <t>tilbroquinolum</t>
         </is>
       </c>
       <c r="J461" t="e">
@@ -28853,22 +28853,22 @@
       </c>
       <c r="N461" t="inlineStr">
         <is>
-          <t>100060-3,88375-1,88377-7</t>
+          <t/>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>TIL</t>
+          <t>TIP</t>
         </is>
       </c>
       <c r="B462">
-        <v>5282521</v>
+        <v>24860548</v>
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>Tilmicosin</t>
+          <t>Tildipirosin</t>
         </is>
       </c>
       <c r="D462" t="inlineStr">
@@ -28878,7 +28878,7 @@
       </c>
       <c r="E462" t="inlineStr">
         <is>
-          <t>QJ01FA91</t>
+          <t>QJ01FA96</t>
         </is>
       </c>
       <c r="F462" t="e">
@@ -28894,7 +28894,7 @@
       </c>
       <c r="I462" t="inlineStr">
         <is>
-          <t>micotil,pulmotil,tilmicosina,tilmicosine,tilmicosinum</t>
+          <t>zuprevo</t>
         </is>
       </c>
       <c r="J462" t="e">
@@ -28911,169 +28911,167 @@
       </c>
       <c r="N462" t="inlineStr">
         <is>
-          <t>35849-9,35850-7,35851-5,87588-0</t>
+          <t>100060-3,88375-1,88377-7</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>TIN</t>
+          <t>TIL</t>
         </is>
       </c>
       <c r="B463">
-        <v>5479</v>
+        <v>5282521</v>
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>Tinidazole</t>
+          <t>Tilmicosin</t>
         </is>
       </c>
       <c r="D463" t="inlineStr">
         <is>
-          <t>Other antibacterials</t>
+          <t>Macrolides/lincosamides</t>
         </is>
       </c>
       <c r="E463" t="inlineStr">
         <is>
-          <t>G01AF21,J01XD02,P01AB02</t>
-        </is>
-      </c>
-      <c r="F463" t="inlineStr">
-        <is>
-          <t>Other antibacterials</t>
-        </is>
-      </c>
-      <c r="G463" t="inlineStr">
-        <is>
-          <t>Imidazole derivatives</t>
-        </is>
+          <t>QJ01FA91</t>
+        </is>
+      </c>
+      <c r="F463" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G463" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H463" t="inlineStr">
         <is>
-          <t>tini</t>
+          <t/>
         </is>
       </c>
       <c r="I463" t="inlineStr">
         <is>
-          <t>amtiba,bioshik,ethylsulfone,fasigin,fasigyn,fasigyntrademark,fasygin,glongyn,haisigyn,pletil,simplotan,simplotantrademark,sorquetan,symplotan,tindamax,tindamaxtrademark,tinidazol,tinidazolum,tricolam,trimonase</t>
-        </is>
-      </c>
-      <c r="J463">
-        <v>2</v>
-      </c>
-      <c r="K463" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="L463">
-        <v>1.5</v>
-      </c>
-      <c r="M463" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
+          <t>micotil,pulmotil,tilmicosina,tilmicosine,tilmicosinum</t>
+        </is>
+      </c>
+      <c r="J463" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K463" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L463" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M463" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N463" t="inlineStr">
         <is>
-          <t>54928-7,55720-7,55721-5,55722-3</t>
+          <t>35849-9,35850-7,35851-5,87588-0</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>TCR</t>
+          <t>TIN</t>
         </is>
       </c>
       <c r="B464">
-        <v>3001386</v>
+        <v>5479</v>
       </c>
       <c r="C464" t="inlineStr">
         <is>
-          <t>Tiocarlide</t>
+          <t>Tinidazole</t>
         </is>
       </c>
       <c r="D464" t="inlineStr">
         <is>
-          <t>Antimycobacterials</t>
+          <t>Other antibacterials</t>
         </is>
       </c>
       <c r="E464" t="inlineStr">
         <is>
-          <t>J04AD02</t>
+          <t>G01AF21,J01XD02,P01AB02</t>
         </is>
       </c>
       <c r="F464" t="inlineStr">
         <is>
-          <t>Drugs for treatment of tuberculosis</t>
+          <t>Other antibacterials</t>
         </is>
       </c>
       <c r="G464" t="inlineStr">
         <is>
-          <t>Thiocarbamide derivatives</t>
+          <t>Imidazole derivatives</t>
         </is>
       </c>
       <c r="H464" t="inlineStr">
         <is>
-          <t/>
+          <t>tini</t>
         </is>
       </c>
       <c r="I464" t="inlineStr">
         <is>
-          <t>amixyl,datanil,disocarban,disoxyl,isoxyl,thiocarlide,tiocarlid,tiocarlida,tiocarlidum</t>
+          <t>amtiba,bioshik,ethylsulfone,fasigin,fasigyn,fasigyntrademark,fasygin,glongyn,haisigyn,pletil,simplotan,simplotantrademark,sorquetan,symplotan,tindamax,tindamaxtrademark,tinidazol,tinidazolum,tricolam,trimonase</t>
         </is>
       </c>
       <c r="J464">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K464" t="inlineStr">
         <is>
           <t>g</t>
         </is>
       </c>
-      <c r="L464" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M464" t="e">
-        <v>#N/A</v>
+      <c r="L464">
+        <v>1.5</v>
+      </c>
+      <c r="M464" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
       </c>
       <c r="N464" t="inlineStr">
         <is>
-          <t/>
+          <t>54928-7,55720-7,55721-5,55722-3</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>TDC</t>
+          <t>TCR</t>
         </is>
       </c>
       <c r="B465">
-        <v>10247721</v>
+        <v>3001386</v>
       </c>
       <c r="C465" t="inlineStr">
         <is>
-          <t>Tiodonium chloride</t>
+          <t>Tiocarlide</t>
         </is>
       </c>
       <c r="D465" t="inlineStr">
         <is>
-          <t>Other antibacterials</t>
+          <t>Antimycobacterials</t>
         </is>
       </c>
       <c r="E465" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F465" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G465" t="e">
-        <v>#N/A</v>
+          <t>J04AD02</t>
+        </is>
+      </c>
+      <c r="F465" t="inlineStr">
+        <is>
+          <t>Drugs for treatment of tuberculosis</t>
+        </is>
+      </c>
+      <c r="G465" t="inlineStr">
+        <is>
+          <t>Thiocarbamide derivatives</t>
+        </is>
       </c>
       <c r="H465" t="inlineStr">
         <is>
@@ -29082,14 +29080,16 @@
       </c>
       <c r="I465" t="inlineStr">
         <is>
-          <t>clorurodetiodonio,tiodoniichloridum,tiodoniumchloride</t>
-        </is>
-      </c>
-      <c r="J465" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K465" t="e">
-        <v>#N/A</v>
+          <t>amixyl,datanil,disocarban,disoxyl,isoxyl,thiocarlide,tiocarlid,tiocarlida,tiocarlidum</t>
+        </is>
+      </c>
+      <c r="J465">
+        <v>7</v>
+      </c>
+      <c r="K465" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
       </c>
       <c r="L465" t="e">
         <v>#N/A</v>
@@ -29106,20 +29106,20 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>TXC</t>
+          <t>TDC</t>
         </is>
       </c>
       <c r="B466">
-        <v>65788</v>
+        <v>10247721</v>
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>Tioxacin</t>
+          <t>Tiodonium chloride</t>
         </is>
       </c>
       <c r="D466" t="inlineStr">
         <is>
-          <t>Quinolones</t>
+          <t>Other antibacterials</t>
         </is>
       </c>
       <c r="E466" t="inlineStr">
@@ -29140,7 +29140,7 @@
       </c>
       <c r="I466" t="inlineStr">
         <is>
-          <t>tioxacine,tioxacino,tioxacinum,tioxicacid</t>
+          <t>clorurodetiodonio,tiodoniichloridum,tiodoniumchloride</t>
         </is>
       </c>
       <c r="J466" t="e">
@@ -29164,20 +29164,20 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>TIZ</t>
+          <t>TXC</t>
         </is>
       </c>
       <c r="B467">
-        <v>394397</v>
+        <v>65788</v>
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>Tizoxanide</t>
+          <t>Tioxacin</t>
         </is>
       </c>
       <c r="D467" t="inlineStr">
         <is>
-          <t>Other antibacterials</t>
+          <t>Quinolones</t>
         </is>
       </c>
       <c r="E467" t="inlineStr">
@@ -29198,7 +29198,7 @@
       </c>
       <c r="I467" t="inlineStr">
         <is>
-          <t>ntzdes</t>
+          <t>tioxacine,tioxacino,tioxacinum,tioxicacid</t>
         </is>
       </c>
       <c r="J467" t="e">
@@ -29215,52 +29215,48 @@
       </c>
       <c r="N467" t="inlineStr">
         <is>
-          <t>73585-2,73607-4,73629-8</t>
+          <t/>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>TOB</t>
+          <t>TIZ</t>
         </is>
       </c>
       <c r="B468">
-        <v>36294</v>
+        <v>394397</v>
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>Tobramycin</t>
+          <t>Tizoxanide</t>
         </is>
       </c>
       <c r="D468" t="inlineStr">
         <is>
-          <t>Aminoglycosides</t>
+          <t>Other antibacterials</t>
         </is>
       </c>
       <c r="E468" t="inlineStr">
         <is>
-          <t>J01GB01,S01AA12</t>
-        </is>
-      </c>
-      <c r="F468" t="inlineStr">
-        <is>
-          <t>Aminoglycoside antibacterials</t>
-        </is>
-      </c>
-      <c r="G468" t="inlineStr">
-        <is>
-          <t>Other aminoglycosides</t>
-        </is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F468" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G468" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H468" t="inlineStr">
         <is>
-          <t>nn,tm,to,tob,tobr</t>
+          <t/>
         </is>
       </c>
       <c r="I468" t="inlineStr">
         <is>
-          <t>bethkis,brulamycin,deoxykanamycinb,distobram,gernebcin,gotabiotic,kitabis,kitabispak,nebcin,nebicin,nebramycin,nebramycinvi,obramycin,sybryx,tenebrimycin,tenemycin,tobacin,tobipodhaler,tobracin,tobradex,tobradistin,tobralex,tobramaxin,tobramicin,tobramicina,tobramitsetin,tobramycetin,tobramycinbase,tobramycinsulfate,tobramycine,tobramycinum,tobrased,tobrasone,tobrex</t>
+          <t>ntzdes</t>
         </is>
       </c>
       <c r="J468" t="e">
@@ -29269,32 +29265,30 @@
       <c r="K468" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L468">
-        <v>0.24</v>
-      </c>
-      <c r="M468" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
+      <c r="L468" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M468" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N468" t="inlineStr">
         <is>
-          <t>101496-8,13584-8,17808-7,18996-9,22750-4,22751-2,22752-0,25227-0,25800-4,31094-6,31095-3,31096-1,35239-3,35670-9,4057-6,4058-4,4059-2,507-4,508-2,509-0,50927-3,510-8,52962-8,59380-6,7055-7,80966-5</t>
+          <t>73585-2,73607-4,73629-8</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>TOH</t>
-        </is>
-      </c>
-      <c r="B469" t="e">
-        <v>#N/A</v>
+          <t>TOB</t>
+        </is>
+      </c>
+      <c r="B469">
+        <v>36294</v>
       </c>
       <c r="C469" t="inlineStr">
         <is>
-          <t>Tobramycin-high</t>
+          <t>Tobramycin</t>
         </is>
       </c>
       <c r="D469" t="inlineStr">
@@ -29304,23 +29298,27 @@
       </c>
       <c r="E469" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F469" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G469" t="e">
-        <v>#N/A</v>
+          <t>J01GB01,S01AA12</t>
+        </is>
+      </c>
+      <c r="F469" t="inlineStr">
+        <is>
+          <t>Aminoglycoside antibacterials</t>
+        </is>
+      </c>
+      <c r="G469" t="inlineStr">
+        <is>
+          <t>Other aminoglycosides</t>
+        </is>
       </c>
       <c r="H469" t="inlineStr">
         <is>
-          <t>tobra high,tobramycin high,tohl</t>
+          <t>nn,tm,to,tob,tobr</t>
         </is>
       </c>
       <c r="I469" t="inlineStr">
         <is>
-          <t/>
+          <t>bethkis,brulamycin,deoxykanamycinb,distobram,gernebcin,gotabiotic,kitabis,kitabispak,nebcin,nebicin,nebramycin,nebramycinvi,obramycin,sybryx,tenebrimycin,tenemycin,tobacin,tobipodhaler,tobracin,tobradex,tobradistin,tobralex,tobramaxin,tobramicin,tobramicina,tobramitsetin,tobramycetin,tobramycinbase,tobramycine,tobramycinsulfate,tobramycinum,tobrased,tobrasone,tobrex</t>
         </is>
       </c>
       <c r="J469" t="e">
@@ -29329,40 +29327,42 @@
       <c r="K469" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L469" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M469" t="e">
-        <v>#N/A</v>
+      <c r="L469">
+        <v>0.24</v>
+      </c>
+      <c r="M469" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
       </c>
       <c r="N469" t="inlineStr">
         <is>
-          <t/>
+          <t>101496-8,13584-8,17808-7,18996-9,22750-4,22751-2,22752-0,25227-0,25800-4,31094-6,31095-3,31096-1,35239-3,35670-9,4057-6,4058-4,4059-2,507-4,508-2,509-0,50927-3,510-8,52962-8,59380-6,7055-7,80966-5</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>TFX</t>
-        </is>
-      </c>
-      <c r="B470">
-        <v>5517</v>
+          <t>TOH</t>
+        </is>
+      </c>
+      <c r="B470" t="e">
+        <v>#N/A</v>
       </c>
       <c r="C470" t="inlineStr">
         <is>
-          <t>Tosufloxacin</t>
+          <t>Tobramycin-high</t>
         </is>
       </c>
       <c r="D470" t="inlineStr">
         <is>
-          <t>Quinolones</t>
+          <t>Aminoglycosides</t>
         </is>
       </c>
       <c r="E470" t="inlineStr">
         <is>
-          <t>J01MA22,S01AE09</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="F470" t="e">
@@ -29373,7 +29373,7 @@
       </c>
       <c r="H470" t="inlineStr">
         <is>
-          <t/>
+          <t>tobra high,tobramycin high,tohl</t>
         </is>
       </c>
       <c r="I470" t="inlineStr">
@@ -29381,13 +29381,11 @@
           <t/>
         </is>
       </c>
-      <c r="J470">
-        <v>0.45</v>
-      </c>
-      <c r="K470" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
+      <c r="J470" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K470" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L470" t="e">
         <v>#N/A</v>
@@ -29397,88 +29395,82 @@
       </c>
       <c r="N470" t="inlineStr">
         <is>
-          <t>100061-1,76146-0</t>
+          <t/>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>TMP</t>
+          <t>TFX</t>
         </is>
       </c>
       <c r="B471">
-        <v>5578</v>
+        <v>5517</v>
       </c>
       <c r="C471" t="inlineStr">
         <is>
-          <t>Trimethoprim</t>
+          <t>Tosufloxacin</t>
         </is>
       </c>
       <c r="D471" t="inlineStr">
         <is>
-          <t>Trimethoprims</t>
+          <t>Quinolones</t>
         </is>
       </c>
       <c r="E471" t="inlineStr">
         <is>
-          <t>J01EA01</t>
-        </is>
-      </c>
-      <c r="F471" t="inlineStr">
-        <is>
-          <t>Sulfonamides and trimethoprim</t>
-        </is>
-      </c>
-      <c r="G471" t="inlineStr">
-        <is>
-          <t>Trimethoprim and derivatives</t>
-        </is>
+          <t>J01MA22,S01AE09</t>
+        </is>
+      </c>
+      <c r="F471" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G471" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H471" t="inlineStr">
         <is>
-          <t>t,tmp,tr,tri,trim,w</t>
+          <t/>
         </is>
       </c>
       <c r="I471" t="inlineStr">
         <is>
-          <t>abaprim,alprim,anitrim,antrima,antrimox,bacdan,bacidal,bacide,bacterial,bacticel,bactifor,bactin,bactoprim,bactramin,bactrim,bencole,bethaprim,biosulten,briscotrim,chemotrin,colizole,colizoleds,conprim,cotrimel,cotrimoxizole,deprim,dosulfin,duocide,esbesul,espectrin,euctrim,exbesul,fermagex,fortrim,idotrim,ikaprim,infectotrimet,instalac,kombinax,lagatrim,lagatrimforte,lastrim,lescot,methoprim,metoprim,monoprim,monotrim,monotrimin,novotrimel,omstat,oraprim,pancidim,polytrim,priloprim,primosept,primsol,proloprim,protrin,purbal,resprim,resprimforte,roubac,roubal,salvatrim,septrinds,septrinforte,septrins,setprin,sinotrim,stopan,streptoplus,sugaprim,sulfamar,sulfamethoprim,sulfoxaprim,sulthrim,sultrex,syraprim,tiempe,tmpsmx,toprim,trimanyl,trimethioprim,trimethopim,trimethoprime,trimethoprimum,trimethopriom,trimetoprim,trimetoprima,trimexazole,trimexol,trimezol,trimogal,trimono,trimopan,trimpex,triprim,trisul,trisulcom,trisulfam,trisural,uretrim,urobactrim,utetrin,velaten,wellcoprim,wellcoprin,xeroprim,zamboprim</t>
+          <t/>
         </is>
       </c>
       <c r="J471">
-        <v>0.4</v>
+        <v>0.45</v>
       </c>
       <c r="K471" t="inlineStr">
         <is>
           <t>g</t>
         </is>
       </c>
-      <c r="L471">
-        <v>0.4</v>
-      </c>
-      <c r="M471" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
+      <c r="L471" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M471" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N471" t="inlineStr">
         <is>
-          <t>101495-0,11005-6,17747-7,18997-7,18998-5,20387-7,23614-1,23631-5,25273-4,32342-8,4079-0,4080-8,4081-6,511-6,512-4,513-2,514-0,515-7,516-5,517-3,518-1,55584-7,7056-5,7057-3,80552-3,80973-1</t>
+          <t>100061-1,76146-0</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>SXT</t>
+          <t>TMP</t>
         </is>
       </c>
       <c r="B472">
-        <v>358641</v>
+        <v>5578</v>
       </c>
       <c r="C472" t="inlineStr">
         <is>
-          <t>Trimethoprim/sulfamethoxazole</t>
+          <t>Trimethoprim</t>
         </is>
       </c>
       <c r="D472" t="inlineStr">
@@ -29488,7 +29480,7 @@
       </c>
       <c r="E472" t="inlineStr">
         <is>
-          <t>J01EE01</t>
+          <t>J01EA01</t>
         </is>
       </c>
       <c r="F472" t="inlineStr">
@@ -29498,88 +29490,90 @@
       </c>
       <c r="G472" t="inlineStr">
         <is>
-          <t>Combinations of sulfonamides and trimethoprim, incl. derivatives</t>
+          <t>Trimethoprim and derivatives</t>
         </is>
       </c>
       <c r="H472" t="inlineStr">
         <is>
-          <t>cot,cotrim,sxt,t/s,tms,trsu,trsx,ts</t>
+          <t>t,tmp,tr,tri,trim,w</t>
         </is>
       </c>
       <c r="I472" t="inlineStr">
         <is>
-          <t>abacin,abactrim,agoprim,alfatrim,aposulfatrim,bacteral,bacterialforte,bactilen,bactiver,bacton,bactoreduct,bactrim,bactrimds,bactrimforte,bactrimpediatric,bactrimel,bactrizol,bactromin,bactropin,baktar,belcomycine,berlocid,bibacrim,biseptol,chemitrim,chemotrim,ciplin,colimycin,colimycinsulphate,colisticin,colistimethate,colistimethatesodium,colistinsulfate,colistinsulphate,colomycin,colymycin,cotribene,cotrimds,cotrimeurho,cotrimholsen,cotrimlut,cotrimaxazol,cotrimazole,cotrimhexal,cotrimoxazol,cotrimoxazolal,cotrimoxazole,cotrimstada,cotriver,dibaprim,drylin,duratrimet,eltrianyl,escoprim,esteprim,eusaprim,fectrim,gantaprim,gantaprin,gantrim,groprim,helveprim,imexim,jenamoxazol,kemoprim,kepinol,kepinolforte,laratrim,linaris,maxtrim,microtrim,microtrimforte,mikrosid,momentol,oecotrim,oriprim,oxaprim,pantoprim,polymyxine,polymyxinesulfate,primazole,promixin,septra,septrads,septragrape,septrim,septrin,servitrim,sigaprim,sigaprin,sulfatrimpediatric,sulfotrim,sulfotrimin,sulmeprimpediatric,sulprim,sumetrolim,supracombin,suprim,tacumil,teleprim,teleprin,thiocuran,totazina,tribakin,trifen,trigonyl,trimesulf,trimethocomp,trimethoprimsulfa,trimetoger,trimexazol,trimforte,trimosulfa,uroplus,uroplusds,uroplusss</t>
-        </is>
-      </c>
-      <c r="J472" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K472" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L472" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M472" t="e">
-        <v>#N/A</v>
+          <t>abaprim,alprim,anitrim,antrima,antrimox,bacdan,bacidal,bacide,bacterial,bacticel,bactifor,bactin,bactoprim,bactramin,bactrim,bencole,bethaprim,biosulten,briscotrim,chemotrin,colizole,colizoleds,conprim,cotrimel,cotrimoxizole,deprim,dosulfin,duocide,esbesul,espectrin,euctrim,exbesul,fermagex,fortrim,idotrim,ikaprim,infectotrimet,instalac,kombinax,lagatrim,lagatrimforte,lastrim,lescot,methoprim,metoprim,monoprim,monotrim,monotrimin,novotrimel,omstat,oraprim,pancidim,polytrim,priloprim,primosept,primsol,proloprim,protrin,purbal,resprim,resprimforte,roubac,roubal,salvatrim,septrinds,septrinforte,septrins,setprin,sinotrim,stopan,streptoplus,sugaprim,sulfamar,sulfamethoprim,sulfoxaprim,sulthrim,sultrex,syraprim,tiempe,tmpsmx,toprim,trimanyl,trimethioprim,trimethopim,trimethoprime,trimethoprimum,trimethopriom,trimetoprim,trimetoprima,trimexazole,trimexol,trimezol,trimogal,trimono,trimopan,trimpex,triprim,trisul,trisulcom,trisulfam,trisural,uretrim,urobactrim,utetrin,velaten,wellcoprim,wellcoprin,xeroprim,zamboprim</t>
+        </is>
+      </c>
+      <c r="J472">
+        <v>0.4</v>
+      </c>
+      <c r="K472" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L472">
+        <v>0.4</v>
+      </c>
+      <c r="M472" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
       </c>
       <c r="N472" t="inlineStr">
         <is>
-          <t>101495-0,18998-5,20387-7,23631-5,25273-4,32342-8,4081-6,515-7,516-5,517-3,518-1,7057-3</t>
+          <t>101495-0,11005-6,17747-7,18997-7,18998-5,20387-7,23614-1,23631-5,25273-4,32342-8,4079-0,4080-8,4081-6,511-6,512-4,513-2,514-0,515-7,516-5,517-3,518-1,55584-7,7056-5,7057-3,80552-3,80973-1</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>TRL</t>
+          <t>SXT</t>
         </is>
       </c>
       <c r="B473">
-        <v>202225</v>
+        <v>358641</v>
       </c>
       <c r="C473" t="inlineStr">
         <is>
-          <t>Troleandomycin</t>
+          <t>Trimethoprim/sulfamethoxazole</t>
         </is>
       </c>
       <c r="D473" t="inlineStr">
         <is>
-          <t>Macrolides/lincosamides</t>
+          <t>Trimethoprims</t>
         </is>
       </c>
       <c r="E473" t="inlineStr">
         <is>
-          <t>J01FA08</t>
+          <t>J01EE01</t>
         </is>
       </c>
       <c r="F473" t="inlineStr">
         <is>
-          <t>Macrolides, lincosamides and streptogramins</t>
+          <t>Sulfonamides and trimethoprim</t>
         </is>
       </c>
       <c r="G473" t="inlineStr">
         <is>
-          <t>Macrolides</t>
+          <t>Combinations of sulfonamides and trimethoprim, incl. derivatives</t>
         </is>
       </c>
       <c r="H473" t="inlineStr">
         <is>
-          <t/>
+          <t>cot,cotrim,sxt,t/s,tms,trsu,trsx,ts</t>
         </is>
       </c>
       <c r="I473" t="inlineStr">
         <is>
-          <t>acetyloleandomycin,aovine,cyclamycin,evramicina,matromicina,matromycint,micotil,oleandocetine,tao,treolmicina,tribiocillina,triocetin,triolan,troleandomicina,troleandomycine,troleandomycinum,viamicina,wytrion</t>
-        </is>
-      </c>
-      <c r="J473">
-        <v>1</v>
-      </c>
-      <c r="K473" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
+          <t>abacin,abactrim,agoprim,alfatrim,aposulfatrim,bacteral,bacterialforte,bactilen,bactiver,bacton,bactoreduct,bactrim,bactrimds,bactrimel,bactrimforte,bactrimpediatric,bactrizol,bactromin,bactropin,baktar,belcomycine,berlocid,bibacrim,biseptol,chemitrim,chemotrim,ciplin,colimycin,colimycinsulphate,colisticin,colistimethate,colistimethatesodium,colistinsulfate,colistinsulphate,colomycin,colymycin,cotribene,cotrimaxazol,cotrimazole,cotrimds,cotrimeurho,cotrimhexal,cotrimholsen,cotrimlut,cotrimoxazol,cotrimoxazolal,cotrimoxazole,cotrimstada,cotriver,dibaprim,drylin,duratrimet,eltrianyl,escoprim,esteprim,eusaprim,fectrim,gantaprim,gantaprin,gantrim,groprim,helveprim,imexim,jenamoxazol,kemoprim,kepinol,kepinolforte,laratrim,linaris,maxtrim,microtrim,microtrimforte,mikrosid,momentol,oecotrim,oriprim,oxaprim,pantoprim,polymyxine,polymyxinesulfate,primazole,promixin,septra,septrads,septragrape,septrim,septrin,servitrim,sigaprim,sigaprin,sulfatrimpediatric,sulfotrim,sulfotrimin,sulmeprimpediatric,sulprim,sumetrolim,supracombin,suprim,tacumil,teleprim,teleprin,thiocuran,totazina,tribakin,trifen,trigonyl,trimesulf,trimethocomp,trimethoprimsulfa,trimetoger,trimexazol,trimforte,trimosulfa,uroplus,uroplusds,uroplusss</t>
+        </is>
+      </c>
+      <c r="J473" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K473" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L473" t="e">
         <v>#N/A</v>
@@ -29589,39 +29583,43 @@
       </c>
       <c r="N473" t="inlineStr">
         <is>
-          <t>18999-3,519-9,520-7,521-5,522-3</t>
+          <t>101495-0,18998-5,20387-7,23631-5,25273-4,32342-8,4081-6,515-7,516-5,517-3,518-1,7057-3</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>TRO</t>
+          <t>TRL</t>
         </is>
       </c>
       <c r="B474">
-        <v>55886</v>
+        <v>202225</v>
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>Trospectomycin</t>
+          <t>Troleandomycin</t>
         </is>
       </c>
       <c r="D474" t="inlineStr">
         <is>
-          <t>Other antibacterials</t>
+          <t>Macrolides/lincosamides</t>
         </is>
       </c>
       <c r="E474" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F474" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G474" t="e">
-        <v>#N/A</v>
+          <t>J01FA08</t>
+        </is>
+      </c>
+      <c r="F474" t="inlineStr">
+        <is>
+          <t>Macrolides, lincosamides and streptogramins</t>
+        </is>
+      </c>
+      <c r="G474" t="inlineStr">
+        <is>
+          <t>Macrolides</t>
+        </is>
       </c>
       <c r="H474" t="inlineStr">
         <is>
@@ -29630,14 +29628,16 @@
       </c>
       <c r="I474" t="inlineStr">
         <is>
-          <t>rubidiumnitrate,trospectinomycin,trospectomicina,trospectomycine,trospectomycinum</t>
-        </is>
-      </c>
-      <c r="J474" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K474" t="e">
-        <v>#N/A</v>
+          <t>acetyloleandomycin,aovine,cyclamycin,evramicina,matromicina,matromycint,micotil,oleandocetine,tao,treolmicina,tribiocillina,triocetin,triolan,troleandomicina,troleandomycine,troleandomycinum,viamicina,wytrion</t>
+        </is>
+      </c>
+      <c r="J474">
+        <v>1</v>
+      </c>
+      <c r="K474" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
       </c>
       <c r="L474" t="e">
         <v>#N/A</v>
@@ -29647,146 +29647,146 @@
       </c>
       <c r="N474" t="inlineStr">
         <is>
-          <t/>
+          <t>18999-3,519-9,520-7,521-5,522-3</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>TVA</t>
+          <t>TRO</t>
         </is>
       </c>
       <c r="B475">
-        <v>62959</v>
+        <v>55886</v>
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>Trovafloxacin</t>
+          <t>Trospectomycin</t>
         </is>
       </c>
       <c r="D475" t="inlineStr">
         <is>
-          <t>Quinolones</t>
+          <t>Other antibacterials</t>
         </is>
       </c>
       <c r="E475" t="inlineStr">
         <is>
-          <t>J01MA13</t>
-        </is>
-      </c>
-      <c r="F475" t="inlineStr">
-        <is>
-          <t>Quinolone antibacterials</t>
-        </is>
-      </c>
-      <c r="G475" t="inlineStr">
-        <is>
-          <t>Fluoroquinolones</t>
-        </is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F475" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G475" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H475" t="inlineStr">
         <is>
-          <t>trov</t>
+          <t/>
         </is>
       </c>
       <c r="I475" t="inlineStr">
         <is>
-          <t>trovan</t>
-        </is>
-      </c>
-      <c r="J475">
-        <v>0.2</v>
-      </c>
-      <c r="K475" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="L475">
-        <v>0.2</v>
-      </c>
-      <c r="M475" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
+          <t>rubidiumnitrate,trospectinomycin,trospectomicina,trospectomycine,trospectomycinum</t>
+        </is>
+      </c>
+      <c r="J475" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K475" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L475" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M475" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N475" t="inlineStr">
         <is>
-          <t>23642-2,23643-0,35855-6,7058-1</t>
+          <t/>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>TUL</t>
+          <t>TVA</t>
         </is>
       </c>
       <c r="B476">
-        <v>9832301</v>
+        <v>62959</v>
       </c>
       <c r="C476" t="inlineStr">
         <is>
-          <t>Tulathromycin</t>
+          <t>Trovafloxacin</t>
         </is>
       </c>
       <c r="D476" t="inlineStr">
         <is>
-          <t>Macrolides/lincosamides</t>
+          <t>Quinolones</t>
         </is>
       </c>
       <c r="E476" t="inlineStr">
         <is>
-          <t>QJ01FA94</t>
-        </is>
-      </c>
-      <c r="F476" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G476" t="e">
-        <v>#N/A</v>
+          <t>J01MA13</t>
+        </is>
+      </c>
+      <c r="F476" t="inlineStr">
+        <is>
+          <t>Quinolone antibacterials</t>
+        </is>
+      </c>
+      <c r="G476" t="inlineStr">
+        <is>
+          <t>Fluoroquinolones</t>
+        </is>
       </c>
       <c r="H476" t="inlineStr">
         <is>
-          <t/>
+          <t>trov</t>
         </is>
       </c>
       <c r="I476" t="inlineStr">
         <is>
-          <t>draxxin,tulathrmycina,tulathromycina</t>
-        </is>
-      </c>
-      <c r="J476" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K476" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L476" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M476" t="e">
-        <v>#N/A</v>
+          <t>trovan</t>
+        </is>
+      </c>
+      <c r="J476">
+        <v>0.2</v>
+      </c>
+      <c r="K476" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L476">
+        <v>0.2</v>
+      </c>
+      <c r="M476" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
       </c>
       <c r="N476" t="inlineStr">
         <is>
-          <t>76149-4,87798-5</t>
+          <t>23642-2,23643-0,35855-6,7058-1</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>TYL</t>
+          <t>TUL</t>
         </is>
       </c>
       <c r="B477">
-        <v>5280440</v>
+        <v>9832301</v>
       </c>
       <c r="C477" t="inlineStr">
         <is>
-          <t>Tylosin</t>
+          <t>Tulathromycin</t>
         </is>
       </c>
       <c r="D477" t="inlineStr">
@@ -29796,7 +29796,7 @@
       </c>
       <c r="E477" t="inlineStr">
         <is>
-          <t>QJ01FA90,QJ51FA90</t>
+          <t>QJ01FA94</t>
         </is>
       </c>
       <c r="F477" t="e">
@@ -29812,7 +29812,7 @@
       </c>
       <c r="I477" t="inlineStr">
         <is>
-          <t>fradizine,tilosina,tylocine,tylosina,tylosine,tylosinum</t>
+          <t>draxxin,tulathrmycina,tulathromycina</t>
         </is>
       </c>
       <c r="J477" t="e">
@@ -29829,22 +29829,22 @@
       </c>
       <c r="N477" t="inlineStr">
         <is>
-          <t>35856-4,35857-2,35858-0,87587-2</t>
+          <t>76149-4,87798-5</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>TYL1</t>
+          <t>TYL</t>
         </is>
       </c>
       <c r="B478">
-        <v>6441094</v>
+        <v>5280440</v>
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>Tylvalosin</t>
+          <t>Tylosin</t>
         </is>
       </c>
       <c r="D478" t="inlineStr">
@@ -29854,7 +29854,7 @@
       </c>
       <c r="E478" t="inlineStr">
         <is>
-          <t>QJ01FA92</t>
+          <t>QJ01FA90,QJ51FA90</t>
         </is>
       </c>
       <c r="F478" t="e">
@@ -29865,12 +29865,12 @@
       </c>
       <c r="H478" t="inlineStr">
         <is>
-          <t>tvn</t>
+          <t/>
         </is>
       </c>
       <c r="I478" t="inlineStr">
         <is>
-          <t/>
+          <t>fradizine,tilosina,tylocine,tylosina,tylosine,tylosinum</t>
         </is>
       </c>
       <c r="J478" t="e">
@@ -29887,32 +29887,32 @@
       </c>
       <c r="N478" t="inlineStr">
         <is>
-          <t>101526-2,87586-4</t>
+          <t>35856-4,35857-2,35858-0,87587-2</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>PRU1</t>
+          <t>TYL1</t>
         </is>
       </c>
       <c r="B479">
-        <v>124225</v>
+        <v>6441094</v>
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>Ulifloxacin (Prulifloxacin)</t>
+          <t>Tylvalosin</t>
         </is>
       </c>
       <c r="D479" t="inlineStr">
         <is>
-          <t>Other antibacterials</t>
+          <t>Macrolides/lincosamides</t>
         </is>
       </c>
       <c r="E479" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>QJ01FA92</t>
         </is>
       </c>
       <c r="F479" t="e">
@@ -29923,12 +29923,12 @@
       </c>
       <c r="H479" t="inlineStr">
         <is>
-          <t/>
+          <t>tvn</t>
         </is>
       </c>
       <c r="I479" t="inlineStr">
         <is>
-          <t>ulifloxacin</t>
+          <t/>
         </is>
       </c>
       <c r="J479" t="e">
@@ -29945,88 +29945,80 @@
       </c>
       <c r="N479" t="inlineStr">
         <is>
-          <t/>
+          <t>101526-2,87586-4</t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>PRU1</t>
         </is>
       </c>
       <c r="B480">
-        <v>14969</v>
+        <v>124225</v>
       </c>
       <c r="C480" t="inlineStr">
         <is>
-          <t>Vancomycin</t>
+          <t>Ulifloxacin (Prulifloxacin)</t>
         </is>
       </c>
       <c r="D480" t="inlineStr">
         <is>
-          <t>Glycopeptides</t>
+          <t>Other antibacterials</t>
         </is>
       </c>
       <c r="E480" t="inlineStr">
         <is>
-          <t>A07AA09,J01XA01,S01AA28</t>
-        </is>
-      </c>
-      <c r="F480" t="inlineStr">
-        <is>
-          <t>Other antibacterials</t>
-        </is>
-      </c>
-      <c r="G480" t="inlineStr">
-        <is>
-          <t>Glycopeptide antibacterials</t>
-        </is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F480" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G480" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H480" t="inlineStr">
         <is>
-          <t>va,van,vanc</t>
+          <t/>
         </is>
       </c>
       <c r="I480" t="inlineStr">
         <is>
-          <t>vancocin,vancocinhcl,vancoled,vancomicina,vancomycinhcl,vancomycine,vancomycinum,vancor,viomycinderivative</t>
-        </is>
-      </c>
-      <c r="J480">
-        <v>2</v>
-      </c>
-      <c r="K480" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="L480">
-        <v>2</v>
-      </c>
-      <c r="M480" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
+          <t>ulifloxacin</t>
+        </is>
+      </c>
+      <c r="J480" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K480" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L480" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M480" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N480" t="inlineStr">
         <is>
-          <t>13586-3,13587-1,19000-9,20578-1,23615-8,25228-8,31012-8,39092-2,39796-8,39797-6,4089-9,4090-7,4091-5,4092-3,50938-0,523-1,524-9,525-6,526-4,59381-4,7059-9,92241-9,97657-1</t>
+          <t/>
         </is>
       </c>
     </row>
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>VAM</t>
-        </is>
-      </c>
-      <c r="B481" t="e">
-        <v>#N/A</v>
+          <t>VAN</t>
+        </is>
+      </c>
+      <c r="B481">
+        <v>14969</v>
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>Vancomycin-macromethod</t>
+          <t>Vancomycin</t>
         </is>
       </c>
       <c r="D481" t="inlineStr">
@@ -30036,60 +30028,68 @@
       </c>
       <c r="E481" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F481" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G481" t="e">
-        <v>#N/A</v>
+          <t>A07AA09,J01XA01,S01AA28</t>
+        </is>
+      </c>
+      <c r="F481" t="inlineStr">
+        <is>
+          <t>Other antibacterials</t>
+        </is>
+      </c>
+      <c r="G481" t="inlineStr">
+        <is>
+          <t>Glycopeptide antibacterials</t>
+        </is>
       </c>
       <c r="H481" t="inlineStr">
         <is>
-          <t/>
+          <t>va,van,vanc</t>
         </is>
       </c>
       <c r="I481" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J481" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K481" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L481" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M481" t="e">
-        <v>#N/A</v>
+          <t>vancocin,vancocinhcl,vancoled,vancomicina,vancomycine,vancomycinhcl,vancomycinum,vancor,viomycinderivative</t>
+        </is>
+      </c>
+      <c r="J481">
+        <v>2</v>
+      </c>
+      <c r="K481" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L481">
+        <v>2</v>
+      </c>
+      <c r="M481" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
       </c>
       <c r="N481" t="inlineStr">
         <is>
-          <t/>
+          <t>13586-3,13587-1,19000-9,20578-1,23615-8,25228-8,31012-8,39092-2,39796-8,39797-6,4089-9,4090-7,4091-5,4092-3,50938-0,523-1,524-9,525-6,526-4,59381-4,7059-9,92241-9,97657-1</t>
         </is>
       </c>
     </row>
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>VIO</t>
-        </is>
-      </c>
-      <c r="B482">
-        <v>135398671</v>
+          <t>VAM</t>
+        </is>
+      </c>
+      <c r="B482" t="e">
+        <v>#N/A</v>
       </c>
       <c r="C482" t="inlineStr">
         <is>
-          <t>Viomycin</t>
+          <t>Vancomycin-macromethod</t>
         </is>
       </c>
       <c r="D482" t="inlineStr">
         <is>
-          <t>Antimycobacterials</t>
+          <t>Glycopeptides</t>
         </is>
       </c>
       <c r="E482" t="inlineStr">
@@ -30110,7 +30110,7 @@
       </c>
       <c r="I482" t="inlineStr">
         <is>
-          <t>celiomycin,florimycin,floromycin,tuberactinomycinb,vinacetina,vioactane,viomicina,viomycine,viomycinum</t>
+          <t/>
         </is>
       </c>
       <c r="J482" t="e">
@@ -30127,27 +30127,27 @@
       </c>
       <c r="N482" t="inlineStr">
         <is>
-          <t>19001-7,23616-6,527-2,528-0,529-8,530-6</t>
+          <t/>
         </is>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>VIR</t>
+          <t>VIO</t>
         </is>
       </c>
       <c r="B483">
-        <v>11979535</v>
+        <v>135398671</v>
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>Virginiamycine</t>
+          <t>Viomycin</t>
         </is>
       </c>
       <c r="D483" t="inlineStr">
         <is>
-          <t>Other antibacterials</t>
+          <t>Antimycobacterials</t>
         </is>
       </c>
       <c r="E483" t="inlineStr">
@@ -30168,7 +30168,7 @@
       </c>
       <c r="I483" t="inlineStr">
         <is>
-          <t>eskalin,eskalinv,micamicina,mikamycin,mikamycine,mikamycinum,ostreogricina,ostreogrycin,ostreogrycine,ostreogrycinum,pristinamicina,pristinamycine,pristinamycinum,pyostacine,stafac,stafytracine,staphylomycin,stapyocine,starfac,streptogramin,vernamycin,virgimycin,virgimycine,virginiamicina,virginiamycin,virginiamycina,virginiamycinum</t>
+          <t>celiomycin,florimycin,floromycin,tuberactinomycinb,vinacetina,vioactane,viomicina,viomycine,viomycinum</t>
         </is>
       </c>
       <c r="J483" t="e">
@@ -30185,150 +30185,146 @@
       </c>
       <c r="N483" t="inlineStr">
         <is>
-          <t/>
+          <t>19001-7,23616-6,527-2,528-0,529-8,530-6</t>
         </is>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>VOR</t>
+          <t>VIR</t>
         </is>
       </c>
       <c r="B484">
-        <v>71616</v>
+        <v>11979535</v>
       </c>
       <c r="C484" t="inlineStr">
         <is>
-          <t>Voriconazole</t>
+          <t>Virginiamycine</t>
         </is>
       </c>
       <c r="D484" t="inlineStr">
         <is>
-          <t>Antifungals/antimycotics</t>
+          <t>Other antibacterials</t>
         </is>
       </c>
       <c r="E484" t="inlineStr">
         <is>
-          <t>J02AC03</t>
-        </is>
-      </c>
-      <c r="F484" t="inlineStr">
-        <is>
-          <t>Antimycotics for systemic use</t>
-        </is>
-      </c>
-      <c r="G484" t="inlineStr">
-        <is>
-          <t>Triazole derivatives</t>
-        </is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F484" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G484" t="e">
+        <v>#N/A</v>
       </c>
       <c r="H484" t="inlineStr">
         <is>
-          <t>vori,vrc</t>
+          <t/>
         </is>
       </c>
       <c r="I484" t="inlineStr">
         <is>
-          <t>pfizer,vfendiv,voriconazol,voriconazolevfend,voriconazolum,voriconzole,vorikonazole</t>
-        </is>
-      </c>
-      <c r="J484">
-        <v>0.4</v>
-      </c>
-      <c r="K484" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
-      </c>
-      <c r="L484">
-        <v>0.4</v>
-      </c>
-      <c r="M484" t="inlineStr">
-        <is>
-          <t>g</t>
-        </is>
+          <t>eskalin,eskalinv,micamicina,mikamycin,mikamycine,mikamycinum,ostreogricina,ostreogrycin,ostreogrycine,ostreogrycinum,pristinamicina,pristinamycine,pristinamycinum,pyostacine,stafac,stafytracine,staphylomycin,stapyocine,starfac,streptogramin,vernamycin,virgimycin,virgimycine,virginiamicina,virginiamycin,virginiamycina,virginiamycinum</t>
+        </is>
+      </c>
+      <c r="J484" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K484" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L484" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M484" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N484" t="inlineStr">
         <is>
-          <t>32379-0,35862-2,35863-0,38370-3,41199-1,41200-7,53902-3,73676-9,80553-1,80651-3</t>
+          <t/>
         </is>
       </c>
     </row>
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>XBR</t>
+          <t>VOR</t>
         </is>
       </c>
       <c r="B485">
-        <v>72144</v>
+        <v>71616</v>
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>Xibornol</t>
+          <t>Voriconazole</t>
         </is>
       </c>
       <c r="D485" t="inlineStr">
         <is>
-          <t>Other antibacterials</t>
+          <t>Antifungals/antimycotics</t>
         </is>
       </c>
       <c r="E485" t="inlineStr">
         <is>
-          <t>J01XX02</t>
+          <t>J02AC03</t>
         </is>
       </c>
       <c r="F485" t="inlineStr">
         <is>
-          <t>Other antibacterials</t>
+          <t>Antimycotics for systemic use</t>
         </is>
       </c>
       <c r="G485" t="inlineStr">
         <is>
-          <t>Other antibacterials</t>
+          <t>Triazole derivatives</t>
         </is>
       </c>
       <c r="H485" t="inlineStr">
         <is>
-          <t/>
+          <t>vori,vrc</t>
         </is>
       </c>
       <c r="I485" t="inlineStr">
         <is>
-          <t>bactacine,bracen,nanbacine,xibornolo,xibornolum</t>
-        </is>
-      </c>
-      <c r="J485" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K485" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L485" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M485" t="e">
-        <v>#N/A</v>
+          <t>pfizer,vfendiv,voriconazol,voriconazolevfend,voriconazolum,voriconzole,vorikonazole</t>
+        </is>
+      </c>
+      <c r="J485">
+        <v>0.4</v>
+      </c>
+      <c r="K485" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="L485">
+        <v>0.4</v>
+      </c>
+      <c r="M485" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
       </c>
       <c r="N485" t="inlineStr">
         <is>
-          <t/>
+          <t>32379-0,35862-2,35863-0,38370-3,41199-1,41200-7,53902-3,73676-9,80553-1,80651-3</t>
         </is>
       </c>
     </row>
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>ZID</t>
+          <t>XBR</t>
         </is>
       </c>
       <c r="B486">
-        <v>77846445</v>
+        <v>72144</v>
       </c>
       <c r="C486" t="inlineStr">
         <is>
-          <t>Zidebactam</t>
+          <t>Xibornol</t>
         </is>
       </c>
       <c r="D486" t="inlineStr">
@@ -30338,14 +30334,18 @@
       </c>
       <c r="E486" t="inlineStr">
         <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="F486" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G486" t="e">
-        <v>#N/A</v>
+          <t>J01XX02</t>
+        </is>
+      </c>
+      <c r="F486" t="inlineStr">
+        <is>
+          <t>Other antibacterials</t>
+        </is>
+      </c>
+      <c r="G486" t="inlineStr">
+        <is>
+          <t>Other antibacterials</t>
+        </is>
       </c>
       <c r="H486" t="inlineStr">
         <is>
@@ -30354,7 +30354,7 @@
       </c>
       <c r="I486" t="inlineStr">
         <is>
-          <t/>
+          <t>bactacine,bracen,nanbacine,xibornolo,xibornolum</t>
         </is>
       </c>
       <c r="J486" t="e">
@@ -30378,54 +30378,112 @@
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
+          <t>ZID</t>
+        </is>
+      </c>
+      <c r="B487">
+        <v>77846445</v>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>Zidebactam</t>
+        </is>
+      </c>
+      <c r="D487" t="inlineStr">
+        <is>
+          <t>Other antibacterials</t>
+        </is>
+      </c>
+      <c r="E487" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F487" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G487" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H487" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I487" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J487" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K487" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L487" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M487" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N487" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
           <t>ZFD</t>
         </is>
       </c>
-      <c r="B487" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C487" t="inlineStr">
+      <c r="B488" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C488" t="inlineStr">
         <is>
           <t>Zoliflodacin</t>
         </is>
       </c>
-      <c r="D487" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E487" t="inlineStr">
+      <c r="D488" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E488" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="F487" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G487" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H487" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I487" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="J487" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K487" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L487" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M487" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N487" t="inlineStr">
+      <c r="F488" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G488" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H488" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I488" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J488" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K488" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L488" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M488" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N488" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>